<commit_message>
Making Chart...(Change JudgeLine from 3D to 2D next time)
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Chart示例.xlsx
+++ b/Assets/Scripts/Chart示例.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzh\Xenody-master\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D40CA54-F8AB-4BAE-A14A-16FB2025A656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4D0D89-42D8-46C8-81A5-2260D97DFFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="planes" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="slides" sheetId="4" r:id="rId4"/>
     <sheet name="flicks" sheetId="5" r:id="rId5"/>
     <sheet name="stars" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="32">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -118,10 +119,6 @@
     <t>Linear</t>
   </si>
   <si>
-    <t>Sin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Cos</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -130,13 +127,37 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UpperCir</t>
+    <t>每拍时间戳</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>24分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="176" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -176,8 +197,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -494,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA789EFB-BCA3-4FCA-98D4-565CD71AE543}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -533,13 +557,13 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>3</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="E2">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -547,19 +571,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="C3">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>6</v>
+        <v>1.246</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -567,19 +591,19 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>1.246</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>3.246</v>
       </c>
       <c r="E4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -587,16 +611,16 @@
         <v>1</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>3.246</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>12</v>
+        <v>6.4450000000000003</v>
       </c>
       <c r="E5">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
         <v>23</v>
@@ -604,42 +628,42 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>12</v>
+        <v>1.246</v>
       </c>
       <c r="C6">
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>6.4450000000000003</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>6.4450000000000003</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>14</v>
+        <v>8.0259999999999998</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -647,18 +671,218 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>6.4450000000000003</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>60</v>
+        <v>8.0259999999999998</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>8.0259999999999998</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>10.036000000000001</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>8.0259999999999998</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>10.036000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>10.036000000000001</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>10.135999999999999</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>10.036000000000001</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>10.135999999999999</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>10.135999999999999</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>13.236000000000004</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>10.135999999999999</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>13.236000000000004</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>13.236000000000004</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>13.336</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>13.236000000000004</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>13.336</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>13.336</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>10000</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>13.336</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>10000</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
         <v>23</v>
       </c>
     </row>
@@ -671,10 +895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7059D0-50D6-42B0-899B-7876B4BEDB4C}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -695,13 +919,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>5.4690000000000003</v>
       </c>
       <c r="B2">
-        <v>-1.8</v>
+        <v>1.2</v>
       </c>
       <c r="C2">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -709,41 +933,41 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1.2</v>
+        <v>5.569</v>
       </c>
       <c r="B3">
-        <v>1.6</v>
+        <v>-0.3</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1.4</v>
+        <v>5.6689999999999996</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="C4">
         <v>0.6</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1.6</v>
+        <v>5.7689999999999992</v>
       </c>
       <c r="B5">
-        <v>0.4</v>
+        <v>-1.2</v>
       </c>
       <c r="C5">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -751,69 +975,69 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1.8</v>
+        <v>8.4359999999999999</v>
       </c>
       <c r="B6">
-        <v>0.6</v>
+        <v>-1</v>
       </c>
       <c r="C6">
         <v>0.8</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2</v>
+        <v>8.4359999999999999</v>
       </c>
       <c r="B7">
-        <v>-1.8</v>
+        <v>1</v>
       </c>
       <c r="C7">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2.2000000000000002</v>
+        <v>8.5359999999999996</v>
       </c>
       <c r="B8">
-        <v>1.6</v>
+        <v>-1</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2.4</v>
+        <v>8.5359999999999996</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2.6</v>
+        <v>8.7359999999999989</v>
       </c>
       <c r="B10">
-        <v>0.4</v>
+        <v>-1</v>
       </c>
       <c r="C10">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -821,10 +1045,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2.8</v>
+        <v>8.7359999999999989</v>
       </c>
       <c r="B11">
-        <v>0.6</v>
+        <v>1</v>
       </c>
       <c r="C11">
         <v>0.8</v>
@@ -835,13 +1059,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>3</v>
+        <v>8.9359999999999982</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C12">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -849,127 +1073,298 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>6</v>
+        <v>8.9359999999999982</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>6.2</v>
+        <v>9.1359999999999975</v>
       </c>
       <c r="B14">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="C14">
-        <v>1.1000000000000001</v>
+        <v>0.8</v>
       </c>
       <c r="D14">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>6.4</v>
+        <v>9.1359999999999975</v>
       </c>
       <c r="B15">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="C15">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="D15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>6.6</v>
+        <v>9.2359999999999971</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C16">
-        <v>1.3</v>
+        <v>0.8</v>
       </c>
       <c r="D16">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>6.8</v>
+        <v>9.2359999999999971</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17">
-        <v>1.4</v>
+        <v>0.8</v>
       </c>
       <c r="D17">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>7</v>
+        <v>10.636000000000001</v>
       </c>
       <c r="B18">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
       <c r="C18">
-        <v>1.4</v>
+        <v>0.8</v>
       </c>
       <c r="D18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>7.2</v>
+        <v>10.936</v>
       </c>
       <c r="B19">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <v>1.4</v>
+        <v>0.8</v>
       </c>
       <c r="D19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>7.4</v>
+        <v>11.235999999999999</v>
       </c>
       <c r="B20">
-        <v>-1.8</v>
+        <v>-1</v>
       </c>
       <c r="C20">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="D20">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>7.6</v>
+        <v>11.535999999999998</v>
       </c>
       <c r="B21">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <v>0.8</v>
       </c>
       <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>12.035999999999996</v>
+      </c>
+      <c r="B22">
+        <v>-1.2</v>
+      </c>
+      <c r="C22">
+        <v>0.6</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>12.135999999999996</v>
+      </c>
+      <c r="B23">
+        <v>0.2</v>
+      </c>
+      <c r="C23">
+        <v>0.6</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>12.335999999999995</v>
+      </c>
+      <c r="B24">
+        <v>-1.7</v>
+      </c>
+      <c r="C24">
+        <v>0.6</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>12.335999999999995</v>
+      </c>
+      <c r="B25">
+        <v>0.8</v>
+      </c>
+      <c r="C25">
+        <v>0.6</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>12.635999999999994</v>
+      </c>
+      <c r="B26">
+        <v>-0.4</v>
+      </c>
+      <c r="C26">
+        <v>0.6</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>12.735999999999994</v>
+      </c>
+      <c r="B27">
+        <v>0.3</v>
+      </c>
+      <c r="C27">
+        <v>0.6</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>12.835999999999993</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0.6</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>13.035999999999992</v>
+      </c>
+      <c r="B29">
+        <v>-1</v>
+      </c>
+      <c r="C29">
+        <v>0.6</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>13.836000000000004</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30">
+        <v>0.8</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>14.136000000000003</v>
+      </c>
+      <c r="B31">
+        <v>-1</v>
+      </c>
+      <c r="C31">
+        <v>0.8</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>14.436000000000002</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0.8</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>14.736000000000001</v>
+      </c>
+      <c r="B33">
+        <v>-1</v>
+      </c>
+      <c r="C33">
+        <v>0.8</v>
+      </c>
+      <c r="D33">
         <v>2</v>
       </c>
     </row>
@@ -981,10 +1376,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B2D43-E0B0-4050-83A2-AF5C6E5EE029}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1029,28 +1424,28 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>0.42699999999999999</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>-0.3</v>
       </c>
       <c r="E2">
-        <v>0.8</v>
+        <v>0.3</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1.246</v>
       </c>
       <c r="G2">
-        <v>-0.3</v>
+        <v>-1</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1058,31 +1453,31 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1.246</v>
       </c>
       <c r="D3">
-        <v>-0.8</v>
+        <v>-1</v>
       </c>
       <c r="E3">
-        <v>-0.1</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>3</v>
+        <v>3.206</v>
       </c>
       <c r="G3">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="H3">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1090,28 +1485,28 @@
         <v>1</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>3.6360000000000015</v>
       </c>
       <c r="D4">
-        <v>-2</v>
+        <v>-1.8</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>-1.2</v>
       </c>
       <c r="F4">
-        <v>6</v>
+        <v>3.7990000000000008</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>-1.8</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>-1.2</v>
       </c>
       <c r="I4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
         <v>25</v>
@@ -1125,28 +1520,28 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>3.6360000000000015</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>1.8</v>
       </c>
       <c r="F5">
-        <v>7</v>
+        <v>3.7990000000000008</v>
       </c>
       <c r="G5">
-        <v>-1</v>
+        <v>1.2</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="I5" t="s">
         <v>25</v>
       </c>
       <c r="J5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1157,25 +1552,25 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>7.5</v>
+        <v>3.9620000000000002</v>
       </c>
       <c r="D6">
-        <v>-2</v>
+        <v>-1.8</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>-1.2</v>
       </c>
       <c r="F6">
-        <v>8</v>
+        <v>4.1059999999999999</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>-1.8</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>-1.2</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J6" t="s">
         <v>25</v>
@@ -1183,34 +1578,34 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>3.9620000000000002</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="F7">
-        <v>8.5</v>
+        <v>4.1059999999999999</v>
       </c>
       <c r="G7">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="I7" t="s">
         <v>25</v>
       </c>
       <c r="J7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1218,31 +1613,31 @@
         <v>2</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>4.25</v>
       </c>
       <c r="D8">
-        <v>0.1</v>
+        <v>-1.8</v>
       </c>
       <c r="E8">
-        <v>0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="F8">
-        <v>10</v>
+        <v>4.399</v>
       </c>
       <c r="G8">
-        <v>-0.3</v>
+        <v>-1.8</v>
       </c>
       <c r="H8">
-        <v>2</v>
+        <v>-1.2</v>
       </c>
       <c r="I8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1250,31 +1645,255 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9">
+        <v>4.25</v>
+      </c>
+      <c r="D9">
+        <v>1.2</v>
+      </c>
+      <c r="E9">
+        <v>1.8</v>
+      </c>
+      <c r="F9">
+        <v>4.399</v>
+      </c>
+      <c r="G9">
+        <v>1.2</v>
+      </c>
+      <c r="H9">
+        <v>1.8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>4.548</v>
+      </c>
+      <c r="D10">
+        <v>-0.6</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>4.7059999999999995</v>
+      </c>
+      <c r="G10">
+        <v>-0.6</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="B11">
         <v>9</v>
       </c>
-      <c r="D9">
-        <v>-0.1</v>
-      </c>
-      <c r="E9">
-        <v>-0.8</v>
-      </c>
-      <c r="F9">
+      <c r="C11">
+        <v>4.548</v>
+      </c>
+      <c r="D11">
+        <v>1.2</v>
+      </c>
+      <c r="E11">
+        <v>1.8</v>
+      </c>
+      <c r="F11">
+        <v>4.7059999999999995</v>
+      </c>
+      <c r="G11">
+        <v>1.2</v>
+      </c>
+      <c r="H11">
+        <v>1.8</v>
+      </c>
+      <c r="I11" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
         <v>10</v>
       </c>
-      <c r="G9">
+      <c r="C12">
+        <v>4.8639999999999999</v>
+      </c>
+      <c r="D12">
+        <v>-1.8</v>
+      </c>
+      <c r="E12">
+        <v>-1.2</v>
+      </c>
+      <c r="F12">
+        <v>5.0219999999999994</v>
+      </c>
+      <c r="G12">
+        <v>-1.8</v>
+      </c>
+      <c r="H12">
+        <v>-1.2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>4.8639999999999999</v>
+      </c>
+      <c r="D13">
+        <v>1.2</v>
+      </c>
+      <c r="E13">
+        <v>1.8</v>
+      </c>
+      <c r="F13">
+        <v>5.0219999999999994</v>
+      </c>
+      <c r="G13">
+        <v>1.2</v>
+      </c>
+      <c r="H13">
+        <v>1.8</v>
+      </c>
+      <c r="I13" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>5.8689999999999998</v>
+      </c>
+      <c r="D14">
+        <v>-1.8</v>
+      </c>
+      <c r="E14">
+        <v>-1.2</v>
+      </c>
+      <c r="F14">
+        <v>8.0259999999999998</v>
+      </c>
+      <c r="G14">
+        <v>-2</v>
+      </c>
+      <c r="H14">
+        <v>-1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>5.8689999999999998</v>
+      </c>
+      <c r="D15">
+        <v>1.2</v>
+      </c>
+      <c r="E15">
+        <v>1.8</v>
+      </c>
+      <c r="F15">
+        <v>8.0259999999999998</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>6.4450000000000003</v>
+      </c>
+      <c r="D16">
+        <v>-0.3</v>
+      </c>
+      <c r="E16">
         <v>0.3</v>
       </c>
-      <c r="H9">
-        <v>-2</v>
-      </c>
-      <c r="I9" t="s">
-        <v>26</v>
-      </c>
-      <c r="J9" t="s">
-        <v>26</v>
+      <c r="F16">
+        <v>8.0259999999999998</v>
+      </c>
+      <c r="G16">
+        <v>-0.5</v>
+      </c>
+      <c r="H16">
+        <v>0.5</v>
+      </c>
+      <c r="I16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1286,10 +1905,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C76DC57-EF49-44CE-8A21-D4353938F627}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1310,55 +1929,55 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>8</v>
+        <v>1.9810000000000001</v>
       </c>
       <c r="B2">
-        <v>-1.7</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>0.6</v>
+        <v>1.2</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>8.1</v>
+      <c r="A3" s="1">
+        <v>2.427</v>
       </c>
       <c r="B3">
-        <v>-1.4</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.68</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>8.1999999999999993</v>
+      <c r="A4" s="1">
+        <v>2.7149999999999999</v>
       </c>
       <c r="B4">
-        <v>-1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.76</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>8.3000000000000007</v>
+      <c r="A5" s="1">
+        <v>2.9289999999999998</v>
       </c>
       <c r="B5">
-        <v>-0.8</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0.84</v>
+        <v>0.9</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1366,83 +1985,83 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>8.4</v>
+        <v>3.2360000000000002</v>
       </c>
       <c r="B6">
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C6">
-        <v>0.92</v>
+        <v>0.6</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>8.5</v>
+      <c r="A7" s="1">
+        <v>3.3026666666666671</v>
       </c>
       <c r="B7">
-        <v>-0.2</v>
+        <v>-0.9</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>8.6</v>
+      <c r="A8" s="1">
+        <v>3.369333333333334</v>
       </c>
       <c r="B8">
-        <v>0.1</v>
+        <v>-0.3</v>
       </c>
       <c r="C8">
-        <v>1.08</v>
+        <v>0.6</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>8.6999999999999993</v>
+      <c r="A9" s="1">
+        <v>3.4360000000000008</v>
       </c>
       <c r="B9">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="C9">
-        <v>1.1599999999999999</v>
+        <v>0.6</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8.8000000000000007</v>
+      <c r="A10" s="1">
+        <v>3.5026666666666677</v>
       </c>
       <c r="B10">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="C10">
-        <v>1.24</v>
+        <v>0.6</v>
       </c>
       <c r="D10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>8.9</v>
+      <c r="A11" s="1">
+        <v>3.5693333333333346</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C11">
-        <v>1.32</v>
+        <v>0.6</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -1450,15 +2069,43 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>9</v>
+        <v>9.636000000000001</v>
       </c>
       <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0.8</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11.835999999999997</v>
+      </c>
+      <c r="B13">
         <v>1.3</v>
       </c>
-      <c r="C12">
-        <v>1.4</v>
-      </c>
-      <c r="D12">
+      <c r="C13">
+        <v>0.6</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>11.885999999999999</v>
+      </c>
+      <c r="B14">
+        <v>1.7</v>
+      </c>
+      <c r="C14">
+        <v>0.6</v>
+      </c>
+      <c r="D14">
         <v>1</v>
       </c>
     </row>
@@ -1471,10 +2118,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F96158-71D4-4C19-99F5-47E7932AF572}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1498,13 +2145,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>7</v>
+        <v>10.036000000000001</v>
       </c>
       <c r="B2">
-        <v>-1.6</v>
+        <v>-1</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>1.6</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1515,16 +2162,16 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>7.2</v>
+        <v>10.036000000000001</v>
       </c>
       <c r="B3">
-        <v>-1.2</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>0.7</v>
+        <v>1.6</v>
       </c>
       <c r="D3">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -1532,53 +2179,36 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>7.4</v>
+        <v>13.236000000000004</v>
       </c>
       <c r="B4">
-        <v>-0.8</v>
+        <v>-1</v>
       </c>
       <c r="C4">
-        <v>0.9</v>
+        <v>1.6</v>
       </c>
       <c r="D4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>7.6</v>
+        <v>13.236000000000004</v>
       </c>
       <c r="B5">
-        <v>-0.4</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>1.1000000000000001</v>
+        <v>1.6</v>
       </c>
       <c r="D5">
-        <v>0.75</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>7.8</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>1.3</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1589,10 +2219,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192095B2-1BEA-4365-B4DE-88EEBB6E4423}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C8" sqref="C8:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1631,31 +2261,31 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>9</v>
+        <v>10.436000000000002</v>
       </c>
       <c r="D2">
-        <v>9.5</v>
+        <v>10.436000000000002</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>10.536000000000001</v>
       </c>
       <c r="F2">
         <v>-1</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>-1.6</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
@@ -1663,34 +2293,803 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
+        <v>10.736000000000001</v>
+      </c>
+      <c r="D3">
+        <v>10.736000000000001</v>
+      </c>
+      <c r="E3">
+        <v>10.836</v>
+      </c>
+      <c r="F3">
+        <v>-1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>-0.4</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>11.036</v>
+      </c>
+      <c r="D4">
+        <v>11.036</v>
+      </c>
+      <c r="E4">
+        <v>11.135999999999999</v>
+      </c>
+      <c r="F4">
+        <v>-1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>-1.6</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>11.335999999999999</v>
+      </c>
+      <c r="D5">
+        <v>11.335999999999999</v>
+      </c>
+      <c r="E5">
+        <v>11.435999999999998</v>
+      </c>
+      <c r="F5">
+        <v>-1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>-0.4</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>11.635999999999997</v>
+      </c>
+      <c r="D6">
+        <v>11.635999999999997</v>
+      </c>
+      <c r="E6">
+        <v>11.735999999999997</v>
+      </c>
+      <c r="F6">
+        <v>-1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>-1.6</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>13.636000000000005</v>
+      </c>
+      <c r="D7">
+        <v>13.636000000000005</v>
+      </c>
+      <c r="E7">
+        <v>13.736000000000004</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1.6</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>13.936000000000003</v>
+      </c>
+      <c r="D8">
+        <v>13.936000000000003</v>
+      </c>
+      <c r="E8">
+        <v>14.036000000000003</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>0.4</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>14.236000000000002</v>
+      </c>
+      <c r="D9">
+        <v>14.236000000000002</v>
+      </c>
+      <c r="E9">
+        <v>14.336000000000002</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1.6</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
         <v>9</v>
       </c>
-      <c r="D3">
+      <c r="C10">
+        <v>14.536000000000001</v>
+      </c>
+      <c r="D10">
+        <v>14.536000000000001</v>
+      </c>
+      <c r="E10">
+        <v>14.636000000000001</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0.4</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>10.5</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3">
-        <v>0.5</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="C11">
+        <v>14.836</v>
+      </c>
+      <c r="D11">
+        <v>14.836</v>
+      </c>
+      <c r="E11">
+        <v>14.936</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1.6</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7596AC-A6F6-4FB8-B823-5B4B1777330C}">
+  <dimension ref="A1:N60"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.125" customWidth="1"/>
+    <col min="14" max="14" width="9.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" t="s">
         <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>3.2360000000000002</v>
+      </c>
+      <c r="K2">
+        <v>0.4</v>
+      </c>
+      <c r="L2">
+        <f>K2/2</f>
+        <v>0.2</v>
+      </c>
+      <c r="M2">
+        <f>L2/2</f>
+        <v>0.1</v>
+      </c>
+      <c r="N2" s="1">
+        <f>L2/3</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>8.4359999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <f t="shared" ref="A4:A43" si="0">A3+$K$2</f>
+        <v>8.8360000000000003</v>
+      </c>
+      <c r="L4">
+        <v>3.6360000000000001</v>
+      </c>
+      <c r="M4">
+        <v>5.4690000000000003</v>
+      </c>
+      <c r="N4">
+        <v>3.2360000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>9.2360000000000007</v>
+      </c>
+      <c r="L5">
+        <f>L4+$L$2</f>
+        <v>3.8360000000000003</v>
+      </c>
+      <c r="M5">
+        <f>M4+$M$2</f>
+        <v>5.569</v>
+      </c>
+      <c r="N5" s="1">
+        <f>N4+$N$2</f>
+        <v>3.3026666666666671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>9.636000000000001</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ref="L6:L13" si="1">L5+$L$2</f>
+        <v>4.0360000000000005</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ref="M6:M8" si="2">M5+$M$2</f>
+        <v>5.6689999999999996</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" ref="N6:N10" si="3">N5+$N$2</f>
+        <v>3.369333333333334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>10.036000000000001</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>4.2360000000000007</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>5.7689999999999992</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="3"/>
+        <v>3.4360000000000008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>10.436000000000002</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>4.4360000000000008</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>5.8689999999999989</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="3"/>
+        <v>3.5026666666666677</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>10.836000000000002</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>4.636000000000001</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="3"/>
+        <v>3.5693333333333346</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>11.236000000000002</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>4.8360000000000012</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="3"/>
+        <v>3.6360000000000015</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>11.636000000000003</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>5.0360000000000014</v>
+      </c>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>12.036000000000003</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>5.2360000000000015</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12.436000000000003</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>5.4360000000000017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>12.836000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13.236000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>13.636000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>14.036000000000005</v>
+      </c>
+      <c r="M17">
+        <v>6.4450000000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>14.436000000000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>14.836000000000006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>15.236000000000006</v>
+      </c>
+      <c r="M20">
+        <v>8.4359999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>15.636000000000006</v>
+      </c>
+      <c r="M21">
+        <f>M20+$M$2</f>
+        <v>8.5359999999999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>16.036000000000005</v>
+      </c>
+      <c r="M22">
+        <f t="shared" ref="M22:M31" si="4">M21+$M$2</f>
+        <v>8.6359999999999992</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>16.436000000000003</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="4"/>
+        <v>8.7359999999999989</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>16.836000000000002</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="4"/>
+        <v>8.8359999999999985</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>17.236000000000001</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="4"/>
+        <v>8.9359999999999982</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>17.635999999999999</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="4"/>
+        <v>9.0359999999999978</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <f t="shared" si="4"/>
+        <v>9.1359999999999975</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M28">
+        <f t="shared" si="4"/>
+        <v>9.2359999999999971</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M30">
+        <v>10.436000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M31">
+        <f>M30+$M$2</f>
+        <v>10.536000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <f t="shared" ref="M32:M60" si="5">M31+$M$2</f>
+        <v>10.636000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M33">
+        <f t="shared" si="5"/>
+        <v>10.736000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M34">
+        <f t="shared" si="5"/>
+        <v>10.836</v>
+      </c>
+    </row>
+    <row r="35" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M35">
+        <f t="shared" si="5"/>
+        <v>10.936</v>
+      </c>
+    </row>
+    <row r="36" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M36">
+        <f t="shared" si="5"/>
+        <v>11.036</v>
+      </c>
+    </row>
+    <row r="37" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <f t="shared" si="5"/>
+        <v>11.135999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M38">
+        <f t="shared" si="5"/>
+        <v>11.235999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M39">
+        <f t="shared" si="5"/>
+        <v>11.335999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M40">
+        <f t="shared" si="5"/>
+        <v>11.435999999999998</v>
+      </c>
+    </row>
+    <row r="41" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M41">
+        <f t="shared" si="5"/>
+        <v>11.535999999999998</v>
+      </c>
+    </row>
+    <row r="42" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M42">
+        <f t="shared" si="5"/>
+        <v>11.635999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M43">
+        <f t="shared" si="5"/>
+        <v>11.735999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M44">
+        <f t="shared" si="5"/>
+        <v>11.835999999999997</v>
+      </c>
+    </row>
+    <row r="45" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M45">
+        <f t="shared" si="5"/>
+        <v>11.935999999999996</v>
+      </c>
+    </row>
+    <row r="46" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M46">
+        <f t="shared" si="5"/>
+        <v>12.035999999999996</v>
+      </c>
+    </row>
+    <row r="47" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M47">
+        <f t="shared" si="5"/>
+        <v>12.135999999999996</v>
+      </c>
+    </row>
+    <row r="48" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M48">
+        <f t="shared" si="5"/>
+        <v>12.235999999999995</v>
+      </c>
+    </row>
+    <row r="49" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M49">
+        <f t="shared" si="5"/>
+        <v>12.335999999999995</v>
+      </c>
+    </row>
+    <row r="50" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M50">
+        <f t="shared" si="5"/>
+        <v>12.435999999999995</v>
+      </c>
+    </row>
+    <row r="51" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M51">
+        <f t="shared" si="5"/>
+        <v>12.535999999999994</v>
+      </c>
+    </row>
+    <row r="52" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M52">
+        <f t="shared" si="5"/>
+        <v>12.635999999999994</v>
+      </c>
+    </row>
+    <row r="53" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M53">
+        <f t="shared" si="5"/>
+        <v>12.735999999999994</v>
+      </c>
+    </row>
+    <row r="54" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M54">
+        <f t="shared" si="5"/>
+        <v>12.835999999999993</v>
+      </c>
+    </row>
+    <row r="55" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M55">
+        <f t="shared" si="5"/>
+        <v>12.935999999999993</v>
+      </c>
+    </row>
+    <row r="56" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M56">
+        <f t="shared" si="5"/>
+        <v>13.035999999999992</v>
+      </c>
+    </row>
+    <row r="57" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M57">
+        <f t="shared" si="5"/>
+        <v>13.135999999999992</v>
+      </c>
+    </row>
+    <row r="58" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M58">
+        <f t="shared" si="5"/>
+        <v>13.235999999999992</v>
+      </c>
+    </row>
+    <row r="59" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M59">
+        <f t="shared" si="5"/>
+        <v>13.335999999999991</v>
+      </c>
+    </row>
+    <row r="60" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M60">
+        <f t="shared" si="5"/>
+        <v>13.435999999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change JudgeLine from 3D to 2D, and some others..
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Chart示例.xlsx
+++ b/Assets/Scripts/Chart示例.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzh\Xenody-master\Assets\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Xenody-master\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4D0D89-42D8-46C8-81A5-2260D97DFFDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E9F1C9-481A-4386-B8D6-B27E8DF4C575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="planes" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,26 @@
     <sheet name="stars" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="33">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -148,6 +157,10 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sin</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -518,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA789EFB-BCA3-4FCA-98D4-565CD71AE543}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -857,7 +870,7 @@
         <v>1</v>
       </c>
       <c r="D17">
-        <v>10000</v>
+        <v>16.435999999999989</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -877,12 +890,272 @@
         <v>0</v>
       </c>
       <c r="D18">
+        <v>16.435999999999989</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>16.435999999999989</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>16.536000000000001</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>16.435999999999989</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>16.536000000000001</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>16.536000000000001</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>19.635999999999999</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>16.536000000000001</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>19.635999999999999</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>19.635999999999999</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>20.036000000000001</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>19.635999999999999</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>20.036000000000001</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>20.036000000000001</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>20.436</v>
+      </c>
+      <c r="E25">
+        <v>0.5</v>
+      </c>
+      <c r="F25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26">
+        <v>20.036000000000001</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>20.436</v>
+      </c>
+      <c r="E26">
+        <v>0.5</v>
+      </c>
+      <c r="F26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>20.436</v>
+      </c>
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27">
+        <v>20.835999999999999</v>
+      </c>
+      <c r="E27">
+        <v>0.25</v>
+      </c>
+      <c r="F27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2</v>
+      </c>
+      <c r="B28">
+        <v>20.436</v>
+      </c>
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28">
+        <v>20.835999999999999</v>
+      </c>
+      <c r="E28">
+        <v>0.25</v>
+      </c>
+      <c r="F28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>20.835999999999999</v>
+      </c>
+      <c r="C29">
+        <v>0.25</v>
+      </c>
+      <c r="D29">
+        <v>21.236000000000001</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30">
+        <v>20.835999999999999</v>
+      </c>
+      <c r="C30">
+        <v>0.25</v>
+      </c>
+      <c r="D30">
+        <v>21.236000000000001</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>21.236000000000001</v>
+      </c>
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
         <v>10000</v>
       </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31" t="s">
         <v>23</v>
       </c>
     </row>
@@ -895,10 +1168,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7059D0-50D6-42B0-899B-7876B4BEDB4C}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F88"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1146,7 +1419,7 @@
         <v>10.636000000000001</v>
       </c>
       <c r="B18">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C18">
         <v>0.8</v>
@@ -1174,7 +1447,7 @@
         <v>11.235999999999999</v>
       </c>
       <c r="B20">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C20">
         <v>0.8</v>
@@ -1331,7 +1604,7 @@
         <v>14.136000000000003</v>
       </c>
       <c r="B31">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C31">
         <v>0.8</v>
@@ -1359,27 +1632,798 @@
         <v>14.736000000000001</v>
       </c>
       <c r="B33">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="C33">
         <v>0.8</v>
       </c>
       <c r="D33">
         <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>15.435999999999984</v>
+      </c>
+      <c r="B34">
+        <v>0.8</v>
+      </c>
+      <c r="C34">
+        <v>0.6</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>15.535999999999984</v>
+      </c>
+      <c r="B35">
+        <v>-0.4</v>
+      </c>
+      <c r="C35">
+        <v>0.6</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>15.735999999999983</v>
+      </c>
+      <c r="B36">
+        <v>1.7</v>
+      </c>
+      <c r="C36">
+        <v>0.6</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>15.835999999999983</v>
+      </c>
+      <c r="B37">
+        <v>-1.4</v>
+      </c>
+      <c r="C37">
+        <v>0.6</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>15.935999999999982</v>
+      </c>
+      <c r="B38">
+        <v>0.8</v>
+      </c>
+      <c r="C38">
+        <v>0.6</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>16.035999999999984</v>
+      </c>
+      <c r="B39">
+        <v>-0.5</v>
+      </c>
+      <c r="C39">
+        <v>0.6</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>16.135999999999985</v>
+      </c>
+      <c r="B40">
+        <v>1.5</v>
+      </c>
+      <c r="C40">
+        <v>0.6</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>16.235999999999986</v>
+      </c>
+      <c r="B41">
+        <v>-1.5</v>
+      </c>
+      <c r="C41">
+        <v>0.6</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>16.335999999999988</v>
+      </c>
+      <c r="B42">
+        <v>1.7</v>
+      </c>
+      <c r="C42">
+        <v>0.6</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>17.035999999999998</v>
+      </c>
+      <c r="B43">
+        <v>-1</v>
+      </c>
+      <c r="C43">
+        <v>0.8</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>17.336000000000002</v>
+      </c>
+      <c r="B44">
+        <v>1</v>
+      </c>
+      <c r="C44">
+        <v>0.8</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>17.636000000000006</v>
+      </c>
+      <c r="B45">
+        <v>-1</v>
+      </c>
+      <c r="C45">
+        <v>0.8</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>17.936000000000011</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>0.8</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>18.236000000000015</v>
+      </c>
+      <c r="B47">
+        <v>0.3</v>
+      </c>
+      <c r="C47">
+        <v>0.6</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>18.436000000000018</v>
+      </c>
+      <c r="B48">
+        <v>-1.7</v>
+      </c>
+      <c r="C48">
+        <v>0.6</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>18.536000000000019</v>
+      </c>
+      <c r="B49">
+        <v>1.7</v>
+      </c>
+      <c r="C49">
+        <v>0.6</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>18.736000000000022</v>
+      </c>
+      <c r="B50">
+        <v>-0.7</v>
+      </c>
+      <c r="C50">
+        <v>0.6</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>18.736000000000022</v>
+      </c>
+      <c r="B51">
+        <v>0.5</v>
+      </c>
+      <c r="C51">
+        <v>0.6</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>19.236000000000029</v>
+      </c>
+      <c r="B52">
+        <v>0</v>
+      </c>
+      <c r="C52">
+        <v>0.6</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>19.33600000000003</v>
+      </c>
+      <c r="B53">
+        <v>1.2</v>
+      </c>
+      <c r="C53">
+        <v>0.6</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>19.536000000000033</v>
+      </c>
+      <c r="B54">
+        <v>1.7</v>
+      </c>
+      <c r="C54">
+        <v>0.6</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>21.236000000000001</v>
+      </c>
+      <c r="B55">
+        <v>-1.5</v>
+      </c>
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>21.236000000000001</v>
+      </c>
+      <c r="B56">
+        <v>1.5</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>21.651</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>0.5</v>
+      </c>
+      <c r="D57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>21.731999999999999</v>
+      </c>
+      <c r="B58">
+        <v>0</v>
+      </c>
+      <c r="C58">
+        <v>0.5</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>21.81</v>
+      </c>
+      <c r="B59">
+        <v>0.5</v>
+      </c>
+      <c r="C59">
+        <v>0.5</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>21.898</v>
+      </c>
+      <c r="B60">
+        <v>-0.5</v>
+      </c>
+      <c r="C60">
+        <v>0.7</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>21.969000000000001</v>
+      </c>
+      <c r="B61">
+        <v>0</v>
+      </c>
+      <c r="C61">
+        <v>0.7</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>22.036000000000001</v>
+      </c>
+      <c r="B62">
+        <v>-0.2</v>
+      </c>
+      <c r="C62">
+        <v>0.7</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>22.136000000000003</v>
+      </c>
+      <c r="B63">
+        <v>0.8</v>
+      </c>
+      <c r="C63">
+        <v>0.7</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>22.336000000000006</v>
+      </c>
+      <c r="B64">
+        <v>1.4</v>
+      </c>
+      <c r="C64">
+        <v>0.7</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>22.536000000000008</v>
+      </c>
+      <c r="B65">
+        <v>-1</v>
+      </c>
+      <c r="C65">
+        <v>0.8</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>22.63600000000001</v>
+      </c>
+      <c r="B66">
+        <v>0.6</v>
+      </c>
+      <c r="C66">
+        <v>0.8</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>23.036000000000001</v>
+      </c>
+      <c r="B67">
+        <v>-0.8</v>
+      </c>
+      <c r="C67">
+        <v>1.2</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>23.036000000000001</v>
+      </c>
+      <c r="B68">
+        <v>0.8</v>
+      </c>
+      <c r="C68">
+        <v>1.2</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>23.33600000000002</v>
+      </c>
+      <c r="B69">
+        <v>-1.4</v>
+      </c>
+      <c r="C69">
+        <v>1.2</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>23.33600000000002</v>
+      </c>
+      <c r="B70">
+        <v>0.2</v>
+      </c>
+      <c r="C70">
+        <v>1.2</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>23.536000000000023</v>
+      </c>
+      <c r="B71">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C71">
+        <v>1.2</v>
+      </c>
+      <c r="D71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>23.636000000000024</v>
+      </c>
+      <c r="B72">
+        <v>-0.2</v>
+      </c>
+      <c r="C72">
+        <v>1.2</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>23.636000000000024</v>
+      </c>
+      <c r="B73">
+        <v>1.4</v>
+      </c>
+      <c r="C73">
+        <v>1.2</v>
+      </c>
+      <c r="D73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>23.836000000000027</v>
+      </c>
+      <c r="B74">
+        <v>-0.8</v>
+      </c>
+      <c r="C74">
+        <v>1.2</v>
+      </c>
+      <c r="D74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>23.836000000000027</v>
+      </c>
+      <c r="B75">
+        <v>0.8</v>
+      </c>
+      <c r="C75">
+        <v>1.2</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>24.03600000000003</v>
+      </c>
+      <c r="B76">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C76">
+        <v>1.2</v>
+      </c>
+      <c r="D76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>24.03600000000003</v>
+      </c>
+      <c r="B77">
+        <v>0.5</v>
+      </c>
+      <c r="C77">
+        <v>1.2</v>
+      </c>
+      <c r="D77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>24.136000000000031</v>
+      </c>
+      <c r="B78">
+        <v>-1.4</v>
+      </c>
+      <c r="C78">
+        <v>1.2</v>
+      </c>
+      <c r="D78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>24.136000000000031</v>
+      </c>
+      <c r="B79">
+        <v>0.2</v>
+      </c>
+      <c r="C79">
+        <v>1.2</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>24.336000000000034</v>
+      </c>
+      <c r="B80">
+        <v>-0.8</v>
+      </c>
+      <c r="C80">
+        <v>1.2</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>24.336000000000034</v>
+      </c>
+      <c r="B81">
+        <v>0.8</v>
+      </c>
+      <c r="C81">
+        <v>1.2</v>
+      </c>
+      <c r="D81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>24.636000000000038</v>
+      </c>
+      <c r="B82">
+        <v>1.4</v>
+      </c>
+      <c r="C82">
+        <v>1.2</v>
+      </c>
+      <c r="D82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>24.73600000000004</v>
+      </c>
+      <c r="B83">
+        <v>0</v>
+      </c>
+      <c r="C83">
+        <v>1.2</v>
+      </c>
+      <c r="D83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>24.936000000000043</v>
+      </c>
+      <c r="B84">
+        <v>-1.2</v>
+      </c>
+      <c r="C84">
+        <v>1.2</v>
+      </c>
+      <c r="D84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>25.036000000000044</v>
+      </c>
+      <c r="B85">
+        <v>0.7</v>
+      </c>
+      <c r="C85">
+        <v>1.2</v>
+      </c>
+      <c r="D85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>25.136000000000045</v>
+      </c>
+      <c r="B86">
+        <v>0.5</v>
+      </c>
+      <c r="C86">
+        <v>1.2</v>
+      </c>
+      <c r="D86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>25.336000000000048</v>
+      </c>
+      <c r="B87">
+        <v>0</v>
+      </c>
+      <c r="C87">
+        <v>1.2</v>
+      </c>
+      <c r="D87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>25.43600000000005</v>
+      </c>
+      <c r="B88">
+        <v>-0.2</v>
+      </c>
+      <c r="C88">
+        <v>1.2</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B2D43-E0B0-4050-83A2-AF5C6E5EE029}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1893,6 +2937,294 @@
         <v>25</v>
       </c>
       <c r="J16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>19.635999999999999</v>
+      </c>
+      <c r="D17">
+        <v>1.2</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>20.036000000000001</v>
+      </c>
+      <c r="G17">
+        <v>-1.6</v>
+      </c>
+      <c r="H17">
+        <v>-1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>32</v>
+      </c>
+      <c r="J17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>20.036000000000001</v>
+      </c>
+      <c r="D18">
+        <v>-1.6</v>
+      </c>
+      <c r="E18">
+        <v>-1</v>
+      </c>
+      <c r="F18">
+        <v>20.436</v>
+      </c>
+      <c r="G18">
+        <v>-2</v>
+      </c>
+      <c r="H18">
+        <v>-1.6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>20.436</v>
+      </c>
+      <c r="D19">
+        <v>-2</v>
+      </c>
+      <c r="E19">
+        <v>-1.6</v>
+      </c>
+      <c r="F19">
+        <v>20.736000000000001</v>
+      </c>
+      <c r="G19">
+        <v>-1.6</v>
+      </c>
+      <c r="H19">
+        <v>-1</v>
+      </c>
+      <c r="I19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>20.736000000000001</v>
+      </c>
+      <c r="D20">
+        <v>-1.6</v>
+      </c>
+      <c r="E20">
+        <v>-1</v>
+      </c>
+      <c r="F20">
+        <v>21.036000000000001</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>19.635999999999999</v>
+      </c>
+      <c r="D21">
+        <v>-2</v>
+      </c>
+      <c r="E21">
+        <v>-1.2</v>
+      </c>
+      <c r="F21">
+        <v>20.036000000000001</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1.6</v>
+      </c>
+      <c r="I21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22">
+        <v>16</v>
+      </c>
+      <c r="C22">
+        <v>20.036000000000001</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1.6</v>
+      </c>
+      <c r="F22">
+        <v>20.436</v>
+      </c>
+      <c r="G22">
+        <v>1.6</v>
+      </c>
+      <c r="H22">
+        <v>2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>16</v>
+      </c>
+      <c r="C23">
+        <v>20.436</v>
+      </c>
+      <c r="D23">
+        <v>1.6</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>20.736000000000001</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1.6</v>
+      </c>
+      <c r="I23" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24">
+        <v>16</v>
+      </c>
+      <c r="C24">
+        <v>20.736000000000001</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1.6</v>
+      </c>
+      <c r="F24">
+        <v>21.036000000000001</v>
+      </c>
+      <c r="G24">
+        <v>-2</v>
+      </c>
+      <c r="H24">
+        <v>-1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>24</v>
+      </c>
+      <c r="J24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>25.036000000000044</v>
+      </c>
+      <c r="D25">
+        <v>-2</v>
+      </c>
+      <c r="E25">
+        <v>-0.6</v>
+      </c>
+      <c r="F25">
+        <v>25.43600000000005</v>
+      </c>
+      <c r="G25">
+        <v>-2</v>
+      </c>
+      <c r="H25">
+        <v>-0.6</v>
+      </c>
+      <c r="I25" t="s">
+        <v>25</v>
+      </c>
+      <c r="J25" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1905,10 +3237,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C76DC57-EF49-44CE-8A21-D4353938F627}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2106,6 +3438,118 @@
         <v>0.6</v>
       </c>
       <c r="D14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>15.035999999999985</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0.6</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15.085999999999986</v>
+      </c>
+      <c r="B16">
+        <v>-0.4</v>
+      </c>
+      <c r="C16">
+        <v>0.6</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15.135999999999987</v>
+      </c>
+      <c r="B17">
+        <v>-0.8</v>
+      </c>
+      <c r="C17">
+        <v>0.6</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>15.185999999999988</v>
+      </c>
+      <c r="B18">
+        <v>-1.2</v>
+      </c>
+      <c r="C18">
+        <v>0.6</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>15.235999999999988</v>
+      </c>
+      <c r="B19">
+        <v>-1.6</v>
+      </c>
+      <c r="C19">
+        <v>0.6</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18.936000000000025</v>
+      </c>
+      <c r="B20">
+        <v>1.5</v>
+      </c>
+      <c r="C20">
+        <v>0.6</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>18.986000000000001</v>
+      </c>
+      <c r="B21">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C21">
+        <v>0.6</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>19.036000000000026</v>
+      </c>
+      <c r="B22">
+        <v>0.7</v>
+      </c>
+      <c r="C22">
+        <v>0.6</v>
+      </c>
+      <c r="D22">
         <v>1</v>
       </c>
     </row>
@@ -2118,10 +3562,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F96158-71D4-4C19-99F5-47E7932AF572}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2208,6 +3652,74 @@
         <v>0</v>
       </c>
       <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>16.435999999999989</v>
+      </c>
+      <c r="B6">
+        <v>-1</v>
+      </c>
+      <c r="C6">
+        <v>1.6</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>16.435999999999989</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1.6</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>22.835999999999999</v>
+      </c>
+      <c r="B8">
+        <v>-1</v>
+      </c>
+      <c r="C8">
+        <v>1.6</v>
+      </c>
+      <c r="D8">
+        <v>0.75</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>22.835999999999999</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1.6</v>
+      </c>
+      <c r="D9">
+        <v>0.25</v>
+      </c>
+      <c r="E9">
         <v>1</v>
       </c>
     </row>
@@ -2219,10 +3731,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192095B2-1BEA-4365-B4DE-88EEBB6E4423}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C11"/>
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2579,18 +4091,179 @@
         <v>23</v>
       </c>
     </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>16.835999999999995</v>
+      </c>
+      <c r="D12">
+        <v>16.835999999999995</v>
+      </c>
+      <c r="E12">
+        <v>16.935999999999996</v>
+      </c>
+      <c r="F12">
+        <v>-1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>-1.6</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>17.135999999999999</v>
+      </c>
+      <c r="D13">
+        <v>17.135999999999999</v>
+      </c>
+      <c r="E13">
+        <v>17.236000000000001</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1.6</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>17.436000000000003</v>
+      </c>
+      <c r="D14">
+        <v>17.436000000000003</v>
+      </c>
+      <c r="E14">
+        <v>17.536000000000005</v>
+      </c>
+      <c r="F14">
+        <v>-1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>-1.6</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>17.736000000000008</v>
+      </c>
+      <c r="D15">
+        <v>17.736000000000008</v>
+      </c>
+      <c r="E15">
+        <v>17.836000000000009</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1.6</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>18.036000000000012</v>
+      </c>
+      <c r="D16">
+        <v>18.036000000000012</v>
+      </c>
+      <c r="E16">
+        <v>18.136000000000013</v>
+      </c>
+      <c r="F16">
+        <v>-1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>-1.6</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7596AC-A6F6-4FB8-B823-5B4B1777330C}">
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M37" activeCellId="1" sqref="M33:M35 M37:M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2632,8 +4305,7 @@
         <v>0.1</v>
       </c>
       <c r="N2" s="1">
-        <f>L2/3</f>
-        <v>6.6666666666666666E-2</v>
+        <v>6.7000000000000004E-2</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -2643,14 +4315,14 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4">
-        <f t="shared" ref="A4:A43" si="0">A3+$K$2</f>
+        <f t="shared" ref="A4:A26" si="0">A3+$K$2</f>
         <v>8.8360000000000003</v>
       </c>
       <c r="L4">
         <v>3.6360000000000001</v>
       </c>
       <c r="M4">
-        <v>5.4690000000000003</v>
+        <v>22.036000000000001</v>
       </c>
       <c r="N4">
         <v>3.2360000000000002</v>
@@ -2666,12 +4338,12 @@
         <v>3.8360000000000003</v>
       </c>
       <c r="M5">
-        <f>M4+$M$2</f>
-        <v>5.569</v>
+        <f>M4+0.1</f>
+        <v>22.136000000000003</v>
       </c>
       <c r="N5" s="1">
         <f>N4+$N$2</f>
-        <v>3.3026666666666671</v>
+        <v>3.3030000000000004</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -2684,12 +4356,12 @@
         <v>4.0360000000000005</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6:M8" si="2">M5+$M$2</f>
-        <v>5.6689999999999996</v>
+        <f t="shared" ref="M6:M41" si="2">M5+0.1</f>
+        <v>22.236000000000004</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" ref="N6:N10" si="3">N5+$N$2</f>
-        <v>3.369333333333334</v>
+        <v>3.3700000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -2703,11 +4375,11 @@
       </c>
       <c r="M7">
         <f t="shared" si="2"/>
-        <v>5.7689999999999992</v>
+        <v>22.336000000000006</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="3"/>
-        <v>3.4360000000000008</v>
+        <v>3.4370000000000007</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -2721,11 +4393,11 @@
       </c>
       <c r="M8">
         <f t="shared" si="2"/>
-        <v>5.8689999999999989</v>
+        <v>22.436000000000007</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="3"/>
-        <v>3.5026666666666677</v>
+        <v>3.5040000000000009</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -2737,9 +4409,13 @@
         <f t="shared" si="1"/>
         <v>4.636000000000001</v>
       </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>22.536000000000008</v>
+      </c>
       <c r="N9" s="1">
         <f t="shared" si="3"/>
-        <v>3.5693333333333346</v>
+        <v>3.5710000000000011</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -2751,9 +4427,13 @@
         <f t="shared" si="1"/>
         <v>4.8360000000000012</v>
       </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>22.63600000000001</v>
+      </c>
       <c r="N10" s="1">
         <f t="shared" si="3"/>
-        <v>3.6360000000000015</v>
+        <v>3.6380000000000012</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -2765,6 +4445,10 @@
         <f t="shared" si="1"/>
         <v>5.0360000000000014</v>
       </c>
+      <c r="M11">
+        <f t="shared" si="2"/>
+        <v>22.736000000000011</v>
+      </c>
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -2776,6 +4460,10 @@
         <f t="shared" si="1"/>
         <v>5.2360000000000015</v>
       </c>
+      <c r="M12">
+        <f t="shared" si="2"/>
+        <v>22.836000000000013</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -2786,24 +4474,51 @@
         <f t="shared" si="1"/>
         <v>5.4360000000000017</v>
       </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>22.936000000000014</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>12.836000000000004</v>
       </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>23.036000000000016</v>
+      </c>
+      <c r="N14">
+        <v>21.635999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>13.236000000000004</v>
       </c>
+      <c r="M15">
+        <f t="shared" si="2"/>
+        <v>23.136000000000017</v>
+      </c>
+      <c r="N15">
+        <f>N14+$N$2</f>
+        <v>21.702999999999999</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>13.636000000000005</v>
       </c>
+      <c r="M16">
+        <f t="shared" si="2"/>
+        <v>23.236000000000018</v>
+      </c>
+      <c r="N16">
+        <f>N15+$N$2</f>
+        <v>21.77</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -2811,7 +4526,8 @@
         <v>14.036000000000005</v>
       </c>
       <c r="M17">
-        <v>6.4450000000000003</v>
+        <f t="shared" si="2"/>
+        <v>23.33600000000002</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -2819,12 +4535,20 @@
         <f t="shared" si="0"/>
         <v>14.436000000000005</v>
       </c>
+      <c r="M18">
+        <f t="shared" si="2"/>
+        <v>23.436000000000021</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>14.836000000000006</v>
       </c>
+      <c r="M19">
+        <f t="shared" si="2"/>
+        <v>23.536000000000023</v>
+      </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -2832,7 +4556,8 @@
         <v>15.236000000000006</v>
       </c>
       <c r="M20">
-        <v>8.4359999999999999</v>
+        <f t="shared" si="2"/>
+        <v>23.636000000000024</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -2841,8 +4566,8 @@
         <v>15.636000000000006</v>
       </c>
       <c r="M21">
-        <f>M20+$M$2</f>
-        <v>8.5359999999999996</v>
+        <f t="shared" si="2"/>
+        <v>23.736000000000026</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -2851,8 +4576,8 @@
         <v>16.036000000000005</v>
       </c>
       <c r="M22">
-        <f t="shared" ref="M22:M31" si="4">M21+$M$2</f>
-        <v>8.6359999999999992</v>
+        <f t="shared" si="2"/>
+        <v>23.836000000000027</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -2861,8 +4586,8 @@
         <v>16.436000000000003</v>
       </c>
       <c r="M23">
-        <f t="shared" si="4"/>
-        <v>8.7359999999999989</v>
+        <f t="shared" si="2"/>
+        <v>23.936000000000028</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -2871,8 +4596,8 @@
         <v>16.836000000000002</v>
       </c>
       <c r="M24">
-        <f t="shared" si="4"/>
-        <v>8.8359999999999985</v>
+        <f t="shared" si="2"/>
+        <v>24.03600000000003</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -2881,8 +4606,8 @@
         <v>17.236000000000001</v>
       </c>
       <c r="M25">
-        <f t="shared" si="4"/>
-        <v>8.9359999999999982</v>
+        <f t="shared" si="2"/>
+        <v>24.136000000000031</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -2891,209 +4616,145 @@
         <v>17.635999999999999</v>
       </c>
       <c r="M26">
-        <f t="shared" si="4"/>
-        <v>9.0359999999999978</v>
+        <f t="shared" si="2"/>
+        <v>24.236000000000033</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M27">
-        <f t="shared" si="4"/>
-        <v>9.1359999999999975</v>
+        <f t="shared" si="2"/>
+        <v>24.336000000000034</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>19.635999999999999</v>
+      </c>
       <c r="M28">
-        <f t="shared" si="4"/>
-        <v>9.2359999999999971</v>
+        <f t="shared" si="2"/>
+        <v>24.436000000000035</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>20.036000000000001</v>
+      </c>
+      <c r="M29">
+        <f t="shared" si="2"/>
+        <v>24.536000000000037</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>20.436</v>
+      </c>
       <c r="M30">
-        <v>10.436000000000002</v>
+        <f t="shared" si="2"/>
+        <v>24.636000000000038</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>20.835999999999999</v>
+      </c>
       <c r="M31">
-        <f>M30+$M$2</f>
-        <v>10.536000000000001</v>
+        <f t="shared" si="2"/>
+        <v>24.73600000000004</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>21.236000000000001</v>
+      </c>
       <c r="M32">
-        <f t="shared" ref="M32:M60" si="5">M31+$M$2</f>
-        <v>10.636000000000001</v>
-      </c>
-    </row>
-    <row r="33" spans="13:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>24.836000000000041</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>21.635999999999999</v>
+      </c>
       <c r="M33">
-        <f t="shared" si="5"/>
-        <v>10.736000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="13:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>24.936000000000043</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>22.036000000000001</v>
+      </c>
       <c r="M34">
-        <f t="shared" si="5"/>
-        <v>10.836</v>
-      </c>
-    </row>
-    <row r="35" spans="13:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>25.036000000000044</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>22.436</v>
+      </c>
       <c r="M35">
-        <f t="shared" si="5"/>
-        <v>10.936</v>
-      </c>
-    </row>
-    <row r="36" spans="13:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>25.136000000000045</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>22.835999999999999</v>
+      </c>
       <c r="M36">
-        <f t="shared" si="5"/>
-        <v>11.036</v>
-      </c>
-    </row>
-    <row r="37" spans="13:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>25.236000000000047</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>23.236000000000001</v>
+      </c>
       <c r="M37">
-        <f t="shared" si="5"/>
-        <v>11.135999999999999</v>
-      </c>
-    </row>
-    <row r="38" spans="13:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>25.336000000000048</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>23.635999999999999</v>
+      </c>
       <c r="M38">
-        <f t="shared" si="5"/>
-        <v>11.235999999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="13:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>25.43600000000005</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>24.036000000000001</v>
+      </c>
       <c r="M39">
-        <f t="shared" si="5"/>
-        <v>11.335999999999999</v>
-      </c>
-    </row>
-    <row r="40" spans="13:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>25.536000000000051</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>24.436</v>
+      </c>
       <c r="M40">
-        <f t="shared" si="5"/>
-        <v>11.435999999999998</v>
-      </c>
-    </row>
-    <row r="41" spans="13:13" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>25.636000000000053</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>24.835999999999999</v>
+      </c>
       <c r="M41">
-        <f t="shared" si="5"/>
-        <v>11.535999999999998</v>
-      </c>
-    </row>
-    <row r="42" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M42">
-        <f t="shared" si="5"/>
-        <v>11.635999999999997</v>
-      </c>
-    </row>
-    <row r="43" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M43">
-        <f t="shared" si="5"/>
-        <v>11.735999999999997</v>
-      </c>
-    </row>
-    <row r="44" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M44">
-        <f t="shared" si="5"/>
-        <v>11.835999999999997</v>
-      </c>
-    </row>
-    <row r="45" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M45">
-        <f t="shared" si="5"/>
-        <v>11.935999999999996</v>
-      </c>
-    </row>
-    <row r="46" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M46">
-        <f t="shared" si="5"/>
-        <v>12.035999999999996</v>
-      </c>
-    </row>
-    <row r="47" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M47">
-        <f t="shared" si="5"/>
-        <v>12.135999999999996</v>
-      </c>
-    </row>
-    <row r="48" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M48">
-        <f t="shared" si="5"/>
-        <v>12.235999999999995</v>
-      </c>
-    </row>
-    <row r="49" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M49">
-        <f t="shared" si="5"/>
-        <v>12.335999999999995</v>
-      </c>
-    </row>
-    <row r="50" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M50">
-        <f t="shared" si="5"/>
-        <v>12.435999999999995</v>
-      </c>
-    </row>
-    <row r="51" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M51">
-        <f t="shared" si="5"/>
-        <v>12.535999999999994</v>
-      </c>
-    </row>
-    <row r="52" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M52">
-        <f t="shared" si="5"/>
-        <v>12.635999999999994</v>
-      </c>
-    </row>
-    <row r="53" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M53">
-        <f t="shared" si="5"/>
-        <v>12.735999999999994</v>
-      </c>
-    </row>
-    <row r="54" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M54">
-        <f t="shared" si="5"/>
-        <v>12.835999999999993</v>
-      </c>
-    </row>
-    <row r="55" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M55">
-        <f t="shared" si="5"/>
-        <v>12.935999999999993</v>
-      </c>
-    </row>
-    <row r="56" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M56">
-        <f t="shared" si="5"/>
-        <v>13.035999999999992</v>
-      </c>
-    </row>
-    <row r="57" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M57">
-        <f t="shared" si="5"/>
-        <v>13.135999999999992</v>
-      </c>
-    </row>
-    <row r="58" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M58">
-        <f t="shared" si="5"/>
-        <v>13.235999999999992</v>
-      </c>
-    </row>
-    <row r="59" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M59">
-        <f t="shared" si="5"/>
-        <v>13.335999999999991</v>
-      </c>
-    </row>
-    <row r="60" spans="13:13" x14ac:dyDescent="0.2">
-      <c r="M60">
-        <f t="shared" si="5"/>
-        <v>13.435999999999991</v>
+        <f t="shared" si="2"/>
+        <v>25.736000000000054</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Chart(and try Camera Layer...)
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Chart示例.xlsx
+++ b/Assets/Scripts/Chart示例.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Xenody-master\Assets\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzh\Xenody-master\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31E9F1C9-481A-4386-B8D6-B27E8DF4C575}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050C755E-3838-4135-AD32-1BCC6ED2D49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="planes" sheetId="1" r:id="rId1"/>
@@ -21,26 +21,17 @@
     <sheet name="stars" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="33">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -534,7 +525,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -576,7 +567,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -596,7 +587,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1168,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7059D0-50D6-42B0-899B-7876B4BEDB4C}">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="H97" sqref="H97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1730,7 +1721,7 @@
         <v>16.135999999999985</v>
       </c>
       <c r="B40">
-        <v>1.5</v>
+        <v>1.7</v>
       </c>
       <c r="C40">
         <v>0.6</v>
@@ -1758,7 +1749,7 @@
         <v>16.335999999999988</v>
       </c>
       <c r="B42">
-        <v>1.7</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C42">
         <v>0.6</v>
@@ -1898,7 +1889,7 @@
         <v>19.236000000000029</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>-0.7</v>
       </c>
       <c r="C52">
         <v>0.6</v>
@@ -1912,7 +1903,7 @@
         <v>19.33600000000003</v>
       </c>
       <c r="B53">
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
       <c r="C53">
         <v>0.6</v>
@@ -2013,7 +2004,7 @@
         <v>-0.5</v>
       </c>
       <c r="C60">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -2027,7 +2018,7 @@
         <v>0</v>
       </c>
       <c r="C61">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="D61">
         <v>1</v>
@@ -2038,10 +2029,10 @@
         <v>22.036000000000001</v>
       </c>
       <c r="B62">
-        <v>-0.2</v>
+        <v>-0.6</v>
       </c>
       <c r="C62">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -2055,7 +2046,7 @@
         <v>0.8</v>
       </c>
       <c r="C63">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="D63">
         <v>1</v>
@@ -2083,7 +2074,7 @@
         <v>-1</v>
       </c>
       <c r="C65">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D65">
         <v>1</v>
@@ -2097,7 +2088,7 @@
         <v>0.6</v>
       </c>
       <c r="C66">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="D66">
         <v>1</v>
@@ -2111,7 +2102,7 @@
         <v>-0.8</v>
       </c>
       <c r="C67">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D67">
         <v>1</v>
@@ -2125,7 +2116,7 @@
         <v>0.8</v>
       </c>
       <c r="C68">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D68">
         <v>1</v>
@@ -2139,7 +2130,7 @@
         <v>-1.4</v>
       </c>
       <c r="C69">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D69">
         <v>1</v>
@@ -2153,7 +2144,7 @@
         <v>0.2</v>
       </c>
       <c r="C70">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D70">
         <v>1</v>
@@ -2167,7 +2158,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C71">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D71">
         <v>1</v>
@@ -2181,7 +2172,7 @@
         <v>-0.2</v>
       </c>
       <c r="C72">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D72">
         <v>1</v>
@@ -2195,7 +2186,7 @@
         <v>1.4</v>
       </c>
       <c r="C73">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D73">
         <v>1</v>
@@ -2209,7 +2200,7 @@
         <v>-0.8</v>
       </c>
       <c r="C74">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D74">
         <v>1</v>
@@ -2223,7 +2214,7 @@
         <v>0.8</v>
       </c>
       <c r="C75">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D75">
         <v>1</v>
@@ -2234,10 +2225,10 @@
         <v>24.03600000000003</v>
       </c>
       <c r="B76">
-        <v>-1.1000000000000001</v>
+        <v>-1</v>
       </c>
       <c r="C76">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D76">
         <v>1</v>
@@ -2251,7 +2242,7 @@
         <v>0.5</v>
       </c>
       <c r="C77">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D77">
         <v>1</v>
@@ -2262,10 +2253,10 @@
         <v>24.136000000000031</v>
       </c>
       <c r="B78">
-        <v>-1.4</v>
+        <v>-1.5</v>
       </c>
       <c r="C78">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D78">
         <v>1</v>
@@ -2276,10 +2267,10 @@
         <v>24.136000000000031</v>
       </c>
       <c r="B79">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="C79">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D79">
         <v>1</v>
@@ -2293,7 +2284,7 @@
         <v>-0.8</v>
       </c>
       <c r="C80">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D80">
         <v>1</v>
@@ -2307,7 +2298,7 @@
         <v>0.8</v>
       </c>
       <c r="C81">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D81">
         <v>1</v>
@@ -2321,7 +2312,7 @@
         <v>1.4</v>
       </c>
       <c r="C82">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D82">
         <v>1</v>
@@ -2335,7 +2326,7 @@
         <v>0</v>
       </c>
       <c r="C83">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D83">
         <v>1</v>
@@ -2349,7 +2340,7 @@
         <v>-1.2</v>
       </c>
       <c r="C84">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D84">
         <v>1</v>
@@ -2363,7 +2354,7 @@
         <v>0.7</v>
       </c>
       <c r="C85">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D85">
         <v>1</v>
@@ -2374,10 +2365,10 @@
         <v>25.136000000000045</v>
       </c>
       <c r="B86">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C86">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D86">
         <v>1</v>
@@ -2391,7 +2382,7 @@
         <v>0</v>
       </c>
       <c r="C87">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="D87">
         <v>1</v>
@@ -2402,12 +2393,726 @@
         <v>25.43600000000005</v>
       </c>
       <c r="B88">
+        <v>-0.4</v>
+      </c>
+      <c r="C88">
+        <v>1</v>
+      </c>
+      <c r="D88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>26.236000000000001</v>
+      </c>
+      <c r="B89">
+        <v>-0.8</v>
+      </c>
+      <c r="C89">
+        <v>1</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>26.236000000000001</v>
+      </c>
+      <c r="B90">
+        <v>0.8</v>
+      </c>
+      <c r="C90">
+        <v>1</v>
+      </c>
+      <c r="D90">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>26.536000000000001</v>
+      </c>
+      <c r="B91">
         <v>-0.2</v>
       </c>
-      <c r="C88">
+      <c r="C91">
+        <v>1</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>26.536000000000001</v>
+      </c>
+      <c r="B92">
+        <v>1.4</v>
+      </c>
+      <c r="C92">
+        <v>1</v>
+      </c>
+      <c r="D92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>26.736000000000001</v>
+      </c>
+      <c r="B93">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>26.835999999999999</v>
+      </c>
+      <c r="B94">
+        <v>-1.4</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>26.835999999999999</v>
+      </c>
+      <c r="B95">
+        <v>0.2</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>27.036000000000001</v>
+      </c>
+      <c r="B96">
+        <v>-0.8</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>27.036000000000001</v>
+      </c>
+      <c r="B97">
+        <v>0.8</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>27.236000000000001</v>
+      </c>
+      <c r="B98">
+        <v>1.5</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>27.335999999999999</v>
+      </c>
+      <c r="B99">
+        <v>0.5</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>27.436</v>
+      </c>
+      <c r="B100">
+        <v>1.5</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>27.635999999999999</v>
+      </c>
+      <c r="B101">
+        <v>-1.2</v>
+      </c>
+      <c r="C101">
+        <v>1.6</v>
+      </c>
+      <c r="D101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>27.635999999999999</v>
+      </c>
+      <c r="B102">
+        <v>0.5</v>
+      </c>
+      <c r="C102">
+        <v>1.6</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>27.736000000000082</v>
+      </c>
+      <c r="B103">
+        <v>-0.9</v>
+      </c>
+      <c r="C103">
+        <v>1</v>
+      </c>
+      <c r="D103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>27.836000000000084</v>
+      </c>
+      <c r="B104">
+        <v>0</v>
+      </c>
+      <c r="C104">
+        <v>0.8</v>
+      </c>
+      <c r="D104">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>27.936000000000085</v>
+      </c>
+      <c r="B105">
+        <v>-1.5</v>
+      </c>
+      <c r="C105">
+        <v>1</v>
+      </c>
+      <c r="D105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>28.036000000000087</v>
+      </c>
+      <c r="B106">
+        <v>0.5</v>
+      </c>
+      <c r="C106">
+        <v>1</v>
+      </c>
+      <c r="D106">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>28.136000000000088</v>
+      </c>
+      <c r="B107">
+        <v>1</v>
+      </c>
+      <c r="C107">
+        <v>0.8</v>
+      </c>
+      <c r="D107">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>28.236000000000089</v>
+      </c>
+      <c r="B108">
+        <v>-0.2</v>
+      </c>
+      <c r="C108">
+        <v>1</v>
+      </c>
+      <c r="D108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109">
+        <v>28.336000000000091</v>
+      </c>
+      <c r="B109">
+        <v>-0.8</v>
+      </c>
+      <c r="C109">
+        <v>0.8</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110">
+        <v>28.436000000000092</v>
+      </c>
+      <c r="B110">
+        <v>0.4</v>
+      </c>
+      <c r="C110">
+        <v>1</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111">
+        <v>28.536000000000094</v>
+      </c>
+      <c r="B111">
+        <v>-0.4</v>
+      </c>
+      <c r="C111">
+        <v>0.8</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112">
+        <v>28.636000000000095</v>
+      </c>
+      <c r="B112">
+        <v>1.5</v>
+      </c>
+      <c r="C112">
+        <v>1</v>
+      </c>
+      <c r="D112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113">
+        <v>28.736000000000097</v>
+      </c>
+      <c r="B113">
+        <v>-1.5</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114">
+        <v>28.836000000000098</v>
+      </c>
+      <c r="B114">
+        <v>-0.9</v>
+      </c>
+      <c r="C114">
+        <v>0.8</v>
+      </c>
+      <c r="D114">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115">
+        <v>28.936000000000099</v>
+      </c>
+      <c r="B115">
+        <v>0.5</v>
+      </c>
+      <c r="C115">
+        <v>1</v>
+      </c>
+      <c r="D115">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116">
+        <v>29.036000000000101</v>
+      </c>
+      <c r="B116">
+        <v>0</v>
+      </c>
+      <c r="C116">
+        <v>0.8</v>
+      </c>
+      <c r="D116">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>29.136000000000102</v>
+      </c>
+      <c r="B117">
+        <v>-1</v>
+      </c>
+      <c r="C117">
+        <v>1</v>
+      </c>
+      <c r="D117">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118">
+        <v>29.436</v>
+      </c>
+      <c r="B118">
+        <v>0.8</v>
+      </c>
+      <c r="C118">
+        <v>1</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>29.436</v>
+      </c>
+      <c r="B119">
+        <v>-0.8</v>
+      </c>
+      <c r="C119">
+        <v>1</v>
+      </c>
+      <c r="D119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>29.736000000000018</v>
+      </c>
+      <c r="B120">
+        <v>1.4</v>
+      </c>
+      <c r="C120">
+        <v>1</v>
+      </c>
+      <c r="D120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>29.736000000000018</v>
+      </c>
+      <c r="B121">
+        <v>-0.2</v>
+      </c>
+      <c r="C121">
+        <v>1</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>29.936000000000021</v>
+      </c>
+      <c r="B122">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="D122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123">
+        <v>30.036000000000023</v>
+      </c>
+      <c r="B123">
+        <v>0.2</v>
+      </c>
+      <c r="C123">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>30.036000000000023</v>
+      </c>
+      <c r="B124">
+        <v>-1.4</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>30.236000000000026</v>
+      </c>
+      <c r="B125">
+        <v>0.8</v>
+      </c>
+      <c r="C125">
+        <v>1</v>
+      </c>
+      <c r="D125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>30.236000000000026</v>
+      </c>
+      <c r="B126">
+        <v>-0.8</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
+      <c r="D126">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127">
+        <v>30.436000000000028</v>
+      </c>
+      <c r="B127">
+        <v>1</v>
+      </c>
+      <c r="C127">
+        <v>1</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128">
+        <v>30.436000000000028</v>
+      </c>
+      <c r="B128">
+        <v>-0.5</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129">
+        <v>30.53600000000003</v>
+      </c>
+      <c r="B129">
+        <v>1.5</v>
+      </c>
+      <c r="C129">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130">
+        <v>30.53600000000003</v>
+      </c>
+      <c r="B130">
+        <v>0</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131">
+        <v>30.736000000000033</v>
+      </c>
+      <c r="B131">
+        <v>0.8</v>
+      </c>
+      <c r="C131">
+        <v>1</v>
+      </c>
+      <c r="D131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132">
+        <v>30.736000000000033</v>
+      </c>
+      <c r="B132">
+        <v>-0.8</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+      <c r="D132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133">
+        <v>31.036000000000037</v>
+      </c>
+      <c r="B133">
+        <v>-1.4</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134">
+        <v>31.136000000000038</v>
+      </c>
+      <c r="B134">
+        <v>0</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+      <c r="D134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135">
+        <v>31.336000000000041</v>
+      </c>
+      <c r="B135">
         <v>1.2</v>
       </c>
-      <c r="D88">
+      <c r="C135">
+        <v>1</v>
+      </c>
+      <c r="D135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136">
+        <v>31.436000000000043</v>
+      </c>
+      <c r="B136">
+        <v>-0.7</v>
+      </c>
+      <c r="C136">
+        <v>1</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137">
+        <v>31.536000000000001</v>
+      </c>
+      <c r="B137">
+        <v>-0.3</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+      <c r="D137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138">
+        <v>31.736000000000001</v>
+      </c>
+      <c r="B138">
+        <v>0</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139">
+        <v>31.835999999999999</v>
+      </c>
+      <c r="B139">
+        <v>0.4</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+      <c r="D139">
         <v>1</v>
       </c>
     </row>
@@ -2420,10 +3125,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B2D43-E0B0-4050-83A2-AF5C6E5EE029}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3210,7 +3915,7 @@
         <v>-2</v>
       </c>
       <c r="E25">
-        <v>-0.6</v>
+        <v>-1</v>
       </c>
       <c r="F25">
         <v>25.43600000000005</v>
@@ -3219,12 +3924,172 @@
         <v>-2</v>
       </c>
       <c r="H25">
-        <v>-0.6</v>
+        <v>-1</v>
       </c>
       <c r="I25" t="s">
         <v>25</v>
       </c>
       <c r="J25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>18</v>
+      </c>
+      <c r="C26">
+        <v>25.635999999999999</v>
+      </c>
+      <c r="D26">
+        <v>-2</v>
+      </c>
+      <c r="E26">
+        <v>-0.5</v>
+      </c>
+      <c r="F26">
+        <v>25.936</v>
+      </c>
+      <c r="G26">
+        <v>0.5</v>
+      </c>
+      <c r="H26">
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>25</v>
+      </c>
+      <c r="J26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>19</v>
+      </c>
+      <c r="C27">
+        <v>25.635999999999999</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>1.5</v>
+      </c>
+      <c r="F27">
+        <v>25.936</v>
+      </c>
+      <c r="G27">
+        <v>0.5</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>20</v>
+      </c>
+      <c r="C28">
+        <v>31.436</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
+      <c r="F28">
+        <v>31.835999999999999</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>2</v>
+      </c>
+      <c r="I28" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>21</v>
+      </c>
+      <c r="C29">
+        <v>32.036000000000001</v>
+      </c>
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>32.335999999999999</v>
+      </c>
+      <c r="G29">
+        <v>-2</v>
+      </c>
+      <c r="H29">
+        <v>-0.5</v>
+      </c>
+      <c r="I29" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>22</v>
+      </c>
+      <c r="C30">
+        <v>32.036000000000001</v>
+      </c>
+      <c r="D30">
+        <v>-1.5</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>32.335999999999999</v>
+      </c>
+      <c r="G30">
+        <v>-2</v>
+      </c>
+      <c r="H30">
+        <v>-0.5</v>
+      </c>
+      <c r="I30" t="s">
+        <v>25</v>
+      </c>
+      <c r="J30" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3562,10 +4427,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F96158-71D4-4C19-99F5-47E7932AF572}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3720,6 +4585,108 @@
         <v>0.25</v>
       </c>
       <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>26.036000000000001</v>
+      </c>
+      <c r="B10">
+        <v>-1</v>
+      </c>
+      <c r="C10">
+        <v>1.6</v>
+      </c>
+      <c r="D10">
+        <v>0.75</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>26.036000000000001</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1.6</v>
+      </c>
+      <c r="D11">
+        <v>0.25</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>29.236000000000001</v>
+      </c>
+      <c r="B12">
+        <v>-1</v>
+      </c>
+      <c r="C12">
+        <v>1.6</v>
+      </c>
+      <c r="D12">
+        <v>0.75</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>29.236000000000001</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1.6</v>
+      </c>
+      <c r="D13">
+        <v>0.25</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>32.436</v>
+      </c>
+      <c r="B14">
+        <v>-1</v>
+      </c>
+      <c r="C14">
+        <v>1.6</v>
+      </c>
+      <c r="D14">
+        <v>0.75</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>32.436</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1.6</v>
+      </c>
+      <c r="D15">
+        <v>0.25</v>
+      </c>
+      <c r="E15">
         <v>1</v>
       </c>
     </row>
@@ -4260,10 +5227,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC7596AC-A6F6-4FB8-B823-5B4B1777330C}">
-  <dimension ref="A1:N41"/>
+  <dimension ref="A1:N83"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="M37" activeCellId="1" sqref="M33:M35 M37:M38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4322,7 +5289,7 @@
         <v>3.6360000000000001</v>
       </c>
       <c r="M4">
-        <v>22.036000000000001</v>
+        <v>29.236000000000001</v>
       </c>
       <c r="N4">
         <v>3.2360000000000002</v>
@@ -4338,8 +5305,7 @@
         <v>3.8360000000000003</v>
       </c>
       <c r="M5">
-        <f>M4+0.1</f>
-        <v>22.136000000000003</v>
+        <v>29.335999999999999</v>
       </c>
       <c r="N5" s="1">
         <f>N4+$N$2</f>
@@ -4356,11 +5322,10 @@
         <v>4.0360000000000005</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6:M41" si="2">M5+0.1</f>
-        <v>22.236000000000004</v>
+        <v>29.436</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" ref="N6:N10" si="3">N5+$N$2</f>
+        <f t="shared" ref="N6:N10" si="2">N5+$N$2</f>
         <v>3.3700000000000006</v>
       </c>
     </row>
@@ -4374,11 +5339,10 @@
         <v>4.2360000000000007</v>
       </c>
       <c r="M7">
+        <v>29.536000000000001</v>
+      </c>
+      <c r="N7" s="1">
         <f t="shared" si="2"/>
-        <v>22.336000000000006</v>
-      </c>
-      <c r="N7" s="1">
-        <f t="shared" si="3"/>
         <v>3.4370000000000007</v>
       </c>
     </row>
@@ -4392,11 +5356,10 @@
         <v>4.4360000000000008</v>
       </c>
       <c r="M8">
+        <v>29.635999999999999</v>
+      </c>
+      <c r="N8" s="1">
         <f t="shared" si="2"/>
-        <v>22.436000000000007</v>
-      </c>
-      <c r="N8" s="1">
-        <f t="shared" si="3"/>
         <v>3.5040000000000009</v>
       </c>
     </row>
@@ -4410,11 +5373,10 @@
         <v>4.636000000000001</v>
       </c>
       <c r="M9">
+        <v>29.736000000000001</v>
+      </c>
+      <c r="N9" s="1">
         <f t="shared" si="2"/>
-        <v>22.536000000000008</v>
-      </c>
-      <c r="N9" s="1">
-        <f t="shared" si="3"/>
         <v>3.5710000000000011</v>
       </c>
     </row>
@@ -4428,11 +5390,10 @@
         <v>4.8360000000000012</v>
       </c>
       <c r="M10">
+        <v>29.835999999999999</v>
+      </c>
+      <c r="N10" s="1">
         <f t="shared" si="2"/>
-        <v>22.63600000000001</v>
-      </c>
-      <c r="N10" s="1">
-        <f t="shared" si="3"/>
         <v>3.6380000000000012</v>
       </c>
     </row>
@@ -4446,8 +5407,7 @@
         <v>5.0360000000000014</v>
       </c>
       <c r="M11">
-        <f t="shared" si="2"/>
-        <v>22.736000000000011</v>
+        <v>29.936</v>
       </c>
       <c r="N11" s="1"/>
     </row>
@@ -4461,8 +5421,7 @@
         <v>5.2360000000000015</v>
       </c>
       <c r="M12">
-        <f t="shared" si="2"/>
-        <v>22.836000000000013</v>
+        <v>30.036000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -4475,8 +5434,7 @@
         <v>5.4360000000000017</v>
       </c>
       <c r="M13">
-        <f t="shared" si="2"/>
-        <v>22.936000000000014</v>
+        <v>30.135999999999999</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -4485,8 +5443,7 @@
         <v>12.836000000000004</v>
       </c>
       <c r="M14">
-        <f t="shared" si="2"/>
-        <v>23.036000000000016</v>
+        <v>30.236000000000001</v>
       </c>
       <c r="N14">
         <v>21.635999999999999</v>
@@ -4498,8 +5455,7 @@
         <v>13.236000000000004</v>
       </c>
       <c r="M15">
-        <f t="shared" si="2"/>
-        <v>23.136000000000017</v>
+        <v>30.335999999999999</v>
       </c>
       <c r="N15">
         <f>N14+$N$2</f>
@@ -4512,8 +5468,7 @@
         <v>13.636000000000005</v>
       </c>
       <c r="M16">
-        <f t="shared" si="2"/>
-        <v>23.236000000000018</v>
+        <v>30.436</v>
       </c>
       <c r="N16">
         <f>N15+$N$2</f>
@@ -4526,8 +5481,7 @@
         <v>14.036000000000005</v>
       </c>
       <c r="M17">
-        <f t="shared" si="2"/>
-        <v>23.33600000000002</v>
+        <v>30.536000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -4536,8 +5490,7 @@
         <v>14.436000000000005</v>
       </c>
       <c r="M18">
-        <f t="shared" si="2"/>
-        <v>23.436000000000021</v>
+        <v>30.635999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -4546,8 +5499,7 @@
         <v>14.836000000000006</v>
       </c>
       <c r="M19">
-        <f t="shared" si="2"/>
-        <v>23.536000000000023</v>
+        <v>30.736000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -4556,8 +5508,7 @@
         <v>15.236000000000006</v>
       </c>
       <c r="M20">
-        <f t="shared" si="2"/>
-        <v>23.636000000000024</v>
+        <v>30.835999999999999</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -4566,8 +5517,7 @@
         <v>15.636000000000006</v>
       </c>
       <c r="M21">
-        <f t="shared" si="2"/>
-        <v>23.736000000000026</v>
+        <v>30.936</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -4576,8 +5526,7 @@
         <v>16.036000000000005</v>
       </c>
       <c r="M22">
-        <f t="shared" si="2"/>
-        <v>23.836000000000027</v>
+        <v>31.036000000000001</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -4586,8 +5535,7 @@
         <v>16.436000000000003</v>
       </c>
       <c r="M23">
-        <f t="shared" si="2"/>
-        <v>23.936000000000028</v>
+        <v>31.135999999999999</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -4596,8 +5544,7 @@
         <v>16.836000000000002</v>
       </c>
       <c r="M24">
-        <f t="shared" si="2"/>
-        <v>24.03600000000003</v>
+        <v>31.236000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -4606,8 +5553,7 @@
         <v>17.236000000000001</v>
       </c>
       <c r="M25">
-        <f t="shared" si="2"/>
-        <v>24.136000000000031</v>
+        <v>31.335999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -4616,14 +5562,12 @@
         <v>17.635999999999999</v>
       </c>
       <c r="M26">
-        <f t="shared" si="2"/>
-        <v>24.236000000000033</v>
+        <v>31.436</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M27">
-        <f t="shared" si="2"/>
-        <v>24.336000000000034</v>
+        <v>31.536000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -4631,8 +5575,7 @@
         <v>19.635999999999999</v>
       </c>
       <c r="M28">
-        <f t="shared" si="2"/>
-        <v>24.436000000000035</v>
+        <v>31.6359999999999</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -4640,8 +5583,7 @@
         <v>20.036000000000001</v>
       </c>
       <c r="M29">
-        <f t="shared" si="2"/>
-        <v>24.536000000000037</v>
+        <v>31.736000000000001</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -4649,8 +5591,7 @@
         <v>20.436</v>
       </c>
       <c r="M30">
-        <f t="shared" si="2"/>
-        <v>24.636000000000038</v>
+        <v>31.835999999999899</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -4658,8 +5599,7 @@
         <v>20.835999999999999</v>
       </c>
       <c r="M31">
-        <f t="shared" si="2"/>
-        <v>24.73600000000004</v>
+        <v>31.9359999999999</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -4667,8 +5607,7 @@
         <v>21.236000000000001</v>
       </c>
       <c r="M32">
-        <f t="shared" si="2"/>
-        <v>24.836000000000041</v>
+        <v>32.035999999999902</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -4676,8 +5615,7 @@
         <v>21.635999999999999</v>
       </c>
       <c r="M33">
-        <f t="shared" si="2"/>
-        <v>24.936000000000043</v>
+        <v>32.135999999999903</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -4685,8 +5623,7 @@
         <v>22.036000000000001</v>
       </c>
       <c r="M34">
-        <f t="shared" si="2"/>
-        <v>25.036000000000044</v>
+        <v>32.235999999999898</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -4694,8 +5631,7 @@
         <v>22.436</v>
       </c>
       <c r="M35">
-        <f t="shared" si="2"/>
-        <v>25.136000000000045</v>
+        <v>32.335999999999899</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -4703,8 +5639,7 @@
         <v>22.835999999999999</v>
       </c>
       <c r="M36">
-        <f t="shared" si="2"/>
-        <v>25.236000000000047</v>
+        <v>32.4359999999999</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -4712,8 +5647,7 @@
         <v>23.236000000000001</v>
       </c>
       <c r="M37">
-        <f t="shared" si="2"/>
-        <v>25.336000000000048</v>
+        <v>32.535999999999902</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -4721,8 +5655,7 @@
         <v>23.635999999999999</v>
       </c>
       <c r="M38">
-        <f t="shared" si="2"/>
-        <v>25.43600000000005</v>
+        <v>32.635999999999903</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
@@ -4730,8 +5663,7 @@
         <v>24.036000000000001</v>
       </c>
       <c r="M39">
-        <f t="shared" si="2"/>
-        <v>25.536000000000051</v>
+        <v>32.735999999999898</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
@@ -4739,8 +5671,7 @@
         <v>24.436</v>
       </c>
       <c r="M40">
-        <f t="shared" si="2"/>
-        <v>25.636000000000053</v>
+        <v>32.835999999999899</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
@@ -4748,8 +5679,122 @@
         <v>24.835999999999999</v>
       </c>
       <c r="M41">
-        <f t="shared" si="2"/>
-        <v>25.736000000000054</v>
+        <v>32.9359999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>25.236000000000001</v>
+      </c>
+      <c r="M42">
+        <v>33.035999999999902</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>25.635999999999999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>26.036000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>26.436</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>26.835999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>27.236000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>27.635999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>28.036000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>28.436</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>28.835999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>29.236000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>29.635999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>30.036000000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>30.436</v>
+      </c>
+    </row>
+    <row r="77" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M77">
+        <f>M4+0.1</f>
+        <v>29.336000000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M78">
+        <f t="shared" ref="M78:M83" si="3">M77+0.1</f>
+        <v>29.436000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M79">
+        <f t="shared" si="3"/>
+        <v>29.536000000000005</v>
+      </c>
+    </row>
+    <row r="80" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M80">
+        <f t="shared" si="3"/>
+        <v>29.636000000000006</v>
+      </c>
+    </row>
+    <row r="81" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M81">
+        <f t="shared" si="3"/>
+        <v>29.736000000000008</v>
+      </c>
+    </row>
+    <row r="82" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M82">
+        <f t="shared" si="3"/>
+        <v>29.836000000000009</v>
+      </c>
+    </row>
+    <row r="83" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M83">
+        <f t="shared" si="3"/>
+        <v>29.936000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjust Note UI, add Pause function, and others..
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Chart示例.xlsx
+++ b/Assets/Scripts/Chart示例.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzh\Xenody-master\Assets\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Xenody-master\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{050C755E-3838-4135-AD32-1BCC6ED2D49D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA28C80F-67CA-446E-8800-832C310BF9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="planes" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,26 @@
     <sheet name="stars" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="33">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -522,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA789EFB-BCA3-4FCA-98D4-565CD71AE543}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1147,6 +1156,326 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>35.536000000000001</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>36.335999999999999</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>36.335999999999999</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>37.135999999999996</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>36.335999999999999</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>37.135999999999996</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>37.135999999999996</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>37.935999999999993</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>37.135999999999996</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>37.935999999999993</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>37.935999999999993</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>38.73599999999999</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>37.935999999999993</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>38.73599999999999</v>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>38.73599999999999</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>39.535999999999987</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="B40">
+        <v>38.73599999999999</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>39.535999999999987</v>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+      <c r="F40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <v>39.535999999999987</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>40.335999999999984</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>39.535999999999987</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>40.335999999999984</v>
+      </c>
+      <c r="E42">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43">
+        <v>40.335999999999984</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>41.135999999999981</v>
+      </c>
+      <c r="E43">
+        <v>1</v>
+      </c>
+      <c r="F43" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>9</v>
+      </c>
+      <c r="B44">
+        <v>40.335999999999984</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>41.135999999999981</v>
+      </c>
+      <c r="E44">
+        <v>1</v>
+      </c>
+      <c r="F44" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>9</v>
+      </c>
+      <c r="B45">
+        <v>41.135999999999981</v>
+      </c>
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45">
+        <v>41.935999999999979</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>10</v>
+      </c>
+      <c r="B46">
+        <v>41.135999999999981</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>41.935999999999979</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>10</v>
+      </c>
+      <c r="B47">
+        <v>41.935999999999979</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>42.735999999999976</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1159,10 +1488,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7059D0-50D6-42B0-899B-7876B4BEDB4C}">
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:F152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H97" sqref="H97"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1763,7 +2092,7 @@
         <v>17.035999999999998</v>
       </c>
       <c r="B43">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="C43">
         <v>0.8</v>
@@ -1777,7 +2106,7 @@
         <v>17.336000000000002</v>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>-0.8</v>
       </c>
       <c r="C44">
         <v>0.8</v>
@@ -1791,7 +2120,7 @@
         <v>17.636000000000006</v>
       </c>
       <c r="B45">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="C45">
         <v>0.8</v>
@@ -1805,7 +2134,7 @@
         <v>17.936000000000011</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>-0.8</v>
       </c>
       <c r="C46">
         <v>0.8</v>
@@ -3113,6 +3442,188 @@
         <v>1</v>
       </c>
       <c r="D139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>32.835999999999999</v>
+      </c>
+      <c r="B140">
+        <v>-1.5</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+      <c r="D140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141">
+        <v>33.136000000000003</v>
+      </c>
+      <c r="B141">
+        <v>-0.5</v>
+      </c>
+      <c r="C141">
+        <v>1</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142">
+        <v>33.235999999999997</v>
+      </c>
+      <c r="B142">
+        <v>0</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143">
+        <v>33.436</v>
+      </c>
+      <c r="B143">
+        <v>0.75</v>
+      </c>
+      <c r="C143">
+        <v>1</v>
+      </c>
+      <c r="D143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144">
+        <v>34.036000000000001</v>
+      </c>
+      <c r="B144">
+        <v>-1.2</v>
+      </c>
+      <c r="C144">
+        <v>1.6</v>
+      </c>
+      <c r="D144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A145">
+        <v>34.136000000000003</v>
+      </c>
+      <c r="B145">
+        <v>-1</v>
+      </c>
+      <c r="C145">
+        <v>0.8</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A146">
+        <v>34.335999999999999</v>
+      </c>
+      <c r="B146">
+        <v>1.6</v>
+      </c>
+      <c r="C146">
+        <v>0.8</v>
+      </c>
+      <c r="D146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A147">
+        <v>34.536000000000001</v>
+      </c>
+      <c r="B147">
+        <v>-1.6</v>
+      </c>
+      <c r="C147">
+        <v>0.8</v>
+      </c>
+      <c r="D147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A148">
+        <v>34.735999999999997</v>
+      </c>
+      <c r="B148">
+        <v>1.2</v>
+      </c>
+      <c r="C148">
+        <v>0.8</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A149">
+        <v>34.936</v>
+      </c>
+      <c r="B149">
+        <v>-1.2</v>
+      </c>
+      <c r="C149">
+        <v>0.8</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A150">
+        <v>35.136000000000003</v>
+      </c>
+      <c r="B150">
+        <v>1.2</v>
+      </c>
+      <c r="C150">
+        <v>0.8</v>
+      </c>
+      <c r="D150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A151">
+        <v>35.235999999999997</v>
+      </c>
+      <c r="B151">
+        <v>-1.2</v>
+      </c>
+      <c r="C151">
+        <v>0.8</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A152">
+        <v>35.436</v>
+      </c>
+      <c r="B152">
+        <v>-1.6</v>
+      </c>
+      <c r="C152">
+        <v>0.8</v>
+      </c>
+      <c r="D152">
         <v>1</v>
       </c>
     </row>
@@ -3125,10 +3636,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B2D43-E0B0-4050-83A2-AF5C6E5EE029}">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4090,6 +4601,230 @@
         <v>25</v>
       </c>
       <c r="J30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>23</v>
+      </c>
+      <c r="C31">
+        <v>32.436</v>
+      </c>
+      <c r="D31">
+        <v>-2</v>
+      </c>
+      <c r="E31">
+        <v>2</v>
+      </c>
+      <c r="F31">
+        <v>33.835999999999999</v>
+      </c>
+      <c r="G31">
+        <v>-0.5</v>
+      </c>
+      <c r="H31">
+        <v>0.5</v>
+      </c>
+      <c r="I31" t="s">
+        <v>32</v>
+      </c>
+      <c r="J31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>24</v>
+      </c>
+      <c r="C32">
+        <v>34.036000000000001</v>
+      </c>
+      <c r="D32">
+        <v>0.4</v>
+      </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
+      <c r="F32">
+        <v>34.335999999999999</v>
+      </c>
+      <c r="G32">
+        <v>-2</v>
+      </c>
+      <c r="H32">
+        <v>-1.2</v>
+      </c>
+      <c r="I32" t="s">
+        <v>25</v>
+      </c>
+      <c r="J32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>24</v>
+      </c>
+      <c r="C33">
+        <v>34.335999999999999</v>
+      </c>
+      <c r="D33">
+        <v>-2</v>
+      </c>
+      <c r="E33">
+        <v>-1.2</v>
+      </c>
+      <c r="F33">
+        <v>34.536000000000001</v>
+      </c>
+      <c r="G33">
+        <v>1.2</v>
+      </c>
+      <c r="H33">
+        <v>2</v>
+      </c>
+      <c r="I33" t="s">
+        <v>25</v>
+      </c>
+      <c r="J33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>24</v>
+      </c>
+      <c r="C34">
+        <v>34.536000000000001</v>
+      </c>
+      <c r="D34">
+        <v>1.2</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+      <c r="F34">
+        <v>34.735999999999997</v>
+      </c>
+      <c r="G34">
+        <v>-1.6</v>
+      </c>
+      <c r="H34">
+        <v>-0.8</v>
+      </c>
+      <c r="I34" t="s">
+        <v>25</v>
+      </c>
+      <c r="J34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <v>34.735999999999997</v>
+      </c>
+      <c r="D35">
+        <v>-1.6</v>
+      </c>
+      <c r="E35">
+        <v>-0.8</v>
+      </c>
+      <c r="F35">
+        <v>34.936</v>
+      </c>
+      <c r="G35">
+        <v>0.8</v>
+      </c>
+      <c r="H35">
+        <v>1.6</v>
+      </c>
+      <c r="I35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>24</v>
+      </c>
+      <c r="C36">
+        <v>34.936</v>
+      </c>
+      <c r="D36">
+        <v>0.8</v>
+      </c>
+      <c r="E36">
+        <v>1.6</v>
+      </c>
+      <c r="F36">
+        <v>35.136000000000003</v>
+      </c>
+      <c r="G36">
+        <v>-1.6</v>
+      </c>
+      <c r="H36">
+        <v>-0.8</v>
+      </c>
+      <c r="I36" t="s">
+        <v>25</v>
+      </c>
+      <c r="J36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>25</v>
+      </c>
+      <c r="C37">
+        <v>35.536000000000001</v>
+      </c>
+      <c r="D37">
+        <v>-2</v>
+      </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>10000</v>
+      </c>
+      <c r="G37">
+        <v>-2</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37" t="s">
+        <v>25</v>
+      </c>
+      <c r="J37" t="s">
         <v>25</v>
       </c>
     </row>
@@ -4102,10 +4837,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C76DC57-EF49-44CE-8A21-D4353938F627}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4272,7 +5007,7 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0.8</v>
+        <v>1.5</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -4415,6 +5150,48 @@
         <v>0.6</v>
       </c>
       <c r="D22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>33.636000000000003</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>33.735999999999997</v>
+      </c>
+      <c r="B24">
+        <v>0.5</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>33.835999999999999</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
         <v>1</v>
       </c>
     </row>
@@ -4427,10 +5204,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F96158-71D4-4C19-99F5-47E7932AF572}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4653,40 +5430,6 @@
         <v>0.25</v>
       </c>
       <c r="E13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>32.436</v>
-      </c>
-      <c r="B14">
-        <v>-1</v>
-      </c>
-      <c r="C14">
-        <v>1.6</v>
-      </c>
-      <c r="D14">
-        <v>0.75</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>32.436</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1.6</v>
-      </c>
-      <c r="D15">
-        <v>0.25</v>
-      </c>
-      <c r="E15">
         <v>1</v>
       </c>
     </row>
@@ -4701,7 +5444,7 @@
   <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5075,13 +5818,13 @@
         <v>16.935999999999996</v>
       </c>
       <c r="F12">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
       <c r="H12">
-        <v>-1.6</v>
+        <v>-0.6</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -5107,13 +5850,13 @@
         <v>17.236000000000001</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="H13">
-        <v>1.6</v>
+        <v>0.6</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -5139,13 +5882,13 @@
         <v>17.536000000000005</v>
       </c>
       <c r="F14">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="H14">
-        <v>-1.6</v>
+        <v>-0.6</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -5171,13 +5914,13 @@
         <v>17.836000000000009</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
       <c r="H15">
-        <v>1.6</v>
+        <v>0.6</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -5203,13 +5946,13 @@
         <v>18.136000000000013</v>
       </c>
       <c r="F16">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="G16">
         <v>1</v>
       </c>
       <c r="H16">
-        <v>-1.6</v>
+        <v>-0.6</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -5230,7 +5973,7 @@
   <dimension ref="A1:N83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="J8" sqref="J8:J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5285,6 +6028,12 @@
         <f t="shared" ref="A4:A26" si="0">A3+$K$2</f>
         <v>8.8360000000000003</v>
       </c>
+      <c r="J4">
+        <v>35.536000000000001</v>
+      </c>
+      <c r="K4">
+        <v>35.536000000000001</v>
+      </c>
       <c r="L4">
         <v>3.6360000000000001</v>
       </c>
@@ -5300,6 +6049,14 @@
         <f t="shared" si="0"/>
         <v>9.2360000000000007</v>
       </c>
+      <c r="J5">
+        <f>J4+$K$2*2</f>
+        <v>36.335999999999999</v>
+      </c>
+      <c r="K5">
+        <f>K4+$K$2</f>
+        <v>35.936</v>
+      </c>
       <c r="L5">
         <f>L4+$L$2</f>
         <v>3.8360000000000003</v>
@@ -5317,15 +6074,22 @@
         <f t="shared" si="0"/>
         <v>9.636000000000001</v>
       </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J23" si="1">J5+$K$2*2</f>
+        <v>37.135999999999996</v>
+      </c>
+      <c r="K6">
+        <v>36.536000000000001</v>
+      </c>
       <c r="L6">
-        <f t="shared" ref="L6:L13" si="1">L5+$L$2</f>
+        <f t="shared" ref="L6:L13" si="2">L5+$L$2</f>
         <v>4.0360000000000005</v>
       </c>
       <c r="M6">
         <v>29.436</v>
       </c>
       <c r="N6" s="1">
-        <f t="shared" ref="N6:N10" si="2">N5+$N$2</f>
+        <f t="shared" ref="N6:N10" si="3">N5+$N$2</f>
         <v>3.3700000000000006</v>
       </c>
     </row>
@@ -5334,15 +6098,23 @@
         <f t="shared" si="0"/>
         <v>10.036000000000001</v>
       </c>
+      <c r="J7">
+        <f t="shared" si="1"/>
+        <v>37.935999999999993</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="J7:K23" si="4">K6+$K$2</f>
+        <v>36.936</v>
+      </c>
       <c r="L7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.2360000000000007</v>
       </c>
       <c r="M7">
         <v>29.536000000000001</v>
       </c>
       <c r="N7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.4370000000000007</v>
       </c>
     </row>
@@ -5351,15 +6123,22 @@
         <f t="shared" si="0"/>
         <v>10.436000000000002</v>
       </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>38.73599999999999</v>
+      </c>
+      <c r="K8">
+        <v>37.536000000000001</v>
+      </c>
       <c r="L8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.4360000000000008</v>
       </c>
       <c r="M8">
         <v>29.635999999999999</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5040000000000009</v>
       </c>
     </row>
@@ -5368,15 +6147,23 @@
         <f t="shared" si="0"/>
         <v>10.836000000000002</v>
       </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>39.535999999999987</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ref="J9:K23" si="5">K8+$K$2</f>
+        <v>37.936</v>
+      </c>
       <c r="L9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.636000000000001</v>
       </c>
       <c r="M9">
         <v>29.736000000000001</v>
       </c>
       <c r="N9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5710000000000011</v>
       </c>
     </row>
@@ -5385,15 +6172,22 @@
         <f t="shared" si="0"/>
         <v>11.236000000000002</v>
       </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>40.335999999999984</v>
+      </c>
+      <c r="K10">
+        <v>38.536000000000001</v>
+      </c>
       <c r="L10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.8360000000000012</v>
       </c>
       <c r="M10">
         <v>29.835999999999999</v>
       </c>
       <c r="N10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.6380000000000012</v>
       </c>
     </row>
@@ -5402,8 +6196,16 @@
         <f t="shared" si="0"/>
         <v>11.636000000000003</v>
       </c>
+      <c r="J11">
+        <f t="shared" si="1"/>
+        <v>41.135999999999981</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ref="J11:K23" si="6">K10+$K$2</f>
+        <v>38.936</v>
+      </c>
       <c r="L11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.0360000000000014</v>
       </c>
       <c r="M11">
@@ -5416,8 +6218,15 @@
         <f t="shared" si="0"/>
         <v>12.036000000000003</v>
       </c>
+      <c r="J12">
+        <f t="shared" si="1"/>
+        <v>41.935999999999979</v>
+      </c>
+      <c r="K12">
+        <v>39.536000000000001</v>
+      </c>
       <c r="L12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.2360000000000015</v>
       </c>
       <c r="M12">
@@ -5429,8 +6238,16 @@
         <f t="shared" si="0"/>
         <v>12.436000000000003</v>
       </c>
+      <c r="J13">
+        <f t="shared" si="1"/>
+        <v>42.735999999999976</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ref="J13:K23" si="7">K12+$K$2</f>
+        <v>39.936</v>
+      </c>
       <c r="L13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.4360000000000017</v>
       </c>
       <c r="M13">
@@ -5442,6 +6259,13 @@
         <f t="shared" si="0"/>
         <v>12.836000000000004</v>
       </c>
+      <c r="J14">
+        <f t="shared" si="1"/>
+        <v>43.535999999999973</v>
+      </c>
+      <c r="K14">
+        <v>40.536000000000001</v>
+      </c>
       <c r="M14">
         <v>30.236000000000001</v>
       </c>
@@ -5454,6 +6278,14 @@
         <f t="shared" si="0"/>
         <v>13.236000000000004</v>
       </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>44.33599999999997</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ref="J15:K23" si="8">K14+$K$2</f>
+        <v>40.936</v>
+      </c>
       <c r="M15">
         <v>30.335999999999999</v>
       </c>
@@ -5467,6 +6299,13 @@
         <f t="shared" si="0"/>
         <v>13.636000000000005</v>
       </c>
+      <c r="J16">
+        <f t="shared" si="1"/>
+        <v>45.135999999999967</v>
+      </c>
+      <c r="K16">
+        <v>41.536000000000001</v>
+      </c>
       <c r="M16">
         <v>30.436</v>
       </c>
@@ -5480,6 +6319,14 @@
         <f t="shared" si="0"/>
         <v>14.036000000000005</v>
       </c>
+      <c r="J17">
+        <f t="shared" si="1"/>
+        <v>45.935999999999964</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ref="J17:K23" si="9">K16+$K$2</f>
+        <v>41.936</v>
+      </c>
       <c r="M17">
         <v>30.536000000000001</v>
       </c>
@@ -5489,6 +6336,13 @@
         <f t="shared" si="0"/>
         <v>14.436000000000005</v>
       </c>
+      <c r="J18">
+        <f t="shared" si="1"/>
+        <v>46.735999999999962</v>
+      </c>
+      <c r="K18">
+        <v>42.536000000000001</v>
+      </c>
       <c r="M18">
         <v>30.635999999999999</v>
       </c>
@@ -5498,6 +6352,14 @@
         <f t="shared" si="0"/>
         <v>14.836000000000006</v>
       </c>
+      <c r="J19">
+        <f t="shared" si="1"/>
+        <v>47.535999999999959</v>
+      </c>
+      <c r="K19">
+        <f t="shared" ref="J19:K23" si="10">K18+$K$2</f>
+        <v>42.936</v>
+      </c>
       <c r="M19">
         <v>30.736000000000001</v>
       </c>
@@ -5507,6 +6369,13 @@
         <f t="shared" si="0"/>
         <v>15.236000000000006</v>
       </c>
+      <c r="J20">
+        <f t="shared" si="1"/>
+        <v>48.335999999999956</v>
+      </c>
+      <c r="K20">
+        <v>43.536000000000001</v>
+      </c>
       <c r="M20">
         <v>30.835999999999999</v>
       </c>
@@ -5516,6 +6385,14 @@
         <f t="shared" si="0"/>
         <v>15.636000000000006</v>
       </c>
+      <c r="J21">
+        <f t="shared" si="1"/>
+        <v>49.135999999999953</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="J21:K23" si="11">K20+$K$2</f>
+        <v>43.936</v>
+      </c>
       <c r="M21">
         <v>30.936</v>
       </c>
@@ -5525,6 +6402,13 @@
         <f t="shared" si="0"/>
         <v>16.036000000000005</v>
       </c>
+      <c r="J22">
+        <f t="shared" si="1"/>
+        <v>49.93599999999995</v>
+      </c>
+      <c r="K22">
+        <v>44.536000000000001</v>
+      </c>
       <c r="M22">
         <v>31.036000000000001</v>
       </c>
@@ -5534,6 +6418,14 @@
         <f t="shared" si="0"/>
         <v>16.436000000000003</v>
       </c>
+      <c r="J23">
+        <f t="shared" si="1"/>
+        <v>50.735999999999947</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ref="J23:K23" si="12">K22+$K$2</f>
+        <v>44.936</v>
+      </c>
       <c r="M23">
         <v>31.135999999999999</v>
       </c>
@@ -5763,37 +6655,37 @@
     </row>
     <row r="78" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M78">
-        <f t="shared" ref="M78:M83" si="3">M77+0.1</f>
+        <f t="shared" ref="M78:M83" si="13">M77+0.1</f>
         <v>29.436000000000003</v>
       </c>
     </row>
     <row r="79" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M79">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>29.536000000000005</v>
       </c>
     </row>
     <row r="80" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M80">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>29.636000000000006</v>
       </c>
     </row>
     <row r="81" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M81">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>29.736000000000008</v>
       </c>
     </row>
     <row r="82" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M82">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>29.836000000000009</v>
       </c>
     </row>
     <row r="83" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M83">
-        <f t="shared" si="3"/>
+        <f t="shared" si="13"/>
         <v>29.936000000000011</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Arrow Appearance Bug
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Chart示例.xlsx
+++ b/Assets/Scripts/Chart示例.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Xenody-master\Assets\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzh\Xenody-master\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA28C80F-67CA-446E-8800-832C310BF9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8467604-B2BD-436E-9988-7B885C25EC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="planes" sheetId="1" r:id="rId1"/>
@@ -21,26 +21,17 @@
     <sheet name="stars" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="35">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,6 +152,14 @@
   </si>
   <si>
     <t>Sin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LowerCir</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UpperCir</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -534,7 +533,7 @@
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1164,13 +1163,13 @@
         <v>3</v>
       </c>
       <c r="B32">
-        <v>35.536000000000001</v>
+        <v>35.636000000000003</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>36.335999999999999</v>
+        <v>36.036000000000001</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1184,13 +1183,13 @@
         <v>3</v>
       </c>
       <c r="B33">
-        <v>36.335999999999999</v>
+        <v>36.036000000000001</v>
       </c>
       <c r="C33">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>37.135999999999996</v>
+        <v>37.235999999999997</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1204,13 +1203,13 @@
         <v>4</v>
       </c>
       <c r="B34">
-        <v>36.335999999999999</v>
+        <v>36.436</v>
       </c>
       <c r="C34">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>37.135999999999996</v>
+        <v>36.835999999999999</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1224,13 +1223,13 @@
         <v>4</v>
       </c>
       <c r="B35">
-        <v>37.135999999999996</v>
+        <v>36.835999999999999</v>
       </c>
       <c r="C35">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>37.935999999999993</v>
+        <v>38.035999999999994</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1244,13 +1243,13 @@
         <v>5</v>
       </c>
       <c r="B36">
-        <v>37.135999999999996</v>
+        <v>37.235999999999997</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>37.935999999999993</v>
+        <v>37.636000000000003</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1264,13 +1263,13 @@
         <v>5</v>
       </c>
       <c r="B37">
-        <v>37.935999999999993</v>
+        <v>37.636000000000003</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37">
-        <v>38.73599999999999</v>
+        <v>38.835999999999991</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1284,13 +1283,13 @@
         <v>6</v>
       </c>
       <c r="B38">
-        <v>37.935999999999993</v>
+        <v>38.035999999999994</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>38.73599999999999</v>
+        <v>38.436</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1304,13 +1303,13 @@
         <v>6</v>
       </c>
       <c r="B39">
-        <v>38.73599999999999</v>
+        <v>38.436</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39">
-        <v>39.535999999999987</v>
+        <v>39.635999999999989</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1324,13 +1323,13 @@
         <v>7</v>
       </c>
       <c r="B40">
-        <v>38.73599999999999</v>
+        <v>38.835999999999991</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>39.535999999999987</v>
+        <v>39.236000000000004</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1344,13 +1343,13 @@
         <v>7</v>
       </c>
       <c r="B41">
-        <v>39.535999999999987</v>
+        <v>39.236000000000004</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41">
-        <v>40.335999999999984</v>
+        <v>40.435999999999986</v>
       </c>
       <c r="E41">
         <v>1</v>
@@ -1364,13 +1363,13 @@
         <v>8</v>
       </c>
       <c r="B42">
-        <v>39.535999999999987</v>
+        <v>39.635999999999989</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>40.335999999999984</v>
+        <v>40.036000000000001</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1384,13 +1383,13 @@
         <v>8</v>
       </c>
       <c r="B43">
-        <v>40.335999999999984</v>
+        <v>40.036000000000001</v>
       </c>
       <c r="C43">
         <v>1</v>
       </c>
       <c r="D43">
-        <v>41.135999999999981</v>
+        <v>41.235999999999983</v>
       </c>
       <c r="E43">
         <v>1</v>
@@ -1404,13 +1403,13 @@
         <v>9</v>
       </c>
       <c r="B44">
-        <v>40.335999999999984</v>
+        <v>40.435999999999986</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
-        <v>41.135999999999981</v>
+        <v>40.835999999999999</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1424,13 +1423,13 @@
         <v>9</v>
       </c>
       <c r="B45">
-        <v>41.135999999999981</v>
+        <v>40.835999999999999</v>
       </c>
       <c r="C45">
         <v>1</v>
       </c>
       <c r="D45">
-        <v>41.935999999999979</v>
+        <v>42.03599999999998</v>
       </c>
       <c r="E45">
         <v>1</v>
@@ -1444,13 +1443,13 @@
         <v>10</v>
       </c>
       <c r="B46">
-        <v>41.135999999999981</v>
+        <v>41.235999999999983</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46">
-        <v>41.935999999999979</v>
+        <v>41.636000000000003</v>
       </c>
       <c r="E46">
         <v>1</v>
@@ -1464,13 +1463,13 @@
         <v>10</v>
       </c>
       <c r="B47">
-        <v>41.935999999999979</v>
+        <v>41.636000000000003</v>
       </c>
       <c r="C47">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>42.735999999999976</v>
+        <v>42.835999999999977</v>
       </c>
       <c r="E47">
         <v>1</v>
@@ -1488,10 +1487,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7059D0-50D6-42B0-899B-7876B4BEDB4C}">
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:F168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView topLeftCell="A139" workbookViewId="0">
+      <selection activeCell="H166" sqref="H166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3618,12 +3617,236 @@
         <v>35.436</v>
       </c>
       <c r="B152">
-        <v>-1.6</v>
+        <v>1.6</v>
       </c>
       <c r="C152">
         <v>0.8</v>
       </c>
       <c r="D152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A153">
+        <v>35.536000000000001</v>
+      </c>
+      <c r="B153">
+        <v>-1.6</v>
+      </c>
+      <c r="C153">
+        <v>0.8</v>
+      </c>
+      <c r="D153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A154">
+        <v>36.235999999999997</v>
+      </c>
+      <c r="B154">
+        <v>0.8</v>
+      </c>
+      <c r="C154">
+        <v>0.8</v>
+      </c>
+      <c r="D154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A155">
+        <v>36.436</v>
+      </c>
+      <c r="B155">
+        <v>1.6</v>
+      </c>
+      <c r="C155">
+        <v>0.8</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A156">
+        <v>36.735999999999997</v>
+      </c>
+      <c r="B156">
+        <v>1</v>
+      </c>
+      <c r="C156">
+        <v>0.8</v>
+      </c>
+      <c r="D156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A157">
+        <v>40.436</v>
+      </c>
+      <c r="B157">
+        <v>0</v>
+      </c>
+      <c r="C157">
+        <v>1.4</v>
+      </c>
+      <c r="D157">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A158">
+        <v>40.735999999999997</v>
+      </c>
+      <c r="B158">
+        <v>0</v>
+      </c>
+      <c r="C158">
+        <v>1.4</v>
+      </c>
+      <c r="D158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A159">
+        <v>41.036000000000001</v>
+      </c>
+      <c r="B159">
+        <v>0</v>
+      </c>
+      <c r="C159">
+        <v>1.4</v>
+      </c>
+      <c r="D159">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A160">
+        <v>41.436</v>
+      </c>
+      <c r="B160">
+        <v>-1.5</v>
+      </c>
+      <c r="C160">
+        <v>0.8</v>
+      </c>
+      <c r="D160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A161">
+        <v>41.536000000000001</v>
+      </c>
+      <c r="B161">
+        <v>-0.5</v>
+      </c>
+      <c r="C161">
+        <v>0.8</v>
+      </c>
+      <c r="D161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A162">
+        <v>41.636000000000003</v>
+      </c>
+      <c r="B162">
+        <v>-1.5</v>
+      </c>
+      <c r="C162">
+        <v>0.8</v>
+      </c>
+      <c r="D162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A163">
+        <v>41.936</v>
+      </c>
+      <c r="B163">
+        <v>0.5</v>
+      </c>
+      <c r="C163">
+        <v>0.8</v>
+      </c>
+      <c r="D163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A164">
+        <v>42.036000000000001</v>
+      </c>
+      <c r="B164">
+        <v>1.5</v>
+      </c>
+      <c r="C164">
+        <v>0.8</v>
+      </c>
+      <c r="D164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A165">
+        <v>42.335999999999999</v>
+      </c>
+      <c r="B165">
+        <v>-0.5</v>
+      </c>
+      <c r="C165">
+        <v>0.8</v>
+      </c>
+      <c r="D165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>42.436</v>
+      </c>
+      <c r="B166">
+        <v>-1.5</v>
+      </c>
+      <c r="C166">
+        <v>0.8</v>
+      </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>42.735999999999997</v>
+      </c>
+      <c r="B167">
+        <v>0.5</v>
+      </c>
+      <c r="C167">
+        <v>0.8</v>
+      </c>
+      <c r="D167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>42.835999999999999</v>
+      </c>
+      <c r="B168">
+        <v>1.5</v>
+      </c>
+      <c r="C168">
+        <v>0.8</v>
+      </c>
+      <c r="D168">
         <v>1</v>
       </c>
     </row>
@@ -3636,10 +3859,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B2D43-E0B0-4050-83A2-AF5C6E5EE029}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4798,34 +5021,194 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B37">
         <v>25</v>
       </c>
       <c r="C37">
-        <v>35.536000000000001</v>
+        <v>35.636000000000003</v>
       </c>
       <c r="D37">
+        <v>-0.4</v>
+      </c>
+      <c r="E37">
+        <v>0.4</v>
+      </c>
+      <c r="F37">
+        <v>36.036000000000001</v>
+      </c>
+      <c r="G37">
+        <v>1.2</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37" t="s">
+        <v>32</v>
+      </c>
+      <c r="J37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>26</v>
+      </c>
+      <c r="C38">
+        <v>36.436</v>
+      </c>
+      <c r="D38">
+        <v>-0.4</v>
+      </c>
+      <c r="E38">
+        <v>0.4</v>
+      </c>
+      <c r="F38">
+        <v>36.835999999999999</v>
+      </c>
+      <c r="G38">
         <v>-2</v>
       </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37">
-        <v>10000</v>
-      </c>
-      <c r="G37">
+      <c r="H38">
+        <v>-1.2</v>
+      </c>
+      <c r="I38" t="s">
+        <v>32</v>
+      </c>
+      <c r="J38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>27</v>
+      </c>
+      <c r="C39">
+        <v>37.235999999999997</v>
+      </c>
+      <c r="D39">
+        <v>-0.4</v>
+      </c>
+      <c r="E39">
+        <v>0.4</v>
+      </c>
+      <c r="F39">
+        <v>37.636000000000003</v>
+      </c>
+      <c r="G39">
+        <v>1.2</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39" t="s">
+        <v>32</v>
+      </c>
+      <c r="J39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>28</v>
+      </c>
+      <c r="C40">
+        <v>38.036000000000001</v>
+      </c>
+      <c r="D40">
+        <v>-0.4</v>
+      </c>
+      <c r="E40">
+        <v>0.4</v>
+      </c>
+      <c r="F40">
+        <v>38.436</v>
+      </c>
+      <c r="G40">
         <v>-2</v>
       </c>
-      <c r="H37">
-        <v>2</v>
-      </c>
-      <c r="I37" t="s">
-        <v>25</v>
-      </c>
-      <c r="J37" t="s">
-        <v>25</v>
+      <c r="H40">
+        <v>-1.2</v>
+      </c>
+      <c r="I40" t="s">
+        <v>32</v>
+      </c>
+      <c r="J40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <v>29</v>
+      </c>
+      <c r="C41">
+        <v>38.835999999999999</v>
+      </c>
+      <c r="D41">
+        <v>-0.4</v>
+      </c>
+      <c r="E41">
+        <v>0.4</v>
+      </c>
+      <c r="F41">
+        <v>39.235999999999997</v>
+      </c>
+      <c r="G41">
+        <v>1.2</v>
+      </c>
+      <c r="H41">
+        <v>2</v>
+      </c>
+      <c r="I41" t="s">
+        <v>32</v>
+      </c>
+      <c r="J41" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="B42">
+        <v>30</v>
+      </c>
+      <c r="C42">
+        <v>39.636000000000003</v>
+      </c>
+      <c r="D42">
+        <v>-0.4</v>
+      </c>
+      <c r="E42">
+        <v>0.4</v>
+      </c>
+      <c r="F42">
+        <v>40.036000000000001</v>
+      </c>
+      <c r="G42">
+        <v>-2</v>
+      </c>
+      <c r="H42">
+        <v>-1.2</v>
+      </c>
+      <c r="I42" t="s">
+        <v>32</v>
+      </c>
+      <c r="J42" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -4837,10 +5220,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C76DC57-EF49-44CE-8A21-D4353938F627}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5192,6 +5575,48 @@
         <v>1</v>
       </c>
       <c r="D25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>38.235999999999997</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>0.8</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>38.335999999999999</v>
+      </c>
+      <c r="B27">
+        <v>0.5</v>
+      </c>
+      <c r="C27">
+        <v>0.8</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>38.436</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0.8</v>
+      </c>
+      <c r="D28">
         <v>1</v>
       </c>
     </row>
@@ -5204,10 +5629,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F96158-71D4-4C19-99F5-47E7932AF572}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5430,6 +5855,74 @@
         <v>0.25</v>
       </c>
       <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>36.036000000000001</v>
+      </c>
+      <c r="B14">
+        <v>1.6</v>
+      </c>
+      <c r="C14">
+        <v>0.8</v>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>36.835999999999999</v>
+      </c>
+      <c r="B15">
+        <v>-1.6</v>
+      </c>
+      <c r="C15">
+        <v>0.8</v>
+      </c>
+      <c r="D15">
+        <v>0.5</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>37.636000000000003</v>
+      </c>
+      <c r="B16">
+        <v>1.6</v>
+      </c>
+      <c r="C16">
+        <v>0.8</v>
+      </c>
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>40.835999999999999</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
         <v>1</v>
       </c>
     </row>
@@ -5441,10 +5934,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192095B2-1BEA-4365-B4DE-88EEBB6E4423}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28:I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5958,6 +6451,262 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>37.036000000000001</v>
+      </c>
+      <c r="D17">
+        <v>37.235999999999997</v>
+      </c>
+      <c r="E17">
+        <v>37.636000000000003</v>
+      </c>
+      <c r="F17">
+        <v>-1.2</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>37.036000000000001</v>
+      </c>
+      <c r="D18">
+        <v>37.636000000000003</v>
+      </c>
+      <c r="E18">
+        <v>38.036000000000001</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>-1.2</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>38.636000000000003</v>
+      </c>
+      <c r="D19">
+        <v>38.835999999999999</v>
+      </c>
+      <c r="E19">
+        <v>39.235999999999997</v>
+      </c>
+      <c r="F19">
+        <v>-1.2</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>39.436</v>
+      </c>
+      <c r="D20">
+        <v>39.636000000000003</v>
+      </c>
+      <c r="E20">
+        <v>40.036000000000001</v>
+      </c>
+      <c r="F20">
+        <v>1.2</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21">
+        <v>39.436</v>
+      </c>
+      <c r="D21">
+        <v>40.036000000000001</v>
+      </c>
+      <c r="E21">
+        <v>40.436</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1.2</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22">
+        <v>41.835999999999999</v>
+      </c>
+      <c r="D22">
+        <v>42.036000000000001</v>
+      </c>
+      <c r="E22">
+        <v>42.136000000000003</v>
+      </c>
+      <c r="F22">
+        <v>1.5</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23">
+        <v>42.235999999999997</v>
+      </c>
+      <c r="D23">
+        <v>42.436</v>
+      </c>
+      <c r="E23">
+        <v>42.536000000000001</v>
+      </c>
+      <c r="F23">
+        <v>-1.5</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>-1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24">
+        <v>42.636000000000003</v>
+      </c>
+      <c r="D24">
+        <v>42.835999999999999</v>
+      </c>
+      <c r="E24">
+        <v>42.936</v>
+      </c>
+      <c r="F24">
+        <v>1.5</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24" t="s">
         <v>23</v>
       </c>
     </row>
@@ -5973,7 +6722,7 @@
   <dimension ref="A1:N83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8:J23"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6103,7 +6852,7 @@
         <v>37.935999999999993</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="J7:K23" si="4">K6+$K$2</f>
+        <f t="shared" ref="K7" si="4">K6+$K$2</f>
         <v>36.936</v>
       </c>
       <c r="L7">
@@ -6152,7 +6901,7 @@
         <v>39.535999999999987</v>
       </c>
       <c r="K9">
-        <f t="shared" ref="J9:K23" si="5">K8+$K$2</f>
+        <f t="shared" ref="K9" si="5">K8+$K$2</f>
         <v>37.936</v>
       </c>
       <c r="L9">
@@ -6201,7 +6950,7 @@
         <v>41.135999999999981</v>
       </c>
       <c r="K11">
-        <f t="shared" ref="J11:K23" si="6">K10+$K$2</f>
+        <f t="shared" ref="K11" si="6">K10+$K$2</f>
         <v>38.936</v>
       </c>
       <c r="L11">
@@ -6243,7 +6992,7 @@
         <v>42.735999999999976</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="J13:K23" si="7">K12+$K$2</f>
+        <f t="shared" ref="K13" si="7">K12+$K$2</f>
         <v>39.936</v>
       </c>
       <c r="L13">
@@ -6283,7 +7032,7 @@
         <v>44.33599999999997</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="J15:K23" si="8">K14+$K$2</f>
+        <f t="shared" ref="K15" si="8">K14+$K$2</f>
         <v>40.936</v>
       </c>
       <c r="M15">
@@ -6324,7 +7073,7 @@
         <v>45.935999999999964</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="J17:K23" si="9">K16+$K$2</f>
+        <f t="shared" ref="K17" si="9">K16+$K$2</f>
         <v>41.936</v>
       </c>
       <c r="M17">
@@ -6357,7 +7106,7 @@
         <v>47.535999999999959</v>
       </c>
       <c r="K19">
-        <f t="shared" ref="J19:K23" si="10">K18+$K$2</f>
+        <f t="shared" ref="K19" si="10">K18+$K$2</f>
         <v>42.936</v>
       </c>
       <c r="M19">
@@ -6390,7 +7139,7 @@
         <v>49.135999999999953</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="J21:K23" si="11">K20+$K$2</f>
+        <f t="shared" ref="K21" si="11">K20+$K$2</f>
         <v>43.936</v>
       </c>
       <c r="M21">
@@ -6423,7 +7172,7 @@
         <v>50.735999999999947</v>
       </c>
       <c r="K23">
-        <f t="shared" ref="J23:K23" si="12">K22+$K$2</f>
+        <f t="shared" ref="K23" si="12">K22+$K$2</f>
         <v>44.936</v>
       </c>
       <c r="M23">

</xml_diff>

<commit_message>
Refine FlickArrow Appearance, and fix some bugs...
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Chart示例.xlsx
+++ b/Assets/Scripts/Chart示例.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzh\Xenody-master\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8467604-B2BD-436E-9988-7B885C25EC31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4239C662-A1B4-4BAB-8D38-313CDBBB86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="planes" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="35">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -530,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA789EFB-BCA3-4FCA-98D4-565CD71AE543}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1189,7 +1189,7 @@
         <v>1</v>
       </c>
       <c r="D33">
-        <v>37.235999999999997</v>
+        <v>10000</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1220,36 +1220,36 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B35">
-        <v>36.835999999999999</v>
+        <v>37.235999999999997</v>
       </c>
       <c r="C35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>38.035999999999994</v>
+        <v>37.636000000000003</v>
       </c>
       <c r="E35">
         <v>1</v>
       </c>
       <c r="F35" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B36">
-        <v>37.235999999999997</v>
+        <v>38.035999999999994</v>
       </c>
       <c r="C36">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>37.636000000000003</v>
+        <v>38.436</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1260,36 +1260,36 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B37">
-        <v>37.636000000000003</v>
+        <v>38.835999999999991</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>38.835999999999991</v>
+        <v>39.236000000000004</v>
       </c>
       <c r="E37">
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B38">
-        <v>38.035999999999994</v>
+        <v>39.635999999999989</v>
       </c>
       <c r="C38">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>38.436</v>
+        <v>40.036000000000001</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1300,36 +1300,36 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B39">
-        <v>38.436</v>
+        <v>40.435999999999986</v>
       </c>
       <c r="C39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>39.635999999999989</v>
+        <v>40.835999999999999</v>
       </c>
       <c r="E39">
         <v>1</v>
       </c>
       <c r="F39" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B40">
-        <v>38.835999999999991</v>
+        <v>41.235999999999983</v>
       </c>
       <c r="C40">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>39.236000000000004</v>
+        <v>41.636000000000003</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1340,36 +1340,36 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B41">
-        <v>39.236000000000004</v>
+        <v>42.036000000000001</v>
       </c>
       <c r="C41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>40.435999999999986</v>
+        <v>42.436</v>
       </c>
       <c r="E41">
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B42">
-        <v>39.635999999999989</v>
+        <v>42.835999999999999</v>
       </c>
       <c r="C42">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>40.036000000000001</v>
+        <v>43.235999999999997</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1380,36 +1380,36 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B43">
-        <v>40.036000000000001</v>
+        <v>43.636000000000003</v>
       </c>
       <c r="C43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>41.235999999999983</v>
+        <v>44.036000000000001</v>
       </c>
       <c r="E43">
         <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B44">
-        <v>40.435999999999986</v>
+        <v>44.436</v>
       </c>
       <c r="C44">
         <v>0</v>
       </c>
       <c r="D44">
-        <v>40.835999999999999</v>
+        <v>44.835999999999999</v>
       </c>
       <c r="E44">
         <v>1</v>
@@ -1420,62 +1420,42 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B45">
-        <v>40.835999999999999</v>
+        <v>45.235999999999997</v>
       </c>
       <c r="C45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>42.03599999999998</v>
+        <v>45.636000000000003</v>
       </c>
       <c r="E45">
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B46">
-        <v>41.235999999999983</v>
+        <v>46.036000000000001</v>
       </c>
       <c r="C46">
         <v>0</v>
       </c>
       <c r="D46">
-        <v>41.636000000000003</v>
+        <v>46.436</v>
       </c>
       <c r="E46">
         <v>1</v>
       </c>
       <c r="F46" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>10</v>
-      </c>
-      <c r="B47">
-        <v>41.636000000000003</v>
-      </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47">
-        <v>42.835999999999977</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1487,10 +1467,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7059D0-50D6-42B0-899B-7876B4BEDB4C}">
-  <dimension ref="A1:F168"/>
+  <dimension ref="A1:F222"/>
   <sheetViews>
-    <sheetView topLeftCell="A139" workbookViewId="0">
-      <selection activeCell="H166" sqref="H166"/>
+    <sheetView topLeftCell="A190" workbookViewId="0">
+      <selection activeCell="I216" sqref="I216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3735,7 +3715,7 @@
         <v>0.8</v>
       </c>
       <c r="D160">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.2">
@@ -3743,13 +3723,13 @@
         <v>41.536000000000001</v>
       </c>
       <c r="B161">
-        <v>-0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="C161">
         <v>0.8</v>
       </c>
       <c r="D161">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.2">
@@ -3763,7 +3743,7 @@
         <v>0.8</v>
       </c>
       <c r="D162">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.2">
@@ -3771,13 +3751,13 @@
         <v>41.936</v>
       </c>
       <c r="B163">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C163">
         <v>0.8</v>
       </c>
       <c r="D163">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.2">
@@ -3791,7 +3771,7 @@
         <v>0.8</v>
       </c>
       <c r="D164">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.2">
@@ -3799,13 +3779,13 @@
         <v>42.335999999999999</v>
       </c>
       <c r="B165">
-        <v>-0.5</v>
+        <v>0.9</v>
       </c>
       <c r="C165">
         <v>0.8</v>
       </c>
       <c r="D165">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.2">
@@ -3813,13 +3793,13 @@
         <v>42.436</v>
       </c>
       <c r="B166">
-        <v>-1.5</v>
+        <v>-0.3</v>
       </c>
       <c r="C166">
         <v>0.8</v>
       </c>
       <c r="D166">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.2">
@@ -3827,13 +3807,13 @@
         <v>42.735999999999997</v>
       </c>
       <c r="B167">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C167">
         <v>0.8</v>
       </c>
       <c r="D167">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.2">
@@ -3847,6 +3827,762 @@
         <v>0.8</v>
       </c>
       <c r="D168">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>43.536000000000001</v>
+      </c>
+      <c r="B169">
+        <v>-0.3</v>
+      </c>
+      <c r="C169">
+        <v>0.8</v>
+      </c>
+      <c r="D169">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>43.636000000000003</v>
+      </c>
+      <c r="B170">
+        <v>-1.5</v>
+      </c>
+      <c r="C170">
+        <v>0.8</v>
+      </c>
+      <c r="D170">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>43.936</v>
+      </c>
+      <c r="B171">
+        <v>-0.9</v>
+      </c>
+      <c r="C171">
+        <v>0.8</v>
+      </c>
+      <c r="D171">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>44.036000000000001</v>
+      </c>
+      <c r="B172">
+        <v>0.3</v>
+      </c>
+      <c r="C172">
+        <v>0.8</v>
+      </c>
+      <c r="D172">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>44.335999999999999</v>
+      </c>
+      <c r="B173">
+        <v>-0.3</v>
+      </c>
+      <c r="C173">
+        <v>0.8</v>
+      </c>
+      <c r="D173">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>44.436</v>
+      </c>
+      <c r="B174">
+        <v>-1.5</v>
+      </c>
+      <c r="C174">
+        <v>0.8</v>
+      </c>
+      <c r="D174">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>44.636000000000003</v>
+      </c>
+      <c r="B175">
+        <v>1.2</v>
+      </c>
+      <c r="C175">
+        <v>0.8</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>44.735999999999997</v>
+      </c>
+      <c r="B176">
+        <v>-0.5</v>
+      </c>
+      <c r="C176">
+        <v>0.8</v>
+      </c>
+      <c r="D176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>45.036000000000001</v>
+      </c>
+      <c r="B177">
+        <v>-1.6</v>
+      </c>
+      <c r="C177">
+        <v>0.8</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>45.036000000000001</v>
+      </c>
+      <c r="B178">
+        <v>0</v>
+      </c>
+      <c r="C178">
+        <v>0.8</v>
+      </c>
+      <c r="D178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>45.235999999999997</v>
+      </c>
+      <c r="B179">
+        <v>0</v>
+      </c>
+      <c r="C179">
+        <v>0.8</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>46.835999999999999</v>
+      </c>
+      <c r="B180">
+        <v>1.7</v>
+      </c>
+      <c r="C180">
+        <v>0.6</v>
+      </c>
+      <c r="D180">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>46.936</v>
+      </c>
+      <c r="B181">
+        <v>0.5</v>
+      </c>
+      <c r="C181">
+        <v>0.6</v>
+      </c>
+      <c r="D181">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>47.036000000000001</v>
+      </c>
+      <c r="B182">
+        <v>1</v>
+      </c>
+      <c r="C182">
+        <v>0.6</v>
+      </c>
+      <c r="D182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>47.136000000000003</v>
+      </c>
+      <c r="B183">
+        <v>-0.2</v>
+      </c>
+      <c r="C183">
+        <v>0.6</v>
+      </c>
+      <c r="D183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>47.235999999999997</v>
+      </c>
+      <c r="B184">
+        <v>1.2</v>
+      </c>
+      <c r="C184">
+        <v>0.7</v>
+      </c>
+      <c r="D184">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>47.335999999999999</v>
+      </c>
+      <c r="B185">
+        <v>0</v>
+      </c>
+      <c r="C185">
+        <v>0.7</v>
+      </c>
+      <c r="D185">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>47.436</v>
+      </c>
+      <c r="B186">
+        <v>0.5</v>
+      </c>
+      <c r="C186">
+        <v>0.7</v>
+      </c>
+      <c r="D186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>47.536000000000001</v>
+      </c>
+      <c r="B187">
+        <v>-0.7</v>
+      </c>
+      <c r="C187">
+        <v>0.7</v>
+      </c>
+      <c r="D187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>47.636000000000003</v>
+      </c>
+      <c r="B188">
+        <v>0.7</v>
+      </c>
+      <c r="C188">
+        <v>0.8</v>
+      </c>
+      <c r="D188">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>47.735999999999997</v>
+      </c>
+      <c r="B189">
+        <v>-0.5</v>
+      </c>
+      <c r="C189">
+        <v>0.8</v>
+      </c>
+      <c r="D189">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>47.835999999999999</v>
+      </c>
+      <c r="B190">
+        <v>0</v>
+      </c>
+      <c r="C190">
+        <v>0.8</v>
+      </c>
+      <c r="D190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>47.936</v>
+      </c>
+      <c r="B191">
+        <v>-1.2</v>
+      </c>
+      <c r="C191">
+        <v>0.8</v>
+      </c>
+      <c r="D191">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>48.036000000000001</v>
+      </c>
+      <c r="B192">
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="C192">
+        <v>0.9</v>
+      </c>
+      <c r="D192">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>48.136000000000003</v>
+      </c>
+      <c r="B193">
+        <v>-1</v>
+      </c>
+      <c r="C193">
+        <v>0.9</v>
+      </c>
+      <c r="D193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>48.235999999999997</v>
+      </c>
+      <c r="B194">
+        <v>-0.5</v>
+      </c>
+      <c r="C194">
+        <v>0.9</v>
+      </c>
+      <c r="D194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>48.335999999999999</v>
+      </c>
+      <c r="B195">
+        <v>-1.5</v>
+      </c>
+      <c r="C195">
+        <v>0.9</v>
+      </c>
+      <c r="D195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>48.436</v>
+      </c>
+      <c r="B196">
+        <v>-1.5</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+      <c r="D196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>48.636000000000003</v>
+      </c>
+      <c r="B197">
+        <v>-1.5</v>
+      </c>
+      <c r="C197">
+        <v>1</v>
+      </c>
+      <c r="D197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>50.235999999999997</v>
+      </c>
+      <c r="B198">
+        <v>-1.5</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+      <c r="D198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>51.235999999999997</v>
+      </c>
+      <c r="B199">
+        <v>1.5</v>
+      </c>
+      <c r="C199">
+        <v>1</v>
+      </c>
+      <c r="D199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>51.436</v>
+      </c>
+      <c r="B200">
+        <v>-1.5</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+      <c r="D200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>51.436</v>
+      </c>
+      <c r="B201">
+        <v>0</v>
+      </c>
+      <c r="C201">
+        <v>1</v>
+      </c>
+      <c r="D201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A202">
+        <v>51.835999999999999</v>
+      </c>
+      <c r="B202">
+        <v>1.5</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+      <c r="D202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A203">
+        <v>53.436</v>
+      </c>
+      <c r="B203">
+        <v>1.5</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+      <c r="D203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A204">
+        <v>54.436</v>
+      </c>
+      <c r="B204">
+        <v>-1.5</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+      <c r="D204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A205">
+        <v>54.636000000000003</v>
+      </c>
+      <c r="B205">
+        <v>0</v>
+      </c>
+      <c r="C205">
+        <v>1</v>
+      </c>
+      <c r="D205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A206">
+        <v>54.636000000000003</v>
+      </c>
+      <c r="B206">
+        <v>1.5</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+      <c r="D206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A207">
+        <v>55.035999999999994</v>
+      </c>
+      <c r="B207">
+        <v>-1.5</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+      <c r="D207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A208">
+        <v>56.635999999999996</v>
+      </c>
+      <c r="B208">
+        <v>1.5</v>
+      </c>
+      <c r="C208">
+        <v>1</v>
+      </c>
+      <c r="D208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A209">
+        <v>58.235999999999997</v>
+      </c>
+      <c r="B209">
+        <v>-1.5</v>
+      </c>
+      <c r="C209">
+        <v>1</v>
+      </c>
+      <c r="D209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A210">
+        <v>59.436</v>
+      </c>
+      <c r="B210">
+        <v>1.5</v>
+      </c>
+      <c r="C210">
+        <v>1</v>
+      </c>
+      <c r="D210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A211">
+        <v>59.636000000000003</v>
+      </c>
+      <c r="B211">
+        <v>-1</v>
+      </c>
+      <c r="C211">
+        <v>0.8</v>
+      </c>
+      <c r="D211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A212">
+        <v>59.636000000000003</v>
+      </c>
+      <c r="B212">
+        <v>1</v>
+      </c>
+      <c r="C212">
+        <v>0.8</v>
+      </c>
+      <c r="D212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A213">
+        <v>59.736000000000004</v>
+      </c>
+      <c r="B213">
+        <v>-1</v>
+      </c>
+      <c r="C213">
+        <v>0.8</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>59.736000000000004</v>
+      </c>
+      <c r="B214">
+        <v>1</v>
+      </c>
+      <c r="C214">
+        <v>0.8</v>
+      </c>
+      <c r="D214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>59.936</v>
+      </c>
+      <c r="B215">
+        <v>-1</v>
+      </c>
+      <c r="C215">
+        <v>0.8</v>
+      </c>
+      <c r="D215">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>59.936</v>
+      </c>
+      <c r="B216">
+        <v>1</v>
+      </c>
+      <c r="C216">
+        <v>0.8</v>
+      </c>
+      <c r="D216">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>60.136000000000003</v>
+      </c>
+      <c r="B217">
+        <v>-1</v>
+      </c>
+      <c r="C217">
+        <v>0.8</v>
+      </c>
+      <c r="D217">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>60.136000000000003</v>
+      </c>
+      <c r="B218">
+        <v>1</v>
+      </c>
+      <c r="C218">
+        <v>0.8</v>
+      </c>
+      <c r="D218">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>60.335999999999999</v>
+      </c>
+      <c r="B219">
+        <v>-1</v>
+      </c>
+      <c r="C219">
+        <v>0.8</v>
+      </c>
+      <c r="D219">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>60.335999999999999</v>
+      </c>
+      <c r="B220">
+        <v>1</v>
+      </c>
+      <c r="C220">
+        <v>0.8</v>
+      </c>
+      <c r="D220">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>60.436</v>
+      </c>
+      <c r="B221">
+        <v>-1</v>
+      </c>
+      <c r="C221">
+        <v>0.8</v>
+      </c>
+      <c r="D221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>60.436</v>
+      </c>
+      <c r="B222">
+        <v>1</v>
+      </c>
+      <c r="C222">
+        <v>0.8</v>
+      </c>
+      <c r="D222">
         <v>1</v>
       </c>
     </row>
@@ -3859,10 +4595,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B2D43-E0B0-4050-83A2-AF5C6E5EE029}">
-  <dimension ref="A1:J42"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5209,6 +5945,742 @@
       </c>
       <c r="J42" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>31</v>
+      </c>
+      <c r="C43">
+        <v>48.436</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>48.636000000000003</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>2</v>
+      </c>
+      <c r="I43" t="s">
+        <v>25</v>
+      </c>
+      <c r="J43" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>32</v>
+      </c>
+      <c r="C44">
+        <v>49.436</v>
+      </c>
+      <c r="D44">
+        <v>-0.5</v>
+      </c>
+      <c r="E44">
+        <v>0.5</v>
+      </c>
+      <c r="F44">
+        <v>49.636000000000003</v>
+      </c>
+      <c r="G44">
+        <v>-0.5</v>
+      </c>
+      <c r="H44">
+        <v>0.5</v>
+      </c>
+      <c r="I44" t="s">
+        <v>25</v>
+      </c>
+      <c r="J44" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>33</v>
+      </c>
+      <c r="C45">
+        <v>49.636000000000003</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>49.835999999999999</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45" t="s">
+        <v>25</v>
+      </c>
+      <c r="J45" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>34</v>
+      </c>
+      <c r="C46">
+        <v>49.835999999999999</v>
+      </c>
+      <c r="D46">
+        <v>-2</v>
+      </c>
+      <c r="E46">
+        <v>-1</v>
+      </c>
+      <c r="F46">
+        <v>50.036000000000001</v>
+      </c>
+      <c r="G46">
+        <v>-2</v>
+      </c>
+      <c r="H46">
+        <v>-1</v>
+      </c>
+      <c r="I46" t="s">
+        <v>25</v>
+      </c>
+      <c r="J46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>35</v>
+      </c>
+      <c r="C47">
+        <v>50.036000000000001</v>
+      </c>
+      <c r="D47">
+        <v>-0.5</v>
+      </c>
+      <c r="E47">
+        <v>0.5</v>
+      </c>
+      <c r="F47">
+        <v>50.235999999999997</v>
+      </c>
+      <c r="G47">
+        <v>-0.5</v>
+      </c>
+      <c r="H47">
+        <v>0.5</v>
+      </c>
+      <c r="I47" t="s">
+        <v>25</v>
+      </c>
+      <c r="J47" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48">
+        <v>36</v>
+      </c>
+      <c r="C48">
+        <v>51.036000000000001</v>
+      </c>
+      <c r="D48">
+        <v>-0.5</v>
+      </c>
+      <c r="E48">
+        <v>0.5</v>
+      </c>
+      <c r="F48">
+        <v>51.235999999999997</v>
+      </c>
+      <c r="G48">
+        <v>-0.5</v>
+      </c>
+      <c r="H48">
+        <v>0.5</v>
+      </c>
+      <c r="I48" t="s">
+        <v>25</v>
+      </c>
+      <c r="J48" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49">
+        <v>37</v>
+      </c>
+      <c r="C49">
+        <v>51.636000000000003</v>
+      </c>
+      <c r="D49">
+        <v>-2</v>
+      </c>
+      <c r="E49">
+        <v>-1</v>
+      </c>
+      <c r="F49">
+        <v>51.835999999999999</v>
+      </c>
+      <c r="G49">
+        <v>-2</v>
+      </c>
+      <c r="H49">
+        <v>-1</v>
+      </c>
+      <c r="I49" t="s">
+        <v>25</v>
+      </c>
+      <c r="J49" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50">
+        <v>38</v>
+      </c>
+      <c r="C50">
+        <v>52.636000000000003</v>
+      </c>
+      <c r="D50">
+        <v>-0.5</v>
+      </c>
+      <c r="E50">
+        <v>0.5</v>
+      </c>
+      <c r="F50">
+        <v>52.835999999999999</v>
+      </c>
+      <c r="G50">
+        <v>-0.5</v>
+      </c>
+      <c r="H50">
+        <v>0.5</v>
+      </c>
+      <c r="I50" t="s">
+        <v>25</v>
+      </c>
+      <c r="J50" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51">
+        <v>39</v>
+      </c>
+      <c r="C51">
+        <v>52.835999999999999</v>
+      </c>
+      <c r="D51">
+        <v>-2</v>
+      </c>
+      <c r="E51">
+        <v>-1</v>
+      </c>
+      <c r="F51">
+        <v>53.036000000000001</v>
+      </c>
+      <c r="G51">
+        <v>-2</v>
+      </c>
+      <c r="H51">
+        <v>-1</v>
+      </c>
+      <c r="I51" t="s">
+        <v>25</v>
+      </c>
+      <c r="J51" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52">
+        <v>40</v>
+      </c>
+      <c r="C52">
+        <v>53.036000000000001</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>53.235999999999997</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52">
+        <v>2</v>
+      </c>
+      <c r="I52" t="s">
+        <v>25</v>
+      </c>
+      <c r="J52" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53">
+        <v>41</v>
+      </c>
+      <c r="C53">
+        <v>53.235999999999997</v>
+      </c>
+      <c r="D53">
+        <v>-0.5</v>
+      </c>
+      <c r="E53">
+        <v>0.5</v>
+      </c>
+      <c r="F53">
+        <v>53.436</v>
+      </c>
+      <c r="G53">
+        <v>-0.5</v>
+      </c>
+      <c r="H53">
+        <v>0.5</v>
+      </c>
+      <c r="I53" t="s">
+        <v>25</v>
+      </c>
+      <c r="J53" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54">
+        <v>42</v>
+      </c>
+      <c r="C54">
+        <v>54.235999999999997</v>
+      </c>
+      <c r="D54">
+        <v>-0.5</v>
+      </c>
+      <c r="E54">
+        <v>0.5</v>
+      </c>
+      <c r="F54">
+        <v>54.436</v>
+      </c>
+      <c r="G54">
+        <v>-0.5</v>
+      </c>
+      <c r="H54">
+        <v>0.5</v>
+      </c>
+      <c r="I54" t="s">
+        <v>25</v>
+      </c>
+      <c r="J54" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>1</v>
+      </c>
+      <c r="B55">
+        <v>43</v>
+      </c>
+      <c r="C55">
+        <v>54.835999999999999</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+      <c r="F55">
+        <v>55.035999999999994</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55" t="s">
+        <v>25</v>
+      </c>
+      <c r="J55" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>1</v>
+      </c>
+      <c r="B56">
+        <v>44</v>
+      </c>
+      <c r="C56">
+        <v>55.835999999999999</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+      <c r="F56">
+        <v>56.035999999999994</v>
+      </c>
+      <c r="G56">
+        <v>1</v>
+      </c>
+      <c r="H56">
+        <v>2</v>
+      </c>
+      <c r="I56" t="s">
+        <v>25</v>
+      </c>
+      <c r="J56" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>45</v>
+      </c>
+      <c r="C57">
+        <v>56.035999999999994</v>
+      </c>
+      <c r="D57">
+        <v>-2</v>
+      </c>
+      <c r="E57">
+        <v>-1</v>
+      </c>
+      <c r="F57">
+        <v>56.235999999999997</v>
+      </c>
+      <c r="G57">
+        <v>-1</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" t="s">
+        <v>25</v>
+      </c>
+      <c r="J57" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58">
+        <v>46</v>
+      </c>
+      <c r="C58">
+        <v>56.235999999999997</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+      <c r="F58">
+        <v>56.436</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58" t="s">
+        <v>25</v>
+      </c>
+      <c r="J58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59">
+        <v>47</v>
+      </c>
+      <c r="C59">
+        <v>56.436</v>
+      </c>
+      <c r="D59">
+        <v>-2</v>
+      </c>
+      <c r="E59">
+        <v>-1</v>
+      </c>
+      <c r="F59">
+        <v>56.635999999999996</v>
+      </c>
+      <c r="G59">
+        <v>-1</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59" t="s">
+        <v>25</v>
+      </c>
+      <c r="J59" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60">
+        <v>48</v>
+      </c>
+      <c r="C60">
+        <v>57.436</v>
+      </c>
+      <c r="D60">
+        <v>-1</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>57.635999999999996</v>
+      </c>
+      <c r="G60">
+        <v>-2</v>
+      </c>
+      <c r="H60">
+        <v>-1</v>
+      </c>
+      <c r="I60" t="s">
+        <v>25</v>
+      </c>
+      <c r="J60" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61">
+        <v>49</v>
+      </c>
+      <c r="C61">
+        <v>57.635999999999996</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>2</v>
+      </c>
+      <c r="F61">
+        <v>57.835999999999999</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>1</v>
+      </c>
+      <c r="I61" t="s">
+        <v>25</v>
+      </c>
+      <c r="J61" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>50</v>
+      </c>
+      <c r="C62">
+        <v>57.835999999999999</v>
+      </c>
+      <c r="D62">
+        <v>-1</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>58.035999999999994</v>
+      </c>
+      <c r="G62">
+        <v>-2</v>
+      </c>
+      <c r="H62">
+        <v>-1</v>
+      </c>
+      <c r="I62" t="s">
+        <v>25</v>
+      </c>
+      <c r="J62" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63">
+        <v>51</v>
+      </c>
+      <c r="C63">
+        <v>58.035999999999994</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>2</v>
+      </c>
+      <c r="F63">
+        <v>58.235999999999997</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63">
+        <v>1</v>
+      </c>
+      <c r="I63" t="s">
+        <v>25</v>
+      </c>
+      <c r="J63" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64">
+        <v>52</v>
+      </c>
+      <c r="C64">
+        <v>59.036000000000001</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+      <c r="E64">
+        <v>2</v>
+      </c>
+      <c r="F64">
+        <v>59.235999999999997</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64" t="s">
+        <v>25</v>
+      </c>
+      <c r="J64" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>1</v>
+      </c>
+      <c r="B65">
+        <v>53</v>
+      </c>
+      <c r="C65">
+        <v>59.235999999999997</v>
+      </c>
+      <c r="D65">
+        <v>-1</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>59.436</v>
+      </c>
+      <c r="G65">
+        <v>-2</v>
+      </c>
+      <c r="H65">
+        <v>-1</v>
+      </c>
+      <c r="I65" t="s">
+        <v>25</v>
+      </c>
+      <c r="J65" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -5629,10 +7101,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F96158-71D4-4C19-99F5-47E7932AF572}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5889,7 +7361,7 @@
         <v>0.5</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -5906,24 +7378,313 @@
         <v>0.5</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>38.436</v>
+      </c>
+      <c r="B17">
+        <v>-1.6</v>
+      </c>
+      <c r="C17">
+        <v>0.8</v>
+      </c>
+      <c r="D17">
+        <v>0.5</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>39.235999999999997</v>
+      </c>
+      <c r="B18">
+        <v>1.6</v>
+      </c>
+      <c r="C18">
+        <v>0.8</v>
+      </c>
+      <c r="D18">
+        <v>0.5</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>40.036000000000001</v>
+      </c>
+      <c r="B19">
+        <v>-1.6</v>
+      </c>
+      <c r="C19">
+        <v>0.8</v>
+      </c>
+      <c r="D19">
+        <v>0.5</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>40.835999999999999</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>1</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>1</v>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>49.036000000000001</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>49.036000000000001</v>
+      </c>
+      <c r="B22">
+        <v>-1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>0.75</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>50.636000000000003</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0.5</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>50.636000000000003</v>
+      </c>
+      <c r="B24">
+        <v>-1</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <v>0.75</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>52.235999999999997</v>
+      </c>
+      <c r="B25">
+        <v>-1</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0.5</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>52.235999999999997</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0.25</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>53.835999999999999</v>
+      </c>
+      <c r="B27">
+        <v>-1</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27">
+        <v>0.5</v>
+      </c>
+      <c r="E27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>53.835999999999999</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>0.25</v>
+      </c>
+      <c r="E28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>55.436</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>0.5</v>
+      </c>
+      <c r="E29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>55.436</v>
+      </c>
+      <c r="B30">
+        <v>1.5</v>
+      </c>
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30">
+        <v>0.25</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>57.035999999999994</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0.5</v>
+      </c>
+      <c r="E31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>57.035999999999994</v>
+      </c>
+      <c r="B32">
+        <v>-1.5</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>0.75</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>58.536000000000001</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0.5</v>
+      </c>
+      <c r="E33">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>58.536000000000001</v>
+      </c>
+      <c r="B34">
+        <v>1.5</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>0.25</v>
+      </c>
+      <c r="E34">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -5934,10 +7695,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192095B2-1BEA-4365-B4DE-88EEBB6E4423}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28:I28"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6616,7 +8377,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B22">
         <v>19</v>
@@ -6634,13 +8395,13 @@
         <v>1.5</v>
       </c>
       <c r="G22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="s">
         <v>23</v>
@@ -6648,7 +8409,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B23">
         <v>20</v>
@@ -6663,16 +8424,16 @@
         <v>42.536000000000001</v>
       </c>
       <c r="F23">
-        <v>-1.5</v>
+        <v>-0.3</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>-1</v>
+        <v>-0.8</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="s">
         <v>23</v>
@@ -6680,7 +8441,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B24">
         <v>21</v>
@@ -6692,22 +8453,758 @@
         <v>42.835999999999999</v>
       </c>
       <c r="E24">
-        <v>42.936</v>
+        <v>43.036000000000001</v>
       </c>
       <c r="F24">
         <v>1.5</v>
       </c>
       <c r="G24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>21</v>
+      </c>
+      <c r="C25">
+        <v>42.636000000000003</v>
+      </c>
+      <c r="D25">
+        <v>43.036000000000001</v>
+      </c>
+      <c r="E25">
+        <v>43.235999999999997</v>
+      </c>
+      <c r="F25">
+        <v>0.5</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>1.5</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>22</v>
+      </c>
+      <c r="C26">
+        <v>43.436</v>
+      </c>
+      <c r="D26">
+        <v>43.636000000000003</v>
+      </c>
+      <c r="E26">
+        <v>43.735999999999997</v>
+      </c>
+      <c r="F26">
+        <v>-1.5</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>-1</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>23</v>
+      </c>
+      <c r="C27">
+        <v>43.835999999999999</v>
+      </c>
+      <c r="D27">
+        <v>44.036000000000001</v>
+      </c>
+      <c r="E27">
+        <v>44.136000000000003</v>
+      </c>
+      <c r="F27">
+        <v>0.3</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0.8</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>24</v>
+      </c>
+      <c r="C28">
+        <v>44.235999999999997</v>
+      </c>
+      <c r="D28">
+        <v>44.436</v>
+      </c>
+      <c r="E28">
+        <v>44.536000000000001</v>
+      </c>
+      <c r="F28">
+        <v>-1.5</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>-1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>25</v>
+      </c>
+      <c r="C29">
+        <v>45.235999999999997</v>
+      </c>
+      <c r="D29">
+        <v>45.436</v>
+      </c>
+      <c r="E29">
+        <v>45.835999999999999</v>
+      </c>
+      <c r="F29">
+        <v>1.6</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>-1.6</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>25</v>
+      </c>
+      <c r="C30">
+        <v>45.835999999999999</v>
+      </c>
+      <c r="D30">
+        <v>45.835999999999999</v>
+      </c>
+      <c r="E30">
+        <v>46.235999999999997</v>
+      </c>
+      <c r="F30">
+        <v>-1.6</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+      <c r="J30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>25</v>
+      </c>
+      <c r="C31">
+        <v>46.235999999999997</v>
+      </c>
+      <c r="D31">
+        <v>46.235999999999997</v>
+      </c>
+      <c r="E31">
+        <v>46.636000000000003</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>1.6</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>26</v>
+      </c>
+      <c r="C32">
+        <v>45.835999999999999</v>
+      </c>
+      <c r="D32">
+        <v>45.835999999999999</v>
+      </c>
+      <c r="E32">
+        <v>46.235999999999997</v>
+      </c>
+      <c r="F32">
+        <v>-1.5</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>26</v>
+      </c>
+      <c r="C33">
+        <v>46.235999999999997</v>
+      </c>
+      <c r="D33">
+        <v>46.235999999999997</v>
+      </c>
+      <c r="E33">
+        <v>46.636000000000003</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>1.5</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>27</v>
+      </c>
+      <c r="C34">
+        <v>48.735999999999997</v>
+      </c>
+      <c r="D34">
+        <v>49.036000000000001</v>
+      </c>
+      <c r="E34">
+        <v>49.235999999999997</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>-0.2</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>27</v>
+      </c>
+      <c r="C35">
+        <v>48.735999999999997</v>
+      </c>
+      <c r="D35">
+        <v>49.235999999999997</v>
+      </c>
+      <c r="E35">
+        <v>49.436</v>
+      </c>
+      <c r="F35">
+        <v>-0.2</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>-1.5</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>3</v>
+      </c>
+      <c r="B36">
+        <v>28</v>
+      </c>
+      <c r="C36">
+        <v>50.335999999999999</v>
+      </c>
+      <c r="D36">
+        <v>50.636000000000003</v>
+      </c>
+      <c r="E36">
+        <v>50.835999999999999</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>-0.2</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>28</v>
+      </c>
+      <c r="C37">
+        <v>50.335999999999999</v>
+      </c>
+      <c r="D37">
+        <v>50.835999999999999</v>
+      </c>
+      <c r="E37">
+        <v>51.036000000000001</v>
+      </c>
+      <c r="F37">
+        <v>-0.2</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
+        <v>-1.5</v>
+      </c>
+      <c r="I37">
+        <v>0</v>
+      </c>
+      <c r="J37" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38">
+        <v>29</v>
+      </c>
+      <c r="C38">
+        <v>51.936</v>
+      </c>
+      <c r="D38">
+        <v>52.235999999999997</v>
+      </c>
+      <c r="E38">
+        <v>52.436</v>
+      </c>
+      <c r="F38">
+        <v>-1</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>0.2</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="J38" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39">
+        <v>29</v>
+      </c>
+      <c r="C39">
+        <v>51.936</v>
+      </c>
+      <c r="D39">
+        <v>52.436</v>
+      </c>
+      <c r="E39">
+        <v>52.636000000000003</v>
+      </c>
+      <c r="F39">
+        <v>0.2</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>1.5</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>30</v>
+      </c>
+      <c r="C40">
+        <v>53.536000000000001</v>
+      </c>
+      <c r="D40">
+        <v>53.835999999999999</v>
+      </c>
+      <c r="E40">
+        <v>54.036000000000001</v>
+      </c>
+      <c r="F40">
+        <v>-1</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>0.2</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>30</v>
+      </c>
+      <c r="C41">
+        <v>53.536000000000001</v>
+      </c>
+      <c r="D41">
+        <v>54.036000000000001</v>
+      </c>
+      <c r="E41">
+        <v>54.235999999999997</v>
+      </c>
+      <c r="F41">
+        <v>0.2</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
+        <v>1.5</v>
+      </c>
+      <c r="I41">
+        <v>0</v>
+      </c>
+      <c r="J41" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>31</v>
+      </c>
+      <c r="C42">
+        <v>55.135999999999996</v>
+      </c>
+      <c r="D42">
+        <v>55.436</v>
+      </c>
+      <c r="E42">
+        <v>55.635999999999996</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>-1.5</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>31</v>
+      </c>
+      <c r="C43">
+        <v>55.135999999999996</v>
+      </c>
+      <c r="D43">
+        <v>55.635999999999996</v>
+      </c>
+      <c r="E43">
+        <v>55.835999999999999</v>
+      </c>
+      <c r="F43">
+        <v>-1.5</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="J43" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>32</v>
+      </c>
+      <c r="C44">
+        <v>56.735999999999997</v>
+      </c>
+      <c r="D44">
+        <v>57.035999999999994</v>
+      </c>
+      <c r="E44">
+        <v>57.235999999999997</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>1.5</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>3</v>
+      </c>
+      <c r="B45">
+        <v>32</v>
+      </c>
+      <c r="C45">
+        <v>56.735999999999997</v>
+      </c>
+      <c r="D45">
+        <v>57.235999999999997</v>
+      </c>
+      <c r="E45">
+        <v>57.436</v>
+      </c>
+      <c r="F45">
+        <v>1.5</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="J45" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>3</v>
+      </c>
+      <c r="B46">
+        <v>33</v>
+      </c>
+      <c r="C46">
+        <v>58.335999999999999</v>
+      </c>
+      <c r="D46">
+        <v>58.636000000000003</v>
+      </c>
+      <c r="E46">
+        <v>58.835999999999999</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>-1.5</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>33</v>
+      </c>
+      <c r="C47">
+        <v>58.335999999999999</v>
+      </c>
+      <c r="D47">
+        <v>58.835999999999999</v>
+      </c>
+      <c r="E47">
+        <v>59.036000000000001</v>
+      </c>
+      <c r="F47">
+        <v>-1.5</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -6722,7 +9219,7 @@
   <dimension ref="A1:N83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="M4" sqref="M4:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6787,7 +9284,7 @@
         <v>3.6360000000000001</v>
       </c>
       <c r="M4">
-        <v>29.236000000000001</v>
+        <v>46.835999999999999</v>
       </c>
       <c r="N4">
         <v>3.2360000000000002</v>
@@ -6811,7 +9308,7 @@
         <v>3.8360000000000003</v>
       </c>
       <c r="M5">
-        <v>29.335999999999999</v>
+        <v>46.936</v>
       </c>
       <c r="N5" s="1">
         <f>N4+$N$2</f>
@@ -6835,7 +9332,7 @@
         <v>4.0360000000000005</v>
       </c>
       <c r="M6">
-        <v>29.436</v>
+        <v>47.036000000000001</v>
       </c>
       <c r="N6" s="1">
         <f t="shared" ref="N6:N10" si="3">N5+$N$2</f>
@@ -6860,7 +9357,7 @@
         <v>4.2360000000000007</v>
       </c>
       <c r="M7">
-        <v>29.536000000000001</v>
+        <v>47.136000000000003</v>
       </c>
       <c r="N7" s="1">
         <f t="shared" si="3"/>
@@ -6884,7 +9381,7 @@
         <v>4.4360000000000008</v>
       </c>
       <c r="M8">
-        <v>29.635999999999999</v>
+        <v>47.235999999999997</v>
       </c>
       <c r="N8" s="1">
         <f t="shared" si="3"/>
@@ -6909,7 +9406,7 @@
         <v>4.636000000000001</v>
       </c>
       <c r="M9">
-        <v>29.736000000000001</v>
+        <v>47.335999999999999</v>
       </c>
       <c r="N9" s="1">
         <f t="shared" si="3"/>
@@ -6933,7 +9430,7 @@
         <v>4.8360000000000012</v>
       </c>
       <c r="M10">
-        <v>29.835999999999999</v>
+        <v>47.436</v>
       </c>
       <c r="N10" s="1">
         <f t="shared" si="3"/>
@@ -6958,7 +9455,7 @@
         <v>5.0360000000000014</v>
       </c>
       <c r="M11">
-        <v>29.936</v>
+        <v>47.536000000000001</v>
       </c>
       <c r="N11" s="1"/>
     </row>
@@ -6979,7 +9476,7 @@
         <v>5.2360000000000015</v>
       </c>
       <c r="M12">
-        <v>30.036000000000001</v>
+        <v>47.636000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
@@ -7000,7 +9497,7 @@
         <v>5.4360000000000017</v>
       </c>
       <c r="M13">
-        <v>30.135999999999999</v>
+        <v>47.735999999999997</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -7016,7 +9513,7 @@
         <v>40.536000000000001</v>
       </c>
       <c r="M14">
-        <v>30.236000000000001</v>
+        <v>47.835999999999999</v>
       </c>
       <c r="N14">
         <v>21.635999999999999</v>
@@ -7036,7 +9533,7 @@
         <v>40.936</v>
       </c>
       <c r="M15">
-        <v>30.335999999999999</v>
+        <v>47.936</v>
       </c>
       <c r="N15">
         <f>N14+$N$2</f>
@@ -7056,7 +9553,7 @@
         <v>41.536000000000001</v>
       </c>
       <c r="M16">
-        <v>30.436</v>
+        <v>48.036000000000001</v>
       </c>
       <c r="N16">
         <f>N15+$N$2</f>
@@ -7077,7 +9574,7 @@
         <v>41.936</v>
       </c>
       <c r="M17">
-        <v>30.536000000000001</v>
+        <v>48.136000000000003</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
@@ -7093,7 +9590,7 @@
         <v>42.536000000000001</v>
       </c>
       <c r="M18">
-        <v>30.635999999999999</v>
+        <v>48.235999999999997</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
@@ -7110,7 +9607,7 @@
         <v>42.936</v>
       </c>
       <c r="M19">
-        <v>30.736000000000001</v>
+        <v>48.335999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
@@ -7126,7 +9623,7 @@
         <v>43.536000000000001</v>
       </c>
       <c r="M20">
-        <v>30.835999999999999</v>
+        <v>48.436</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -7143,7 +9640,7 @@
         <v>43.936</v>
       </c>
       <c r="M21">
-        <v>30.936</v>
+        <v>48.536000000000001</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
@@ -7159,7 +9656,7 @@
         <v>44.536000000000001</v>
       </c>
       <c r="M22">
-        <v>31.036000000000001</v>
+        <v>48.636000000000003</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
@@ -7176,7 +9673,7 @@
         <v>44.936</v>
       </c>
       <c r="M23">
-        <v>31.135999999999999</v>
+        <v>48.735999999999997</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
@@ -7185,7 +9682,7 @@
         <v>16.836000000000002</v>
       </c>
       <c r="M24">
-        <v>31.236000000000001</v>
+        <v>48.835999999999999</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -7194,7 +9691,7 @@
         <v>17.236000000000001</v>
       </c>
       <c r="M25">
-        <v>31.335999999999999</v>
+        <v>48.936</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -7203,12 +9700,12 @@
         <v>17.635999999999999</v>
       </c>
       <c r="M26">
-        <v>31.436</v>
+        <v>49.036000000000001</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="M27">
-        <v>31.536000000000001</v>
+        <v>49.136000000000003</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -7216,7 +9713,7 @@
         <v>19.635999999999999</v>
       </c>
       <c r="M28">
-        <v>31.6359999999999</v>
+        <v>49.235999999999997</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -7224,7 +9721,7 @@
         <v>20.036000000000001</v>
       </c>
       <c r="M29">
-        <v>31.736000000000001</v>
+        <v>49.335999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -7232,7 +9729,7 @@
         <v>20.436</v>
       </c>
       <c r="M30">
-        <v>31.835999999999899</v>
+        <v>49.436</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -7240,7 +9737,7 @@
         <v>20.835999999999999</v>
       </c>
       <c r="M31">
-        <v>31.9359999999999</v>
+        <v>49.536000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -7248,7 +9745,7 @@
         <v>21.236000000000001</v>
       </c>
       <c r="M32">
-        <v>32.035999999999902</v>
+        <v>49.636000000000003</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -7256,7 +9753,7 @@
         <v>21.635999999999999</v>
       </c>
       <c r="M33">
-        <v>32.135999999999903</v>
+        <v>49.735999999999997</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -7264,72 +9761,48 @@
         <v>22.036000000000001</v>
       </c>
       <c r="M34">
-        <v>32.235999999999898</v>
+        <v>49.835999999999999</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>22.436</v>
       </c>
-      <c r="M35">
-        <v>32.335999999999899</v>
-      </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>22.835999999999999</v>
       </c>
-      <c r="M36">
-        <v>32.4359999999999</v>
-      </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>23.236000000000001</v>
       </c>
-      <c r="M37">
-        <v>32.535999999999902</v>
-      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>23.635999999999999</v>
       </c>
-      <c r="M38">
-        <v>32.635999999999903</v>
-      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>24.036000000000001</v>
       </c>
-      <c r="M39">
-        <v>32.735999999999898</v>
-      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>24.436</v>
       </c>
-      <c r="M40">
-        <v>32.835999999999899</v>
-      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>24.835999999999999</v>
       </c>
-      <c r="M41">
-        <v>32.9359999999999</v>
-      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>25.236000000000001</v>
       </c>
-      <c r="M42">
-        <v>33.035999999999902</v>
-      </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43">
@@ -7399,43 +9872,43 @@
     <row r="77" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M77">
         <f>M4+0.1</f>
-        <v>29.336000000000002</v>
+        <v>46.936</v>
       </c>
     </row>
     <row r="78" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M78">
         <f t="shared" ref="M78:M83" si="13">M77+0.1</f>
-        <v>29.436000000000003</v>
+        <v>47.036000000000001</v>
       </c>
     </row>
     <row r="79" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M79">
         <f t="shared" si="13"/>
-        <v>29.536000000000005</v>
+        <v>47.136000000000003</v>
       </c>
     </row>
     <row r="80" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M80">
         <f t="shared" si="13"/>
-        <v>29.636000000000006</v>
+        <v>47.236000000000004</v>
       </c>
     </row>
     <row r="81" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M81">
         <f t="shared" si="13"/>
-        <v>29.736000000000008</v>
+        <v>47.336000000000006</v>
       </c>
     </row>
     <row r="82" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M82">
         <f t="shared" si="13"/>
-        <v>29.836000000000009</v>
+        <v>47.436000000000007</v>
       </c>
     </row>
     <row r="83" spans="13:13" x14ac:dyDescent="0.2">
       <c r="M83">
         <f t="shared" si="13"/>
-        <v>29.936000000000011</v>
+        <v>47.536000000000008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change StarHead Prefab, Add StarSound...
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Chart示例.xlsx
+++ b/Assets/Scripts/Chart示例.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzh\Xenody-master\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4239C662-A1B4-4BAB-8D38-313CDBBB86D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A13D292-219B-4F15-8F9F-29F0303FFC82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="planes" sheetId="1" r:id="rId1"/>
@@ -1469,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7059D0-50D6-42B0-899B-7876B4BEDB4C}">
   <dimension ref="A1:F222"/>
   <sheetViews>
-    <sheetView topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="I216" sqref="I216"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2309,7 +2309,7 @@
         <v>21.898</v>
       </c>
       <c r="B60">
-        <v>-0.5</v>
+        <v>-0.7</v>
       </c>
       <c r="C60">
         <v>0.6</v>
@@ -2337,7 +2337,7 @@
         <v>22.036000000000001</v>
       </c>
       <c r="B62">
-        <v>-0.6</v>
+        <v>-1</v>
       </c>
       <c r="C62">
         <v>0.6</v>
@@ -4597,8 +4597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B2D43-E0B0-4050-83A2-AF5C6E5EE029}">
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5205,10 +5205,10 @@
         <v>-1</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="J19" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -5333,10 +5333,10 @@
         <v>1.6</v>
       </c>
       <c r="I23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="J23" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -6692,10 +6692,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C76DC57-EF49-44CE-8A21-D4353938F627}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6869,39 +6869,39 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>11.835999999999997</v>
+      <c r="A13" s="1">
+        <v>9.6859999999999999</v>
       </c>
       <c r="B13">
-        <v>1.3</v>
+        <v>0.8</v>
       </c>
       <c r="C13">
         <v>0.6</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>11.885999999999999</v>
+      <c r="A14" s="1">
+        <v>9.7360000000000007</v>
       </c>
       <c r="B14">
-        <v>1.7</v>
+        <v>1.2</v>
       </c>
       <c r="C14">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>15.035999999999985</v>
+      <c r="A15" s="1">
+        <v>9.6859999999999999</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>-0.8</v>
       </c>
       <c r="C15">
         <v>0.6</v>
@@ -6911,14 +6911,14 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>15.085999999999986</v>
+      <c r="A16" s="1">
+        <v>9.7360000000000007</v>
       </c>
       <c r="B16">
-        <v>-0.4</v>
+        <v>-1.2</v>
       </c>
       <c r="C16">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -6926,38 +6926,38 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>15.135999999999987</v>
+        <v>11.835999999999997</v>
       </c>
       <c r="B17">
-        <v>-0.8</v>
+        <v>1.3</v>
       </c>
       <c r="C17">
         <v>0.6</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>15.185999999999988</v>
+        <v>11.885999999999999</v>
       </c>
       <c r="B18">
-        <v>-1.2</v>
+        <v>1.7</v>
       </c>
       <c r="C18">
         <v>0.6</v>
       </c>
       <c r="D18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>15.235999999999988</v>
+        <v>15.035999999999985</v>
       </c>
       <c r="B19">
-        <v>-1.6</v>
+        <v>0</v>
       </c>
       <c r="C19">
         <v>0.6</v>
@@ -6968,69 +6968,69 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>18.936000000000025</v>
+        <v>15.085999999999986</v>
       </c>
       <c r="B20">
-        <v>1.5</v>
+        <v>-0.4</v>
       </c>
       <c r="C20">
         <v>0.6</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>18.986000000000001</v>
+        <v>15.135999999999987</v>
       </c>
       <c r="B21">
-        <v>1.1000000000000001</v>
+        <v>-0.8</v>
       </c>
       <c r="C21">
         <v>0.6</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>19.036000000000026</v>
+        <v>15.185999999999988</v>
       </c>
       <c r="B22">
-        <v>0.7</v>
+        <v>-1.2</v>
       </c>
       <c r="C22">
         <v>0.6</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>33.636000000000003</v>
+        <v>15.235999999999988</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>-1.6</v>
       </c>
       <c r="C23">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>33.735999999999997</v>
+        <v>18.936000000000025</v>
       </c>
       <c r="B24">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -7038,13 +7038,13 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>33.835999999999999</v>
+        <v>18.986000000000001</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D25">
         <v>1</v>
@@ -7052,13 +7052,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>38.235999999999997</v>
+        <v>19.036000000000026</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C26">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="D26">
         <v>1</v>
@@ -7066,13 +7066,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>38.335999999999999</v>
+        <v>33.636000000000003</v>
       </c>
       <c r="B27">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C27">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -7080,16 +7080,142 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
+        <v>33.735999999999997</v>
+      </c>
+      <c r="B28">
+        <v>0.5</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>33.835999999999999</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>38.235999999999997</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+      <c r="C30">
+        <v>0.8</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>38.335999999999999</v>
+      </c>
+      <c r="B31">
+        <v>0.5</v>
+      </c>
+      <c r="C31">
+        <v>0.8</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>38.436</v>
       </c>
-      <c r="B28">
-        <v>1</v>
-      </c>
-      <c r="C28">
-        <v>0.8</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32">
+        <v>0.8</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>60.836000000000006</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>1.5</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>60.886000000000003</v>
+      </c>
+      <c r="B34">
+        <v>0.8</v>
+      </c>
+      <c r="C34">
+        <v>0.6</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>60.936000000000007</v>
+      </c>
+      <c r="B35">
+        <v>1.2</v>
+      </c>
+      <c r="C35">
+        <v>0.4</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>60.886000000000003</v>
+      </c>
+      <c r="B36">
+        <v>-0.8</v>
+      </c>
+      <c r="C36">
+        <v>0.6</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>60.936000000000007</v>
+      </c>
+      <c r="B37">
+        <v>-1.2</v>
+      </c>
+      <c r="C37">
+        <v>0.4</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -7103,8 +7229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F96158-71D4-4C19-99F5-47E7932AF572}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -7460,7 +7586,7 @@
         <v>1</v>
       </c>
       <c r="D21">
-        <v>0.5</v>
+        <v>0.75</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -7528,7 +7654,7 @@
         <v>1</v>
       </c>
       <c r="D25">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="E25">
         <v>3</v>

</xml_diff>

<commit_message>
Write Chart and nearly done!
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Chart示例.xlsx
+++ b/Assets/Scripts/Chart示例.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lzh\Xenody-master\Assets\Scripts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Xenody-master\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA2CCA2-866A-4C26-9D7E-83C8F9AE77A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9A0A12-C613-45AE-819E-5EF56BCEC4CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="34">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -530,10 +530,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA789EFB-BCA3-4FCA-98D4-565CD71AE543}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:F167"/>
+  <dimension ref="A1:F197"/>
   <sheetViews>
-    <sheetView topLeftCell="A134" workbookViewId="0">
-      <selection activeCell="E171" sqref="E171"/>
+    <sheetView topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="D194" sqref="D194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3729,7 +3729,7 @@
         <v>0</v>
       </c>
       <c r="D160">
-        <v>10000</v>
+        <v>187.83600000000001</v>
       </c>
       <c r="E160">
         <v>0</v>
@@ -3869,12 +3869,612 @@
         <v>1</v>
       </c>
       <c r="D167">
+        <v>187.83600000000001</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="F167" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>17</v>
+      </c>
+      <c r="B168">
+        <v>187.83600000000001</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+      <c r="D168">
+        <v>188.036</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
+      </c>
+      <c r="F168" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>1</v>
+      </c>
+      <c r="B169">
+        <v>187.83600000000001</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+      <c r="D169">
+        <v>188.036</v>
+      </c>
+      <c r="E169">
+        <v>1</v>
+      </c>
+      <c r="F169" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>17</v>
+      </c>
+      <c r="B170">
+        <v>188.036</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+      <c r="D170">
+        <v>188.23599999999999</v>
+      </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
+      <c r="F170" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>1</v>
+      </c>
+      <c r="B171">
+        <v>188.036</v>
+      </c>
+      <c r="C171">
+        <v>1</v>
+      </c>
+      <c r="D171">
+        <v>188.23599999999999</v>
+      </c>
+      <c r="E171">
+        <v>0</v>
+      </c>
+      <c r="F171" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>17</v>
+      </c>
+      <c r="B172">
+        <v>188.23599999999999</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+      <c r="D172">
+        <v>188.43600000000001</v>
+      </c>
+      <c r="E172">
+        <v>0</v>
+      </c>
+      <c r="F172" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>1</v>
+      </c>
+      <c r="B173">
+        <v>188.23599999999999</v>
+      </c>
+      <c r="C173">
+        <v>0</v>
+      </c>
+      <c r="D173">
+        <v>188.43600000000001</v>
+      </c>
+      <c r="E173">
+        <v>0</v>
+      </c>
+      <c r="F173" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>19</v>
+      </c>
+      <c r="B174">
+        <v>188.23599999999999</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+      <c r="D174">
+        <v>188.43600000000001</v>
+      </c>
+      <c r="E174">
+        <v>1</v>
+      </c>
+      <c r="F174" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>17</v>
+      </c>
+      <c r="B175">
+        <v>188.43600000000001</v>
+      </c>
+      <c r="C175">
+        <v>0</v>
+      </c>
+      <c r="D175">
+        <v>188.63600000000002</v>
+      </c>
+      <c r="E175">
+        <v>0</v>
+      </c>
+      <c r="F175" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>19</v>
+      </c>
+      <c r="B176">
+        <v>188.43600000000001</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+      <c r="D176">
+        <v>188.63600000000002</v>
+      </c>
+      <c r="E176">
+        <v>0.5</v>
+      </c>
+      <c r="F176" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>17</v>
+      </c>
+      <c r="B177">
+        <v>188.63600000000002</v>
+      </c>
+      <c r="C177">
+        <v>0</v>
+      </c>
+      <c r="D177">
+        <v>188.83600000000001</v>
+      </c>
+      <c r="E177">
+        <v>0.5</v>
+      </c>
+      <c r="F177" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>19</v>
+      </c>
+      <c r="B178">
+        <v>188.63600000000002</v>
+      </c>
+      <c r="C178">
+        <v>0.5</v>
+      </c>
+      <c r="D178">
+        <v>188.83600000000001</v>
+      </c>
+      <c r="E178">
+        <v>0.5</v>
+      </c>
+      <c r="F178" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>17</v>
+      </c>
+      <c r="B179">
+        <v>188.83600000000001</v>
+      </c>
+      <c r="C179">
+        <v>0.5</v>
+      </c>
+      <c r="D179">
+        <v>189.23599999999999</v>
+      </c>
+      <c r="E179">
+        <v>0</v>
+      </c>
+      <c r="F179" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>19</v>
+      </c>
+      <c r="B180">
+        <v>188.83600000000001</v>
+      </c>
+      <c r="C180">
+        <v>0.5</v>
+      </c>
+      <c r="D180">
+        <v>189.036</v>
+      </c>
+      <c r="E180">
+        <v>1.3</v>
+      </c>
+      <c r="F180" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>19</v>
+      </c>
+      <c r="B181">
+        <v>189.036</v>
+      </c>
+      <c r="C181">
+        <v>1.3</v>
+      </c>
+      <c r="D181">
+        <v>189.23599999999999</v>
+      </c>
+      <c r="E181">
+        <v>1</v>
+      </c>
+      <c r="F181" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>17</v>
+      </c>
+      <c r="B182">
+        <v>189.23599999999999</v>
+      </c>
+      <c r="C182">
+        <v>0</v>
+      </c>
+      <c r="D182">
+        <v>194.83600000000001</v>
+      </c>
+      <c r="E182">
+        <v>0</v>
+      </c>
+      <c r="F182" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>19</v>
+      </c>
+      <c r="B183">
+        <v>189.23599999999999</v>
+      </c>
+      <c r="C183">
+        <v>1</v>
+      </c>
+      <c r="D183">
+        <v>194.83600000000001</v>
+      </c>
+      <c r="E183">
+        <v>1</v>
+      </c>
+      <c r="F183" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>17</v>
+      </c>
+      <c r="B184">
+        <v>194.83600000000001</v>
+      </c>
+      <c r="C184">
+        <v>0</v>
+      </c>
+      <c r="D184">
+        <v>195.136</v>
+      </c>
+      <c r="E184">
+        <v>1</v>
+      </c>
+      <c r="F184" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>19</v>
+      </c>
+      <c r="B185">
+        <v>194.83600000000001</v>
+      </c>
+      <c r="C185">
+        <v>1</v>
+      </c>
+      <c r="D185">
+        <v>195.136</v>
+      </c>
+      <c r="E185">
+        <v>0</v>
+      </c>
+      <c r="F185" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>17</v>
+      </c>
+      <c r="B186">
+        <v>195.136</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+      <c r="D186">
+        <v>195.43600000000001</v>
+      </c>
+      <c r="E186">
+        <v>0</v>
+      </c>
+      <c r="F186" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>19</v>
+      </c>
+      <c r="B187">
+        <v>195.136</v>
+      </c>
+      <c r="C187">
+        <v>0</v>
+      </c>
+      <c r="D187">
+        <v>195.43600000000001</v>
+      </c>
+      <c r="E187">
+        <v>1</v>
+      </c>
+      <c r="F187" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>17</v>
+      </c>
+      <c r="B188">
+        <v>195.43600000000001</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+      <c r="D188">
+        <v>195.636</v>
+      </c>
+      <c r="E188">
+        <v>0</v>
+      </c>
+      <c r="F188" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>19</v>
+      </c>
+      <c r="B189">
+        <v>195.43600000000001</v>
+      </c>
+      <c r="C189">
+        <v>1</v>
+      </c>
+      <c r="D189">
+        <v>195.636</v>
+      </c>
+      <c r="E189">
+        <v>1</v>
+      </c>
+      <c r="F189" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>17</v>
+      </c>
+      <c r="B190">
+        <v>195.636</v>
+      </c>
+      <c r="C190">
+        <v>0</v>
+      </c>
+      <c r="D190">
+        <v>195.93600000000001</v>
+      </c>
+      <c r="E190">
+        <v>1</v>
+      </c>
+      <c r="F190" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>19</v>
+      </c>
+      <c r="B191">
+        <v>195.636</v>
+      </c>
+      <c r="C191">
+        <v>1</v>
+      </c>
+      <c r="D191">
+        <v>195.93600000000001</v>
+      </c>
+      <c r="E191">
+        <v>0</v>
+      </c>
+      <c r="F191" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>17</v>
+      </c>
+      <c r="B192">
+        <v>195.93600000000001</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+      <c r="D192">
+        <v>196.23599999999999</v>
+      </c>
+      <c r="E192">
+        <v>0</v>
+      </c>
+      <c r="F192" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>19</v>
+      </c>
+      <c r="B193">
+        <v>195.93600000000001</v>
+      </c>
+      <c r="C193">
+        <v>0</v>
+      </c>
+      <c r="D193">
+        <v>196.23599999999999</v>
+      </c>
+      <c r="E193">
+        <v>1</v>
+      </c>
+      <c r="F193" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>17</v>
+      </c>
+      <c r="B194">
+        <v>196.23599999999999</v>
+      </c>
+      <c r="C194">
+        <v>0</v>
+      </c>
+      <c r="D194">
+        <v>196.43600000000001</v>
+      </c>
+      <c r="E194">
+        <v>1</v>
+      </c>
+      <c r="F194" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>19</v>
+      </c>
+      <c r="B195">
+        <v>196.23599999999999</v>
+      </c>
+      <c r="C195">
+        <v>1</v>
+      </c>
+      <c r="D195">
+        <v>196.43600000000001</v>
+      </c>
+      <c r="E195">
+        <v>0</v>
+      </c>
+      <c r="F195" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>17</v>
+      </c>
+      <c r="B196">
+        <v>196.43600000000001</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+      <c r="D196">
         <v>10000</v>
       </c>
-      <c r="E167">
-        <v>1</v>
-      </c>
-      <c r="F167" t="s">
+      <c r="E196">
+        <v>1</v>
+      </c>
+      <c r="F196" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>19</v>
+      </c>
+      <c r="B197">
+        <v>196.43600000000001</v>
+      </c>
+      <c r="C197">
+        <v>0</v>
+      </c>
+      <c r="D197">
+        <v>10000</v>
+      </c>
+      <c r="E197">
+        <v>0</v>
+      </c>
+      <c r="F197" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3888,10 +4488,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7059D0-50D6-42B0-899B-7876B4BEDB4C}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D711"/>
+  <dimension ref="A1:D826"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A677" workbookViewId="0">
-      <selection activeCell="I704" sqref="I704"/>
+    <sheetView tabSelected="1" topLeftCell="A791" workbookViewId="0">
+      <selection activeCell="H821" sqref="H821"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -13848,6 +14448,1616 @@
       </c>
       <c r="D711">
         <v>17</v>
+      </c>
+    </row>
+    <row r="712" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A712">
+        <v>176.83600000000001</v>
+      </c>
+      <c r="B712">
+        <v>1.5</v>
+      </c>
+      <c r="C712">
+        <v>0.6</v>
+      </c>
+      <c r="D712">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="713" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A713">
+        <v>176.9</v>
+      </c>
+      <c r="B713">
+        <v>-0.3</v>
+      </c>
+      <c r="C713">
+        <v>0.6</v>
+      </c>
+      <c r="D713">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="714" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A714">
+        <v>176.96700000000001</v>
+      </c>
+      <c r="B714">
+        <v>0.7</v>
+      </c>
+      <c r="C714">
+        <v>0.6</v>
+      </c>
+      <c r="D714">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="715" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A715">
+        <v>177.036</v>
+      </c>
+      <c r="B715">
+        <v>-1.2</v>
+      </c>
+      <c r="C715">
+        <v>0.6</v>
+      </c>
+      <c r="D715">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="716" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A716">
+        <v>177.136</v>
+      </c>
+      <c r="B716">
+        <v>0</v>
+      </c>
+      <c r="C716">
+        <v>0.6</v>
+      </c>
+      <c r="D716">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="717" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A717">
+        <v>177.536</v>
+      </c>
+      <c r="B717">
+        <v>1.5</v>
+      </c>
+      <c r="C717">
+        <v>0.7</v>
+      </c>
+      <c r="D717">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="718" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A718">
+        <v>177.83600000000001</v>
+      </c>
+      <c r="B718">
+        <v>0.5</v>
+      </c>
+      <c r="C718">
+        <v>0.7</v>
+      </c>
+      <c r="D718">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="719" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A719">
+        <v>178.036</v>
+      </c>
+      <c r="B719">
+        <v>-0.2</v>
+      </c>
+      <c r="C719">
+        <v>0.7</v>
+      </c>
+      <c r="D719">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="720" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A720">
+        <v>178.33600000000001</v>
+      </c>
+      <c r="B720">
+        <v>1.3</v>
+      </c>
+      <c r="C720">
+        <v>0.7</v>
+      </c>
+      <c r="D720">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="721" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A721">
+        <v>178.83600000000001</v>
+      </c>
+      <c r="B721">
+        <v>0</v>
+      </c>
+      <c r="C721">
+        <v>0.7</v>
+      </c>
+      <c r="D721">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="722" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A722">
+        <v>179.036</v>
+      </c>
+      <c r="B722">
+        <v>-0.8</v>
+      </c>
+      <c r="C722">
+        <v>1</v>
+      </c>
+      <c r="D722">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="723" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A723">
+        <v>179.136</v>
+      </c>
+      <c r="B723">
+        <v>-0.8</v>
+      </c>
+      <c r="C723">
+        <v>1</v>
+      </c>
+      <c r="D723">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="724" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A724">
+        <v>179.33600000000001</v>
+      </c>
+      <c r="B724">
+        <v>0.8</v>
+      </c>
+      <c r="C724">
+        <v>1</v>
+      </c>
+      <c r="D724">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="725" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A725">
+        <v>179.43600000000001</v>
+      </c>
+      <c r="B725">
+        <v>0.8</v>
+      </c>
+      <c r="C725">
+        <v>1</v>
+      </c>
+      <c r="D725">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="726" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A726">
+        <v>179.63600000000002</v>
+      </c>
+      <c r="B726">
+        <v>1</v>
+      </c>
+      <c r="C726">
+        <v>1.5</v>
+      </c>
+      <c r="D726">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="727" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A727">
+        <v>179.63600000000002</v>
+      </c>
+      <c r="B727">
+        <v>-1</v>
+      </c>
+      <c r="C727">
+        <v>1.5</v>
+      </c>
+      <c r="D727">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="728" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A728">
+        <v>180.036</v>
+      </c>
+      <c r="B728">
+        <v>0.3</v>
+      </c>
+      <c r="C728">
+        <v>0.7</v>
+      </c>
+      <c r="D728">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="729" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A729">
+        <v>180.13600000000002</v>
+      </c>
+      <c r="B729">
+        <v>-1.3</v>
+      </c>
+      <c r="C729">
+        <v>0.7</v>
+      </c>
+      <c r="D729">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="730" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A730">
+        <v>180.23599999999999</v>
+      </c>
+      <c r="B730">
+        <v>1</v>
+      </c>
+      <c r="C730">
+        <v>0.7</v>
+      </c>
+      <c r="D730">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="731" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A731">
+        <v>180.33600000000001</v>
+      </c>
+      <c r="B731">
+        <v>-0.1</v>
+      </c>
+      <c r="C731">
+        <v>0.7</v>
+      </c>
+      <c r="D731">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="732" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A732">
+        <v>180.73599999999999</v>
+      </c>
+      <c r="B732">
+        <v>0.2</v>
+      </c>
+      <c r="C732">
+        <v>0.7</v>
+      </c>
+      <c r="D732">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="733" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A733">
+        <v>181.036</v>
+      </c>
+      <c r="B733">
+        <v>-0.5</v>
+      </c>
+      <c r="C733">
+        <v>0.7</v>
+      </c>
+      <c r="D733">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="734" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A734">
+        <v>181.23599999999999</v>
+      </c>
+      <c r="B734">
+        <v>-1.5</v>
+      </c>
+      <c r="C734">
+        <v>0.7</v>
+      </c>
+      <c r="D734">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="735" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A735">
+        <v>181.536</v>
+      </c>
+      <c r="B735">
+        <v>0.2</v>
+      </c>
+      <c r="C735">
+        <v>0.7</v>
+      </c>
+      <c r="D735">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="736" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A736">
+        <v>181.83600000000001</v>
+      </c>
+      <c r="B736">
+        <v>-0.5</v>
+      </c>
+      <c r="C736">
+        <v>0.7</v>
+      </c>
+      <c r="D736">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="737" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A737">
+        <v>182.036</v>
+      </c>
+      <c r="B737">
+        <v>-1.5</v>
+      </c>
+      <c r="C737">
+        <v>0.7</v>
+      </c>
+      <c r="D737">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="738" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A738">
+        <v>182.036</v>
+      </c>
+      <c r="B738">
+        <v>0.2</v>
+      </c>
+      <c r="C738">
+        <v>0.7</v>
+      </c>
+      <c r="D738">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="739" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A739">
+        <v>182.43600000000001</v>
+      </c>
+      <c r="B739">
+        <v>1.5</v>
+      </c>
+      <c r="C739">
+        <v>0.7</v>
+      </c>
+      <c r="D739">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="740" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A740">
+        <v>182.43600000000001</v>
+      </c>
+      <c r="B740">
+        <v>-0.2</v>
+      </c>
+      <c r="C740">
+        <v>0.7</v>
+      </c>
+      <c r="D740">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="741" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A741">
+        <v>182.83600000000001</v>
+      </c>
+      <c r="B741">
+        <v>-1.4</v>
+      </c>
+      <c r="C741">
+        <v>1.2</v>
+      </c>
+      <c r="D741">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="742" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A742">
+        <v>182.93600000000001</v>
+      </c>
+      <c r="B742">
+        <v>1.4</v>
+      </c>
+      <c r="C742">
+        <v>0.7</v>
+      </c>
+      <c r="D742">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="743" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A743">
+        <v>183.036</v>
+      </c>
+      <c r="B743">
+        <v>-0.5</v>
+      </c>
+      <c r="C743">
+        <v>0.7</v>
+      </c>
+      <c r="D743">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="744" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A744">
+        <v>183.13600000000002</v>
+      </c>
+      <c r="B744">
+        <v>0.5</v>
+      </c>
+      <c r="C744">
+        <v>0.7</v>
+      </c>
+      <c r="D744">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="745" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A745">
+        <v>183.23599999999999</v>
+      </c>
+      <c r="B745">
+        <v>1.35</v>
+      </c>
+      <c r="C745">
+        <v>1.3</v>
+      </c>
+      <c r="D745">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="746" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A746">
+        <v>183.33600000000001</v>
+      </c>
+      <c r="B746">
+        <v>-1.2</v>
+      </c>
+      <c r="C746">
+        <v>0.7</v>
+      </c>
+      <c r="D746">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="747" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A747">
+        <v>183.43600000000001</v>
+      </c>
+      <c r="B747">
+        <v>0.6</v>
+      </c>
+      <c r="C747">
+        <v>0.7</v>
+      </c>
+      <c r="D747">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="748" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A748">
+        <v>183.536</v>
+      </c>
+      <c r="B748">
+        <v>-0.4</v>
+      </c>
+      <c r="C748">
+        <v>0.7</v>
+      </c>
+      <c r="D748">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="749" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A749">
+        <v>183.63600000000002</v>
+      </c>
+      <c r="B749">
+        <v>-1.3</v>
+      </c>
+      <c r="C749">
+        <v>1.4</v>
+      </c>
+      <c r="D749">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="750" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A750">
+        <v>183.73599999999999</v>
+      </c>
+      <c r="B750">
+        <v>1</v>
+      </c>
+      <c r="C750">
+        <v>0.7</v>
+      </c>
+      <c r="D750">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="751" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A751">
+        <v>183.83600000000001</v>
+      </c>
+      <c r="B751">
+        <v>-0.7</v>
+      </c>
+      <c r="C751">
+        <v>0.7</v>
+      </c>
+      <c r="D751">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="752" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A752">
+        <v>183.93600000000001</v>
+      </c>
+      <c r="B752">
+        <v>0.3</v>
+      </c>
+      <c r="C752">
+        <v>0.7</v>
+      </c>
+      <c r="D752">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="753" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A753">
+        <v>184.036</v>
+      </c>
+      <c r="B753">
+        <v>1.25</v>
+      </c>
+      <c r="C753">
+        <v>1.5</v>
+      </c>
+      <c r="D753">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="754" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A754">
+        <v>184.13600000000002</v>
+      </c>
+      <c r="B754">
+        <v>-0.8</v>
+      </c>
+      <c r="C754">
+        <v>0.7</v>
+      </c>
+      <c r="D754">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="755" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A755">
+        <v>184.23599999999999</v>
+      </c>
+      <c r="B755">
+        <v>0.8</v>
+      </c>
+      <c r="C755">
+        <v>0.7</v>
+      </c>
+      <c r="D755">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="756" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A756">
+        <v>184.33600000000001</v>
+      </c>
+      <c r="B756">
+        <v>-0.2</v>
+      </c>
+      <c r="C756">
+        <v>0.7</v>
+      </c>
+      <c r="D756">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="757" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A757">
+        <v>184.43600000000001</v>
+      </c>
+      <c r="B757">
+        <v>-1.2</v>
+      </c>
+      <c r="C757">
+        <v>1.6</v>
+      </c>
+      <c r="D757">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="758" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A758">
+        <v>184.536</v>
+      </c>
+      <c r="B758">
+        <v>0.6</v>
+      </c>
+      <c r="C758">
+        <v>0.8</v>
+      </c>
+      <c r="D758">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="759" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A759">
+        <v>184.63600000000002</v>
+      </c>
+      <c r="B759">
+        <v>-0.9</v>
+      </c>
+      <c r="C759">
+        <v>0.8</v>
+      </c>
+      <c r="D759">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="760" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A760">
+        <v>184.73599999999999</v>
+      </c>
+      <c r="B760">
+        <v>0.1</v>
+      </c>
+      <c r="C760">
+        <v>0.8</v>
+      </c>
+      <c r="D760">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="761" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A761">
+        <v>184.83600000000001</v>
+      </c>
+      <c r="B761">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="C761">
+        <v>1.7</v>
+      </c>
+      <c r="D761">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="762" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A762">
+        <v>184.93600000000001</v>
+      </c>
+      <c r="B762">
+        <v>-0.4</v>
+      </c>
+      <c r="C762">
+        <v>0.8</v>
+      </c>
+      <c r="D762">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="763" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A763">
+        <v>185.036</v>
+      </c>
+      <c r="B763">
+        <v>1</v>
+      </c>
+      <c r="C763">
+        <v>0.8</v>
+      </c>
+      <c r="D763">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="764" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A764">
+        <v>185.13600000000002</v>
+      </c>
+      <c r="B764">
+        <v>0</v>
+      </c>
+      <c r="C764">
+        <v>0.8</v>
+      </c>
+      <c r="D764">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="765" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A765">
+        <v>185.23599999999999</v>
+      </c>
+      <c r="B765">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C765">
+        <v>1.8</v>
+      </c>
+      <c r="D765">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="766" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A766">
+        <v>185.33600000000001</v>
+      </c>
+      <c r="B766">
+        <v>0.2</v>
+      </c>
+      <c r="C766">
+        <v>0.8</v>
+      </c>
+      <c r="D766">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="767" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A767">
+        <v>185.43600000000001</v>
+      </c>
+      <c r="B767">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C767">
+        <v>0.8</v>
+      </c>
+      <c r="D767">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="768" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A768">
+        <v>185.536</v>
+      </c>
+      <c r="B768">
+        <v>-0.1</v>
+      </c>
+      <c r="C768">
+        <v>0.8</v>
+      </c>
+      <c r="D768">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="769" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A769">
+        <v>185.63600000000002</v>
+      </c>
+      <c r="B769">
+        <v>1.05</v>
+      </c>
+      <c r="C769">
+        <v>1.9</v>
+      </c>
+      <c r="D769">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="770" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A770">
+        <v>185.73599999999999</v>
+      </c>
+      <c r="B770">
+        <v>0</v>
+      </c>
+      <c r="C770">
+        <v>0.8</v>
+      </c>
+      <c r="D770">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="771" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A771">
+        <v>185.83600000000001</v>
+      </c>
+      <c r="B771">
+        <v>1.2</v>
+      </c>
+      <c r="C771">
+        <v>0.8</v>
+      </c>
+      <c r="D771">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="772" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A772">
+        <v>185.93600000000001</v>
+      </c>
+      <c r="B772">
+        <v>-0.2</v>
+      </c>
+      <c r="C772">
+        <v>0.8</v>
+      </c>
+      <c r="D772">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="773" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A773">
+        <v>186.036</v>
+      </c>
+      <c r="B773">
+        <v>-1</v>
+      </c>
+      <c r="C773">
+        <v>2</v>
+      </c>
+      <c r="D773">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="774" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A774">
+        <v>186.23599999999999</v>
+      </c>
+      <c r="B774">
+        <v>-0.33300000000000002</v>
+      </c>
+      <c r="C774">
+        <v>2</v>
+      </c>
+      <c r="D774">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="775" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A775">
+        <v>186.43600000000001</v>
+      </c>
+      <c r="B775">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="C775">
+        <v>2</v>
+      </c>
+      <c r="D775">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="776" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A776">
+        <v>186.63600000000002</v>
+      </c>
+      <c r="B776">
+        <v>1</v>
+      </c>
+      <c r="C776">
+        <v>2</v>
+      </c>
+      <c r="D776">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="777" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A777">
+        <v>186.83600000000001</v>
+      </c>
+      <c r="B777">
+        <v>1</v>
+      </c>
+      <c r="C777">
+        <v>2</v>
+      </c>
+      <c r="D777">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="778" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A778">
+        <v>187.036</v>
+      </c>
+      <c r="B778">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="C778">
+        <v>2</v>
+      </c>
+      <c r="D778">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="779" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A779">
+        <v>187.23599999999999</v>
+      </c>
+      <c r="B779">
+        <v>-0.33300000000000002</v>
+      </c>
+      <c r="C779">
+        <v>2</v>
+      </c>
+      <c r="D779">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="780" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A780">
+        <v>187.43600000000001</v>
+      </c>
+      <c r="B780">
+        <v>-1</v>
+      </c>
+      <c r="C780">
+        <v>2</v>
+      </c>
+      <c r="D780">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="781" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A781">
+        <v>189.636</v>
+      </c>
+      <c r="B781">
+        <v>1.5</v>
+      </c>
+      <c r="C781">
+        <v>1</v>
+      </c>
+      <c r="D781">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="782" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A782">
+        <v>189.73599999999999</v>
+      </c>
+      <c r="B782">
+        <v>1.5</v>
+      </c>
+      <c r="C782">
+        <v>1</v>
+      </c>
+      <c r="D782">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="783" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A783">
+        <v>189.83600000000001</v>
+      </c>
+      <c r="B783">
+        <v>-1.5</v>
+      </c>
+      <c r="C783">
+        <v>1</v>
+      </c>
+      <c r="D783">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="784" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A784">
+        <v>189.93600000000001</v>
+      </c>
+      <c r="B784">
+        <v>-1.5</v>
+      </c>
+      <c r="C784">
+        <v>1</v>
+      </c>
+      <c r="D784">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="785" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A785">
+        <v>190.43600000000001</v>
+      </c>
+      <c r="B785">
+        <v>-1.2</v>
+      </c>
+      <c r="C785">
+        <v>1.6</v>
+      </c>
+      <c r="D785">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="786" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A786">
+        <v>190.536</v>
+      </c>
+      <c r="B786">
+        <v>0.6</v>
+      </c>
+      <c r="C786">
+        <v>1.2</v>
+      </c>
+      <c r="D786">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="787" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A787">
+        <v>190.636</v>
+      </c>
+      <c r="B787">
+        <v>0.4</v>
+      </c>
+      <c r="C787">
+        <v>1.2</v>
+      </c>
+      <c r="D787">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="788" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A788">
+        <v>190.73599999999999</v>
+      </c>
+      <c r="B788">
+        <v>0.2</v>
+      </c>
+      <c r="C788">
+        <v>1.2</v>
+      </c>
+      <c r="D788">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="789" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A789">
+        <v>190.83600000000001</v>
+      </c>
+      <c r="B789">
+        <v>0</v>
+      </c>
+      <c r="C789">
+        <v>1.2</v>
+      </c>
+      <c r="D789">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="790" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A790">
+        <v>190.93600000000001</v>
+      </c>
+      <c r="B790">
+        <v>-0.2</v>
+      </c>
+      <c r="C790">
+        <v>1.2</v>
+      </c>
+      <c r="D790">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="791" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A791">
+        <v>191.036</v>
+      </c>
+      <c r="B791">
+        <v>-0.4</v>
+      </c>
+      <c r="C791">
+        <v>1.2</v>
+      </c>
+      <c r="D791">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="792" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A792">
+        <v>191.136</v>
+      </c>
+      <c r="B792">
+        <v>-0.6</v>
+      </c>
+      <c r="C792">
+        <v>1.2</v>
+      </c>
+      <c r="D792">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="793" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A793">
+        <v>191.23599999999999</v>
+      </c>
+      <c r="B793">
+        <v>-0.8</v>
+      </c>
+      <c r="C793">
+        <v>1.2</v>
+      </c>
+      <c r="D793">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="794" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A794">
+        <v>191.33600000000001</v>
+      </c>
+      <c r="B794">
+        <v>-1</v>
+      </c>
+      <c r="C794">
+        <v>1.2</v>
+      </c>
+      <c r="D794">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="795" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A795">
+        <v>192.536</v>
+      </c>
+      <c r="B795">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C795">
+        <v>1.2</v>
+      </c>
+      <c r="D795">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="796" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A796">
+        <v>192.636</v>
+      </c>
+      <c r="B796">
+        <v>0.9</v>
+      </c>
+      <c r="C796">
+        <v>1.2</v>
+      </c>
+      <c r="D796">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="797" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A797">
+        <v>192.73599999999999</v>
+      </c>
+      <c r="B797">
+        <v>0.7</v>
+      </c>
+      <c r="C797">
+        <v>1.2</v>
+      </c>
+      <c r="D797">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="798" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A798">
+        <v>192.83600000000001</v>
+      </c>
+      <c r="B798">
+        <v>0.5</v>
+      </c>
+      <c r="C798">
+        <v>1.2</v>
+      </c>
+      <c r="D798">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="799" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A799">
+        <v>192.93600000000001</v>
+      </c>
+      <c r="B799">
+        <v>0.3</v>
+      </c>
+      <c r="C799">
+        <v>1.2</v>
+      </c>
+      <c r="D799">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="800" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A800">
+        <v>193.036</v>
+      </c>
+      <c r="B800">
+        <v>0.1</v>
+      </c>
+      <c r="C800">
+        <v>1.2</v>
+      </c>
+      <c r="D800">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="801" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A801">
+        <v>193.136</v>
+      </c>
+      <c r="B801">
+        <v>-9.9999999999999895E-2</v>
+      </c>
+      <c r="C801">
+        <v>1.2</v>
+      </c>
+      <c r="D801">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="802" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A802">
+        <v>193.73599999999999</v>
+      </c>
+      <c r="B802">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C802">
+        <v>1.2</v>
+      </c>
+      <c r="D802">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="803" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A803">
+        <v>193.83599999999998</v>
+      </c>
+      <c r="B803">
+        <v>-0.9</v>
+      </c>
+      <c r="C803">
+        <v>1.2</v>
+      </c>
+      <c r="D803">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="804" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A804">
+        <v>193.93599999999998</v>
+      </c>
+      <c r="B804">
+        <v>-0.7</v>
+      </c>
+      <c r="C804">
+        <v>1.2</v>
+      </c>
+      <c r="D804">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="805" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A805">
+        <v>194.036</v>
+      </c>
+      <c r="B805">
+        <v>-0.5</v>
+      </c>
+      <c r="C805">
+        <v>1.2</v>
+      </c>
+      <c r="D805">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="806" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A806">
+        <v>194.136</v>
+      </c>
+      <c r="B806">
+        <v>-0.3</v>
+      </c>
+      <c r="C806">
+        <v>1.2</v>
+      </c>
+      <c r="D806">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="807" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A807">
+        <v>194.23599999999999</v>
+      </c>
+      <c r="B807">
+        <v>-0.1</v>
+      </c>
+      <c r="C807">
+        <v>1.2</v>
+      </c>
+      <c r="D807">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="808" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A808">
+        <v>194.33599999999998</v>
+      </c>
+      <c r="B808">
+        <v>9.9999999999999895E-2</v>
+      </c>
+      <c r="C808">
+        <v>1.2</v>
+      </c>
+      <c r="D808">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="809" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A809">
+        <v>194.43600000000001</v>
+      </c>
+      <c r="B809">
+        <v>0.3</v>
+      </c>
+      <c r="C809">
+        <v>1.2</v>
+      </c>
+      <c r="D809">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="810" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A810">
+        <v>195.43600000000001</v>
+      </c>
+      <c r="B810">
+        <v>0</v>
+      </c>
+      <c r="C810">
+        <v>1</v>
+      </c>
+      <c r="D810">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="811" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A811">
+        <v>195.636</v>
+      </c>
+      <c r="B811">
+        <v>-1.5</v>
+      </c>
+      <c r="C811">
+        <v>1</v>
+      </c>
+      <c r="D811">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="812" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A812">
+        <v>196.83600000000001</v>
+      </c>
+      <c r="B812">
+        <v>-1</v>
+      </c>
+      <c r="C812">
+        <v>1.6</v>
+      </c>
+      <c r="D812">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="813" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A813">
+        <v>196.83600000000001</v>
+      </c>
+      <c r="B813">
+        <v>1</v>
+      </c>
+      <c r="C813">
+        <v>1.6</v>
+      </c>
+      <c r="D813">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="814" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A814">
+        <v>196.93600000000001</v>
+      </c>
+      <c r="B814">
+        <v>1.5</v>
+      </c>
+      <c r="C814">
+        <v>0.7</v>
+      </c>
+      <c r="D814">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="815" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A815">
+        <v>197.036</v>
+      </c>
+      <c r="B815">
+        <v>-0.5</v>
+      </c>
+      <c r="C815">
+        <v>0.7</v>
+      </c>
+      <c r="D815">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="816" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A816">
+        <v>197.136</v>
+      </c>
+      <c r="B816">
+        <v>0.5</v>
+      </c>
+      <c r="C816">
+        <v>0.7</v>
+      </c>
+      <c r="D816">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="817" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A817">
+        <v>197.23599999999999</v>
+      </c>
+      <c r="B817">
+        <v>-1.5</v>
+      </c>
+      <c r="C817">
+        <v>0.7</v>
+      </c>
+      <c r="D817">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="818" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A818">
+        <v>197.33600000000001</v>
+      </c>
+      <c r="B818">
+        <v>0.5</v>
+      </c>
+      <c r="C818">
+        <v>0.7</v>
+      </c>
+      <c r="D818">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="819" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A819">
+        <v>197.43600000000001</v>
+      </c>
+      <c r="B819">
+        <v>-0.5</v>
+      </c>
+      <c r="C819">
+        <v>0.7</v>
+      </c>
+      <c r="D819">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="820" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A820">
+        <v>197.536</v>
+      </c>
+      <c r="B820">
+        <v>1.5</v>
+      </c>
+      <c r="C820">
+        <v>0.7</v>
+      </c>
+      <c r="D820">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="821" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A821">
+        <v>197.636</v>
+      </c>
+      <c r="B821">
+        <v>-1.5</v>
+      </c>
+      <c r="C821">
+        <v>0.7</v>
+      </c>
+      <c r="D821">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="822" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A822">
+        <v>197.73599999999999</v>
+      </c>
+      <c r="B822">
+        <v>0.5</v>
+      </c>
+      <c r="C822">
+        <v>0.7</v>
+      </c>
+      <c r="D822">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="823" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A823">
+        <v>197.83600000000001</v>
+      </c>
+      <c r="B823">
+        <v>-0.5</v>
+      </c>
+      <c r="C823">
+        <v>0.7</v>
+      </c>
+      <c r="D823">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="824" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A824">
+        <v>197.93600000000001</v>
+      </c>
+      <c r="B824">
+        <v>1.5</v>
+      </c>
+      <c r="C824">
+        <v>0.7</v>
+      </c>
+      <c r="D824">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="825" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A825">
+        <v>198.036</v>
+      </c>
+      <c r="B825">
+        <v>1.2</v>
+      </c>
+      <c r="C825">
+        <v>1.6</v>
+      </c>
+      <c r="D825">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="826" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A826">
+        <v>198.036</v>
+      </c>
+      <c r="B826">
+        <v>0.3</v>
+      </c>
+      <c r="C826">
+        <v>1.6</v>
+      </c>
+      <c r="D826">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -13860,10 +16070,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{967B2D43-E0B0-4050-83A2-AF5C6E5EE029}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:J239"/>
+  <dimension ref="A1:J265"/>
   <sheetViews>
-    <sheetView topLeftCell="A205" workbookViewId="0">
-      <selection activeCell="G242" sqref="G242"/>
+    <sheetView topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="N250" sqref="N250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -21514,6 +23724,838 @@
       </c>
       <c r="J239" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A240">
+        <v>1</v>
+      </c>
+      <c r="B240">
+        <v>182</v>
+      </c>
+      <c r="C240">
+        <v>186.13600000000002</v>
+      </c>
+      <c r="D240">
+        <v>-1.8</v>
+      </c>
+      <c r="E240">
+        <v>-1</v>
+      </c>
+      <c r="F240">
+        <v>186.23600000000002</v>
+      </c>
+      <c r="G240">
+        <v>-1.8</v>
+      </c>
+      <c r="H240">
+        <v>-1</v>
+      </c>
+      <c r="I240" t="s">
+        <v>25</v>
+      </c>
+      <c r="J240" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A241">
+        <v>1</v>
+      </c>
+      <c r="B241">
+        <v>183</v>
+      </c>
+      <c r="C241">
+        <v>186.33600000000001</v>
+      </c>
+      <c r="D241">
+        <v>-0.86699999999999999</v>
+      </c>
+      <c r="E241">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="F241">
+        <v>186.43600000000001</v>
+      </c>
+      <c r="G241">
+        <v>-0.86699999999999999</v>
+      </c>
+      <c r="H241">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="I241" t="s">
+        <v>25</v>
+      </c>
+      <c r="J241" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A242">
+        <v>1</v>
+      </c>
+      <c r="B242">
+        <v>184</v>
+      </c>
+      <c r="C242">
+        <v>186.536</v>
+      </c>
+      <c r="D242">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E242">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="F242">
+        <v>186.636</v>
+      </c>
+      <c r="G242">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H242">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I242" t="s">
+        <v>25</v>
+      </c>
+      <c r="J242" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A243">
+        <v>1</v>
+      </c>
+      <c r="B243">
+        <v>185</v>
+      </c>
+      <c r="C243">
+        <v>186.73599999999999</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+      <c r="E243">
+        <v>1.8</v>
+      </c>
+      <c r="F243">
+        <v>186.83599999999998</v>
+      </c>
+      <c r="G243">
+        <v>1</v>
+      </c>
+      <c r="H243">
+        <v>1.8</v>
+      </c>
+      <c r="I243" t="s">
+        <v>25</v>
+      </c>
+      <c r="J243" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A244">
+        <v>17</v>
+      </c>
+      <c r="B244">
+        <v>186</v>
+      </c>
+      <c r="C244">
+        <v>186.93600000000001</v>
+      </c>
+      <c r="D244">
+        <v>1</v>
+      </c>
+      <c r="E244">
+        <v>1.8</v>
+      </c>
+      <c r="F244">
+        <v>187.036</v>
+      </c>
+      <c r="G244">
+        <v>1</v>
+      </c>
+      <c r="H244">
+        <v>1.8</v>
+      </c>
+      <c r="I244" t="s">
+        <v>25</v>
+      </c>
+      <c r="J244" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A245">
+        <v>17</v>
+      </c>
+      <c r="B245">
+        <v>187</v>
+      </c>
+      <c r="C245">
+        <v>187.13600000000002</v>
+      </c>
+      <c r="D245">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="E245">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="F245">
+        <v>187.23599999999999</v>
+      </c>
+      <c r="G245">
+        <v>6.7000000000000004E-2</v>
+      </c>
+      <c r="H245">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="I245" t="s">
+        <v>25</v>
+      </c>
+      <c r="J245" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A246">
+        <v>17</v>
+      </c>
+      <c r="B246">
+        <v>188</v>
+      </c>
+      <c r="C246">
+        <v>187.33600000000001</v>
+      </c>
+      <c r="D246">
+        <v>-0.86699999999999999</v>
+      </c>
+      <c r="E246">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="F246">
+        <v>187.43600000000001</v>
+      </c>
+      <c r="G246">
+        <v>-0.86699999999999999</v>
+      </c>
+      <c r="H246">
+        <v>-6.7000000000000004E-2</v>
+      </c>
+      <c r="I246" t="s">
+        <v>25</v>
+      </c>
+      <c r="J246" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A247">
+        <v>17</v>
+      </c>
+      <c r="B247">
+        <v>189</v>
+      </c>
+      <c r="C247">
+        <v>187.536</v>
+      </c>
+      <c r="D247">
+        <v>-1.8</v>
+      </c>
+      <c r="E247">
+        <v>-1</v>
+      </c>
+      <c r="F247">
+        <v>187.63600000000002</v>
+      </c>
+      <c r="G247">
+        <v>-1.8</v>
+      </c>
+      <c r="H247">
+        <v>-1</v>
+      </c>
+      <c r="I247" t="s">
+        <v>25</v>
+      </c>
+      <c r="J247" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A248">
+        <v>17</v>
+      </c>
+      <c r="B248">
+        <v>190</v>
+      </c>
+      <c r="C248">
+        <v>189.23599999999999</v>
+      </c>
+      <c r="D248">
+        <v>-1.6</v>
+      </c>
+      <c r="E248">
+        <v>0.4</v>
+      </c>
+      <c r="F248">
+        <v>189.386</v>
+      </c>
+      <c r="G248">
+        <v>1.2</v>
+      </c>
+      <c r="H248">
+        <v>2</v>
+      </c>
+      <c r="I248" t="s">
+        <v>25</v>
+      </c>
+      <c r="J248" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A249">
+        <v>17</v>
+      </c>
+      <c r="B249">
+        <v>190</v>
+      </c>
+      <c r="C249">
+        <v>189.386</v>
+      </c>
+      <c r="D249">
+        <v>1.2</v>
+      </c>
+      <c r="E249">
+        <v>2</v>
+      </c>
+      <c r="F249">
+        <v>189.536</v>
+      </c>
+      <c r="G249">
+        <v>1.2</v>
+      </c>
+      <c r="H249">
+        <v>2</v>
+      </c>
+      <c r="I249" t="s">
+        <v>25</v>
+      </c>
+      <c r="J249" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A250">
+        <v>19</v>
+      </c>
+      <c r="B250">
+        <v>191</v>
+      </c>
+      <c r="C250">
+        <v>189.23599999999999</v>
+      </c>
+      <c r="D250">
+        <v>-0.4</v>
+      </c>
+      <c r="E250">
+        <v>1.6</v>
+      </c>
+      <c r="F250">
+        <v>189.386</v>
+      </c>
+      <c r="G250">
+        <v>-2</v>
+      </c>
+      <c r="H250">
+        <v>-1.2</v>
+      </c>
+      <c r="I250" t="s">
+        <v>25</v>
+      </c>
+      <c r="J250" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A251">
+        <v>19</v>
+      </c>
+      <c r="B251">
+        <v>191</v>
+      </c>
+      <c r="C251">
+        <v>189.386</v>
+      </c>
+      <c r="D251">
+        <v>-2</v>
+      </c>
+      <c r="E251">
+        <v>-1.2</v>
+      </c>
+      <c r="F251">
+        <v>189.73599999999999</v>
+      </c>
+      <c r="G251">
+        <v>-2</v>
+      </c>
+      <c r="H251">
+        <v>-1.2</v>
+      </c>
+      <c r="I251" t="s">
+        <v>25</v>
+      </c>
+      <c r="J251" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A252">
+        <v>19</v>
+      </c>
+      <c r="B252">
+        <v>192</v>
+      </c>
+      <c r="C252">
+        <v>190.036</v>
+      </c>
+      <c r="D252">
+        <v>1.4</v>
+      </c>
+      <c r="E252">
+        <v>2</v>
+      </c>
+      <c r="F252">
+        <v>190.23599999999999</v>
+      </c>
+      <c r="G252">
+        <v>-2</v>
+      </c>
+      <c r="H252">
+        <v>-0.5</v>
+      </c>
+      <c r="I252" t="s">
+        <v>31</v>
+      </c>
+      <c r="J252" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A253">
+        <v>19</v>
+      </c>
+      <c r="B253">
+        <v>192</v>
+      </c>
+      <c r="C253">
+        <v>190.23599999999999</v>
+      </c>
+      <c r="D253">
+        <v>-2</v>
+      </c>
+      <c r="E253">
+        <v>-0.5</v>
+      </c>
+      <c r="F253">
+        <v>190.43600000000001</v>
+      </c>
+      <c r="G253">
+        <v>1</v>
+      </c>
+      <c r="H253">
+        <v>2</v>
+      </c>
+      <c r="I253" t="s">
+        <v>24</v>
+      </c>
+      <c r="J253" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A254">
+        <v>19</v>
+      </c>
+      <c r="B254">
+        <v>192</v>
+      </c>
+      <c r="C254">
+        <v>190.43600000000001</v>
+      </c>
+      <c r="D254">
+        <v>1</v>
+      </c>
+      <c r="E254">
+        <v>2</v>
+      </c>
+      <c r="F254">
+        <v>191.33600000000001</v>
+      </c>
+      <c r="G254">
+        <v>-0.8</v>
+      </c>
+      <c r="H254">
+        <v>0.2</v>
+      </c>
+      <c r="I254" t="s">
+        <v>25</v>
+      </c>
+      <c r="J254" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A255">
+        <v>17</v>
+      </c>
+      <c r="B255">
+        <v>193</v>
+      </c>
+      <c r="C255">
+        <v>191.43600000000001</v>
+      </c>
+      <c r="D255">
+        <v>-2</v>
+      </c>
+      <c r="E255">
+        <v>-0.7</v>
+      </c>
+      <c r="F255">
+        <v>191.636</v>
+      </c>
+      <c r="G255">
+        <v>-1.3</v>
+      </c>
+      <c r="H255">
+        <v>0</v>
+      </c>
+      <c r="I255" t="s">
+        <v>31</v>
+      </c>
+      <c r="J255" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A256">
+        <v>19</v>
+      </c>
+      <c r="B256">
+        <v>194</v>
+      </c>
+      <c r="C256">
+        <v>192.43600000000001</v>
+      </c>
+      <c r="D256">
+        <v>0.2</v>
+      </c>
+      <c r="E256">
+        <v>2</v>
+      </c>
+      <c r="F256">
+        <v>192.536</v>
+      </c>
+      <c r="G256">
+        <v>-0.6</v>
+      </c>
+      <c r="H256">
+        <v>0.4</v>
+      </c>
+      <c r="I256" t="s">
+        <v>25</v>
+      </c>
+      <c r="J256" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A257">
+        <v>19</v>
+      </c>
+      <c r="B257">
+        <v>194</v>
+      </c>
+      <c r="C257">
+        <v>192.536</v>
+      </c>
+      <c r="D257">
+        <v>-0.6</v>
+      </c>
+      <c r="E257">
+        <v>0.4</v>
+      </c>
+      <c r="F257">
+        <v>193.23599999999999</v>
+      </c>
+      <c r="G257">
+        <v>-2</v>
+      </c>
+      <c r="H257">
+        <v>-1</v>
+      </c>
+      <c r="I257" t="s">
+        <v>25</v>
+      </c>
+      <c r="J257" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A258">
+        <v>19</v>
+      </c>
+      <c r="B258">
+        <v>195</v>
+      </c>
+      <c r="C258">
+        <v>193.636</v>
+      </c>
+      <c r="D258">
+        <v>-2</v>
+      </c>
+      <c r="E258">
+        <v>-0.2</v>
+      </c>
+      <c r="F258">
+        <v>193.73599999999999</v>
+      </c>
+      <c r="G258">
+        <v>-0.4</v>
+      </c>
+      <c r="H258">
+        <v>0.6</v>
+      </c>
+      <c r="I258" t="s">
+        <v>25</v>
+      </c>
+      <c r="J258" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A259">
+        <v>19</v>
+      </c>
+      <c r="B259">
+        <v>195</v>
+      </c>
+      <c r="C259">
+        <v>193.73599999999999</v>
+      </c>
+      <c r="D259">
+        <v>-0.4</v>
+      </c>
+      <c r="E259">
+        <v>0.6</v>
+      </c>
+      <c r="F259">
+        <v>194.43599999999998</v>
+      </c>
+      <c r="G259">
+        <v>1</v>
+      </c>
+      <c r="H259">
+        <v>2</v>
+      </c>
+      <c r="I259" t="s">
+        <v>25</v>
+      </c>
+      <c r="J259" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A260">
+        <v>17</v>
+      </c>
+      <c r="B260">
+        <v>196</v>
+      </c>
+      <c r="C260">
+        <v>194.636</v>
+      </c>
+      <c r="D260">
+        <v>0.7</v>
+      </c>
+      <c r="E260">
+        <v>2</v>
+      </c>
+      <c r="F260">
+        <v>194.83600000000001</v>
+      </c>
+      <c r="G260">
+        <v>0</v>
+      </c>
+      <c r="H260">
+        <v>1.3</v>
+      </c>
+      <c r="I260" t="s">
+        <v>24</v>
+      </c>
+      <c r="J260" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A261">
+        <v>19</v>
+      </c>
+      <c r="B261">
+        <v>197</v>
+      </c>
+      <c r="C261">
+        <v>194.83600000000001</v>
+      </c>
+      <c r="D261">
+        <v>-2</v>
+      </c>
+      <c r="E261">
+        <v>-1.2</v>
+      </c>
+      <c r="F261">
+        <v>195.136</v>
+      </c>
+      <c r="G261">
+        <v>0.8</v>
+      </c>
+      <c r="H261">
+        <v>2</v>
+      </c>
+      <c r="I261" t="s">
+        <v>31</v>
+      </c>
+      <c r="J261" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A262">
+        <v>17</v>
+      </c>
+      <c r="B262">
+        <v>198</v>
+      </c>
+      <c r="C262">
+        <v>195.136</v>
+      </c>
+      <c r="D262">
+        <v>-2</v>
+      </c>
+      <c r="E262">
+        <v>-1.2</v>
+      </c>
+      <c r="F262">
+        <v>195.43600000000001</v>
+      </c>
+      <c r="G262">
+        <v>0.8</v>
+      </c>
+      <c r="H262">
+        <v>2</v>
+      </c>
+      <c r="I262" t="s">
+        <v>31</v>
+      </c>
+      <c r="J262" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A263">
+        <v>19</v>
+      </c>
+      <c r="B263">
+        <v>199</v>
+      </c>
+      <c r="C263">
+        <v>195.636</v>
+      </c>
+      <c r="D263">
+        <v>1.2</v>
+      </c>
+      <c r="E263">
+        <v>2</v>
+      </c>
+      <c r="F263">
+        <v>195.93600000000001</v>
+      </c>
+      <c r="G263">
+        <v>-2</v>
+      </c>
+      <c r="H263">
+        <v>-0.8</v>
+      </c>
+      <c r="I263" t="s">
+        <v>31</v>
+      </c>
+      <c r="J263" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A264">
+        <v>17</v>
+      </c>
+      <c r="B264">
+        <v>200</v>
+      </c>
+      <c r="C264">
+        <v>195.93600000000001</v>
+      </c>
+      <c r="D264">
+        <v>1.2</v>
+      </c>
+      <c r="E264">
+        <v>2</v>
+      </c>
+      <c r="F264">
+        <v>196.23599999999999</v>
+      </c>
+      <c r="G264">
+        <v>-2</v>
+      </c>
+      <c r="H264">
+        <v>-0.8</v>
+      </c>
+      <c r="I264" t="s">
+        <v>31</v>
+      </c>
+      <c r="J264" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A265">
+        <v>19</v>
+      </c>
+      <c r="B265">
+        <v>201</v>
+      </c>
+      <c r="C265">
+        <v>196.23599999999999</v>
+      </c>
+      <c r="D265">
+        <v>1.2</v>
+      </c>
+      <c r="E265">
+        <v>2</v>
+      </c>
+      <c r="F265">
+        <v>196.43600000000001</v>
+      </c>
+      <c r="G265">
+        <v>-0.7</v>
+      </c>
+      <c r="H265">
+        <v>0.3</v>
+      </c>
+      <c r="I265" t="s">
+        <v>31</v>
+      </c>
+      <c r="J265" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -21526,10 +24568,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C76DC57-EF49-44CE-8A21-D4353938F627}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:D213"/>
+  <dimension ref="A1:D229"/>
   <sheetViews>
-    <sheetView topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="A208" sqref="A208"/>
+    <sheetView topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="H231" sqref="H231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -24513,6 +27555,230 @@
         <v>0.6</v>
       </c>
       <c r="D213">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A214">
+        <v>177.566</v>
+      </c>
+      <c r="B214">
+        <v>1</v>
+      </c>
+      <c r="C214">
+        <v>0.6</v>
+      </c>
+      <c r="D214">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A215">
+        <v>178.499</v>
+      </c>
+      <c r="B215">
+        <v>1.7</v>
+      </c>
+      <c r="C215">
+        <v>0.6</v>
+      </c>
+      <c r="D215">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A216">
+        <v>178.54300000000001</v>
+      </c>
+      <c r="B216">
+        <v>1.4</v>
+      </c>
+      <c r="C216">
+        <v>0.6</v>
+      </c>
+      <c r="D216">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A217">
+        <v>178.636</v>
+      </c>
+      <c r="B217">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C217">
+        <v>0.6</v>
+      </c>
+      <c r="D217">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A218">
+        <v>191.636</v>
+      </c>
+      <c r="B218">
+        <v>0.3</v>
+      </c>
+      <c r="C218">
+        <v>0.5</v>
+      </c>
+      <c r="D218">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A219">
+        <v>191.703</v>
+      </c>
+      <c r="B219">
+        <v>-0.3</v>
+      </c>
+      <c r="C219">
+        <v>0.8</v>
+      </c>
+      <c r="D219">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A220">
+        <v>191.77</v>
+      </c>
+      <c r="B220">
+        <v>-1</v>
+      </c>
+      <c r="C220">
+        <v>0.5</v>
+      </c>
+      <c r="D220">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A221">
+        <v>191.83700000000002</v>
+      </c>
+      <c r="B221">
+        <v>-1.5</v>
+      </c>
+      <c r="C221">
+        <v>0.8</v>
+      </c>
+      <c r="D221">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A222">
+        <v>191.90400000000002</v>
+      </c>
+      <c r="B222">
+        <v>-1.2</v>
+      </c>
+      <c r="C222">
+        <v>0.5</v>
+      </c>
+      <c r="D222">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A223">
+        <v>191.97100000000003</v>
+      </c>
+      <c r="B223">
+        <v>-0.85</v>
+      </c>
+      <c r="C223">
+        <v>0.8</v>
+      </c>
+      <c r="D223">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A224">
+        <v>192.03800000000004</v>
+      </c>
+      <c r="B224">
+        <v>-0.45</v>
+      </c>
+      <c r="C224">
+        <v>0.5</v>
+      </c>
+      <c r="D224">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A225">
+        <v>192.10500000000005</v>
+      </c>
+      <c r="B225">
+        <v>0</v>
+      </c>
+      <c r="C225">
+        <v>0.8</v>
+      </c>
+      <c r="D225">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A226">
+        <v>192.17200000000005</v>
+      </c>
+      <c r="B226">
+        <v>0.4</v>
+      </c>
+      <c r="C226">
+        <v>0.5</v>
+      </c>
+      <c r="D226">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A227">
+        <v>192.23900000000006</v>
+      </c>
+      <c r="B227">
+        <v>0.8</v>
+      </c>
+      <c r="C227">
+        <v>0.8</v>
+      </c>
+      <c r="D227">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A228">
+        <v>192.30600000000007</v>
+      </c>
+      <c r="B228">
+        <v>1.2</v>
+      </c>
+      <c r="C228">
+        <v>0.5</v>
+      </c>
+      <c r="D228">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A229">
+        <v>192.37300000000008</v>
+      </c>
+      <c r="B229">
+        <v>1.6</v>
+      </c>
+      <c r="C229">
+        <v>0.8</v>
+      </c>
+      <c r="D229">
         <v>17</v>
       </c>
     </row>
@@ -24526,10 +27792,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58F96158-71D4-4C19-99F5-47E7932AF572}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A92" sqref="A92"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -26096,6 +29362,261 @@
       </c>
       <c r="E92">
         <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>177.23599999999999</v>
+      </c>
+      <c r="B93">
+        <v>-1.5</v>
+      </c>
+      <c r="C93">
+        <v>1</v>
+      </c>
+      <c r="D93">
+        <v>0.375</v>
+      </c>
+      <c r="E93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>177.636</v>
+      </c>
+      <c r="B94">
+        <v>-1.5</v>
+      </c>
+      <c r="C94">
+        <v>1</v>
+      </c>
+      <c r="D94">
+        <v>0.375</v>
+      </c>
+      <c r="E94">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>178.036</v>
+      </c>
+      <c r="B95">
+        <v>-1.5</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>0.375</v>
+      </c>
+      <c r="E95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>178.43600000000001</v>
+      </c>
+      <c r="B96">
+        <v>-1.5</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>0.375</v>
+      </c>
+      <c r="E96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>178.83600000000001</v>
+      </c>
+      <c r="B97">
+        <v>-1.5</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>0.375</v>
+      </c>
+      <c r="E97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>180.43600000000001</v>
+      </c>
+      <c r="B98">
+        <v>1.5</v>
+      </c>
+      <c r="C98">
+        <v>1</v>
+      </c>
+      <c r="D98">
+        <v>0.625</v>
+      </c>
+      <c r="E98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>180.83600000000001</v>
+      </c>
+      <c r="B99">
+        <v>1.5</v>
+      </c>
+      <c r="C99">
+        <v>1</v>
+      </c>
+      <c r="D99">
+        <v>0.625</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>181.23599999999999</v>
+      </c>
+      <c r="B100">
+        <v>1.5</v>
+      </c>
+      <c r="C100">
+        <v>1</v>
+      </c>
+      <c r="D100">
+        <v>0.625</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>181.63600000000002</v>
+      </c>
+      <c r="B101">
+        <v>1.5</v>
+      </c>
+      <c r="C101">
+        <v>1</v>
+      </c>
+      <c r="D101">
+        <v>0.625</v>
+      </c>
+      <c r="E101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>189.23599999999999</v>
+      </c>
+      <c r="B102">
+        <v>-0.6</v>
+      </c>
+      <c r="C102">
+        <v>2</v>
+      </c>
+      <c r="D102">
+        <v>0.25</v>
+      </c>
+      <c r="E102">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>189.23599999999999</v>
+      </c>
+      <c r="B103">
+        <v>0.6</v>
+      </c>
+      <c r="C103">
+        <v>2</v>
+      </c>
+      <c r="D103">
+        <v>0.75</v>
+      </c>
+      <c r="E103">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>192.43600000000001</v>
+      </c>
+      <c r="B104">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C104">
+        <v>1.8</v>
+      </c>
+      <c r="D104">
+        <v>0.75</v>
+      </c>
+      <c r="E104">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>193.23599999999999</v>
+      </c>
+      <c r="B105">
+        <v>-0.3</v>
+      </c>
+      <c r="C105">
+        <v>2</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106">
+        <v>193.636</v>
+      </c>
+      <c r="B106">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C106">
+        <v>1.8</v>
+      </c>
+      <c r="D106">
+        <v>0.25</v>
+      </c>
+      <c r="E106">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>196.43600000000001</v>
+      </c>
+      <c r="B107">
+        <v>1.2</v>
+      </c>
+      <c r="C107">
+        <v>1.6</v>
+      </c>
+      <c r="D107">
+        <v>0.875</v>
+      </c>
+      <c r="E107">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Color Line, and adjust Chart..
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Chart示例.xlsx
+++ b/Assets/Scripts/Chart示例.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Xenody-master\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D8C971-1739-4427-86C8-B2C108C58535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD581C71-1D6E-4017-9131-683A265F9B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="38">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -166,55 +166,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#00b2ee</t>
+    <t>#63b8ff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>#ff6347</t>
+    <t>#8ee5ee</t>
   </si>
   <si>
-    <t>#ff6348</t>
-  </si>
-  <si>
-    <t>#ff6349</t>
-  </si>
-  <si>
-    <t>#ff6350</t>
-  </si>
-  <si>
-    <t>#ff6351</t>
-  </si>
-  <si>
-    <t>#ff6352</t>
-  </si>
-  <si>
-    <t>#ff6353</t>
-  </si>
-  <si>
-    <t>#ff6354</t>
-  </si>
-  <si>
-    <t>#ff6355</t>
-  </si>
-  <si>
-    <t>#ff6356</t>
-  </si>
-  <si>
-    <t>#ff6357</t>
-  </si>
-  <si>
-    <t>#ff6358</t>
-  </si>
-  <si>
-    <t>#ff6359</t>
-  </si>
-  <si>
-    <t>#ff6360</t>
-  </si>
-  <si>
-    <t>#ff6361</t>
-  </si>
-  <si>
-    <t>#e066ff</t>
+    <t>#dda0dd</t>
   </si>
 </sst>
 </file>
@@ -597,7 +556,7 @@
   <dimension ref="A1:L240"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -635,8 +594,9 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>35</v>
+      <c r="B2" t="str">
+        <f>VLOOKUP(A2,$K$1:$L$20,2,FALSE)</f>
+        <v>#63b8ff</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -664,8 +624,9 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>35</v>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B66" si="0">VLOOKUP(A3,$K$1:$L$20,2,FALSE)</f>
+        <v>#63b8ff</v>
       </c>
       <c r="C3">
         <v>0.42699999999999999</v>
@@ -693,8 +654,9 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
-        <v>35</v>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C4">
         <v>1.246</v>
@@ -722,8 +684,9 @@
       <c r="A5">
         <v>1</v>
       </c>
-      <c r="B5" t="s">
-        <v>35</v>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C5">
         <v>3.246</v>
@@ -744,15 +707,16 @@
         <v>4</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>36</v>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C6">
         <v>1.246</v>
@@ -773,15 +737,16 @@
         <v>5</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
-      <c r="B7" t="s">
-        <v>35</v>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C7">
         <v>6.4450000000000003</v>
@@ -802,15 +767,16 @@
         <v>6</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>36</v>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C8">
         <v>6.4450000000000003</v>
@@ -831,15 +797,16 @@
         <v>7</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>35</v>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C9">
         <v>8.0259999999999998</v>
@@ -860,15 +827,16 @@
         <v>8</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
-      <c r="B10" t="s">
-        <v>36</v>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C10">
         <v>8.0259999999999998</v>
@@ -889,15 +857,16 @@
         <v>9</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
-        <v>35</v>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C11">
         <v>10.036</v>
@@ -918,15 +887,16 @@
         <v>10</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
-      <c r="B12" t="s">
-        <v>36</v>
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C12">
         <v>10.036</v>
@@ -947,15 +917,16 @@
         <v>11</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>35</v>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C13">
         <v>10.135999999999999</v>
@@ -976,15 +947,16 @@
         <v>12</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
-        <v>36</v>
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C14">
         <v>10.135999999999999</v>
@@ -1005,15 +977,16 @@
         <v>13</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
-        <v>35</v>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C15">
         <v>13.236000000000001</v>
@@ -1034,15 +1007,16 @@
         <v>14</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
-        <v>36</v>
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C16">
         <v>13.236000000000001</v>
@@ -1063,15 +1037,16 @@
         <v>15</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
-        <v>35</v>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C17">
         <v>13.336</v>
@@ -1092,15 +1067,16 @@
         <v>16</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
-      <c r="B18" t="s">
-        <v>36</v>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C18">
         <v>13.336</v>
@@ -1121,15 +1097,16 @@
         <v>17</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
-      <c r="B19" t="s">
-        <v>35</v>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C19">
         <v>16.436</v>
@@ -1150,15 +1127,16 @@
         <v>18</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
-      <c r="B20" t="s">
-        <v>36</v>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C20">
         <v>16.436</v>
@@ -1186,8 +1164,9 @@
       <c r="A21">
         <v>1</v>
       </c>
-      <c r="B21" t="s">
-        <v>35</v>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C21">
         <v>16.536000000000001</v>
@@ -1209,8 +1188,9 @@
       <c r="A22">
         <v>2</v>
       </c>
-      <c r="B22" t="s">
-        <v>36</v>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C22">
         <v>16.536000000000001</v>
@@ -1232,8 +1212,9 @@
       <c r="A23">
         <v>1</v>
       </c>
-      <c r="B23" t="s">
-        <v>35</v>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C23">
         <v>19.635999999999999</v>
@@ -1255,8 +1236,9 @@
       <c r="A24">
         <v>2</v>
       </c>
-      <c r="B24" t="s">
-        <v>36</v>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C24">
         <v>19.635999999999999</v>
@@ -1278,8 +1260,9 @@
       <c r="A25">
         <v>1</v>
       </c>
-      <c r="B25" t="s">
-        <v>35</v>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C25">
         <v>20.036000000000001</v>
@@ -1301,8 +1284,9 @@
       <c r="A26">
         <v>2</v>
       </c>
-      <c r="B26" t="s">
-        <v>36</v>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C26">
         <v>20.036000000000001</v>
@@ -1324,8 +1308,9 @@
       <c r="A27">
         <v>1</v>
       </c>
-      <c r="B27" t="s">
-        <v>35</v>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C27">
         <v>20.436</v>
@@ -1347,8 +1332,9 @@
       <c r="A28">
         <v>2</v>
       </c>
-      <c r="B28" t="s">
-        <v>36</v>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C28">
         <v>20.436</v>
@@ -1370,8 +1356,9 @@
       <c r="A29">
         <v>1</v>
       </c>
-      <c r="B29" t="s">
-        <v>35</v>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C29">
         <v>20.835999999999999</v>
@@ -1393,8 +1380,9 @@
       <c r="A30">
         <v>2</v>
       </c>
-      <c r="B30" t="s">
-        <v>36</v>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C30">
         <v>20.835999999999999</v>
@@ -1416,8 +1404,9 @@
       <c r="A31">
         <v>1</v>
       </c>
-      <c r="B31" t="s">
-        <v>35</v>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C31">
         <v>21.236000000000001</v>
@@ -1439,8 +1428,9 @@
       <c r="A32">
         <v>3</v>
       </c>
-      <c r="B32" t="s">
-        <v>36</v>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C32">
         <v>35.636000000000003</v>
@@ -1462,8 +1452,9 @@
       <c r="A33">
         <v>3</v>
       </c>
-      <c r="B33" t="s">
-        <v>36</v>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C33">
         <v>36.036000000000001</v>
@@ -1485,8 +1476,9 @@
       <c r="A34">
         <v>4</v>
       </c>
-      <c r="B34" t="s">
-        <v>37</v>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C34">
         <v>36.436</v>
@@ -1508,8 +1500,9 @@
       <c r="A35">
         <v>5</v>
       </c>
-      <c r="B35" t="s">
-        <v>38</v>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C35">
         <v>37.235999999999997</v>
@@ -1531,8 +1524,9 @@
       <c r="A36">
         <v>6</v>
       </c>
-      <c r="B36" t="s">
-        <v>39</v>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C36">
         <v>38.036000000000001</v>
@@ -1554,8 +1548,9 @@
       <c r="A37">
         <v>7</v>
       </c>
-      <c r="B37" t="s">
-        <v>40</v>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C37">
         <v>38.835999999999999</v>
@@ -1577,8 +1572,9 @@
       <c r="A38">
         <v>8</v>
       </c>
-      <c r="B38" t="s">
-        <v>41</v>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C38">
         <v>39.636000000000003</v>
@@ -1600,8 +1596,9 @@
       <c r="A39">
         <v>9</v>
       </c>
-      <c r="B39" t="s">
-        <v>42</v>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C39">
         <v>40.436</v>
@@ -1623,8 +1620,9 @@
       <c r="A40">
         <v>10</v>
       </c>
-      <c r="B40" t="s">
-        <v>43</v>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C40">
         <v>41.235999999999997</v>
@@ -1646,8 +1644,9 @@
       <c r="A41">
         <v>11</v>
       </c>
-      <c r="B41" t="s">
-        <v>44</v>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C41">
         <v>42.036000000000001</v>
@@ -1669,8 +1668,9 @@
       <c r="A42">
         <v>12</v>
       </c>
-      <c r="B42" t="s">
-        <v>45</v>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C42">
         <v>42.835999999999999</v>
@@ -1692,8 +1692,9 @@
       <c r="A43">
         <v>13</v>
       </c>
-      <c r="B43" t="s">
-        <v>46</v>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C43">
         <v>43.636000000000003</v>
@@ -1715,8 +1716,9 @@
       <c r="A44">
         <v>14</v>
       </c>
-      <c r="B44" t="s">
-        <v>47</v>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C44">
         <v>44.436</v>
@@ -1738,8 +1740,9 @@
       <c r="A45">
         <v>15</v>
       </c>
-      <c r="B45" t="s">
-        <v>48</v>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C45">
         <v>45.235999999999997</v>
@@ -1761,8 +1764,9 @@
       <c r="A46">
         <v>16</v>
       </c>
-      <c r="B46" t="s">
-        <v>49</v>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C46">
         <v>46.036000000000001</v>
@@ -1784,8 +1788,9 @@
       <c r="A47">
         <v>1</v>
       </c>
-      <c r="B47" t="s">
-        <v>35</v>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C47">
         <v>72.635999999999996</v>
@@ -1807,8 +1812,9 @@
       <c r="A48">
         <v>3</v>
       </c>
-      <c r="B48" t="s">
-        <v>36</v>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C48">
         <v>72.635999999999996</v>
@@ -1830,8 +1836,9 @@
       <c r="A49">
         <v>1</v>
       </c>
-      <c r="B49" t="s">
-        <v>35</v>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C49">
         <v>72.835999999999999</v>
@@ -1853,8 +1860,9 @@
       <c r="A50">
         <v>3</v>
       </c>
-      <c r="B50" t="s">
-        <v>36</v>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C50">
         <v>72.835999999999999</v>
@@ -1876,8 +1884,9 @@
       <c r="A51">
         <v>1</v>
       </c>
-      <c r="B51" t="s">
-        <v>35</v>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C51">
         <v>73.036000000000001</v>
@@ -1899,8 +1908,9 @@
       <c r="A52">
         <v>3</v>
       </c>
-      <c r="B52" t="s">
-        <v>36</v>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C52">
         <v>73.036000000000001</v>
@@ -1922,8 +1932,9 @@
       <c r="A53">
         <v>17</v>
       </c>
-      <c r="B53" t="s">
-        <v>50</v>
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C53">
         <v>73.036000000000001</v>
@@ -1945,8 +1956,9 @@
       <c r="A54">
         <v>1</v>
       </c>
-      <c r="B54" t="s">
-        <v>35</v>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C54">
         <v>73.236000000000004</v>
@@ -1968,8 +1980,9 @@
       <c r="A55">
         <v>17</v>
       </c>
-      <c r="B55" t="s">
-        <v>50</v>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C55">
         <v>73.236000000000004</v>
@@ -1991,8 +2004,9 @@
       <c r="A56">
         <v>1</v>
       </c>
-      <c r="B56" t="s">
-        <v>35</v>
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C56">
         <v>73.436000000000007</v>
@@ -2014,8 +2028,9 @@
       <c r="A57">
         <v>17</v>
       </c>
-      <c r="B57" t="s">
-        <v>50</v>
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C57">
         <v>73.436000000000007</v>
@@ -2037,8 +2052,9 @@
       <c r="A58">
         <v>1</v>
       </c>
-      <c r="B58" t="s">
-        <v>35</v>
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C58">
         <v>73.635999999999996</v>
@@ -2060,8 +2076,9 @@
       <c r="A59">
         <v>17</v>
       </c>
-      <c r="B59" t="s">
-        <v>50</v>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C59">
         <v>73.635999999999996</v>
@@ -2083,8 +2100,9 @@
       <c r="A60">
         <v>17</v>
       </c>
-      <c r="B60" t="s">
-        <v>50</v>
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C60">
         <v>73.835999999999999</v>
@@ -2106,8 +2124,9 @@
       <c r="A61">
         <v>1</v>
       </c>
-      <c r="B61" t="s">
-        <v>35</v>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C61">
         <v>74.036000000000001</v>
@@ -2129,8 +2148,9 @@
       <c r="A62">
         <v>17</v>
       </c>
-      <c r="B62" t="s">
-        <v>50</v>
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C62">
         <v>74.036000000000001</v>
@@ -2152,8 +2172,9 @@
       <c r="A63">
         <v>1</v>
       </c>
-      <c r="B63" t="s">
-        <v>35</v>
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C63">
         <v>76.436000000000007</v>
@@ -2175,8 +2196,9 @@
       <c r="A64">
         <v>17</v>
       </c>
-      <c r="B64" t="s">
-        <v>50</v>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C64">
         <v>76.436000000000007</v>
@@ -2198,8 +2220,9 @@
       <c r="A65">
         <v>1</v>
       </c>
-      <c r="B65" t="s">
-        <v>35</v>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C65">
         <v>76.835999999999999</v>
@@ -2221,8 +2244,9 @@
       <c r="A66">
         <v>17</v>
       </c>
-      <c r="B66" t="s">
-        <v>50</v>
+      <c r="B66" t="str">
+        <f t="shared" si="0"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C66">
         <v>76.835999999999999</v>
@@ -2244,8 +2268,9 @@
       <c r="A67">
         <v>1</v>
       </c>
-      <c r="B67" t="s">
-        <v>35</v>
+      <c r="B67" t="str">
+        <f t="shared" ref="B67:B130" si="1">VLOOKUP(A67,$K$1:$L$20,2,FALSE)</f>
+        <v>#63b8ff</v>
       </c>
       <c r="C67">
         <v>77.236000000000004</v>
@@ -2267,8 +2292,9 @@
       <c r="A68">
         <v>17</v>
       </c>
-      <c r="B68" t="s">
-        <v>50</v>
+      <c r="B68" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C68">
         <v>77.236000000000004</v>
@@ -2290,8 +2316,9 @@
       <c r="A69">
         <v>1</v>
       </c>
-      <c r="B69" t="s">
-        <v>35</v>
+      <c r="B69" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C69">
         <v>82.835999999999999</v>
@@ -2313,8 +2340,9 @@
       <c r="A70">
         <v>17</v>
       </c>
-      <c r="B70" t="s">
-        <v>50</v>
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C70">
         <v>82.835999999999999</v>
@@ -2336,8 +2364,9 @@
       <c r="A71">
         <v>1</v>
       </c>
-      <c r="B71" t="s">
-        <v>35</v>
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C71">
         <v>83.236000000000004</v>
@@ -2359,8 +2388,9 @@
       <c r="A72">
         <v>17</v>
       </c>
-      <c r="B72" t="s">
-        <v>50</v>
+      <c r="B72" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C72">
         <v>83.236000000000004</v>
@@ -2382,8 +2412,9 @@
       <c r="A73">
         <v>1</v>
       </c>
-      <c r="B73" t="s">
-        <v>35</v>
+      <c r="B73" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C73">
         <v>83.635999999999996</v>
@@ -2405,8 +2436,9 @@
       <c r="A74">
         <v>17</v>
       </c>
-      <c r="B74" t="s">
-        <v>50</v>
+      <c r="B74" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C74">
         <v>83.635999999999996</v>
@@ -2428,8 +2460,9 @@
       <c r="A75">
         <v>17</v>
       </c>
-      <c r="B75" t="s">
-        <v>50</v>
+      <c r="B75" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C75">
         <v>85.236000000000004</v>
@@ -2451,8 +2484,9 @@
       <c r="A76">
         <v>1</v>
       </c>
-      <c r="B76" t="s">
-        <v>35</v>
+      <c r="B76" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C76">
         <v>86.036000000000001</v>
@@ -2474,8 +2508,9 @@
       <c r="A77">
         <v>17</v>
       </c>
-      <c r="B77" t="s">
-        <v>50</v>
+      <c r="B77" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C77">
         <v>86.036000000000001</v>
@@ -2497,8 +2532,9 @@
       <c r="A78">
         <v>1</v>
       </c>
-      <c r="B78" t="s">
-        <v>35</v>
+      <c r="B78" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C78">
         <v>86.436000000000007</v>
@@ -2520,8 +2556,9 @@
       <c r="A79">
         <v>1</v>
       </c>
-      <c r="B79" t="s">
-        <v>35</v>
+      <c r="B79" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C79">
         <v>86.835999999999999</v>
@@ -2543,8 +2580,9 @@
       <c r="A80">
         <v>17</v>
       </c>
-      <c r="B80" t="s">
-        <v>50</v>
+      <c r="B80" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C80">
         <v>86.436000000000007</v>
@@ -2566,8 +2604,9 @@
       <c r="A81">
         <v>1</v>
       </c>
-      <c r="B81" t="s">
-        <v>35</v>
+      <c r="B81" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C81">
         <v>89.236000000000004</v>
@@ -2589,8 +2628,9 @@
       <c r="A82">
         <v>17</v>
       </c>
-      <c r="B82" t="s">
-        <v>50</v>
+      <c r="B82" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C82">
         <v>89.236000000000004</v>
@@ -2612,8 +2652,9 @@
       <c r="A83">
         <v>1</v>
       </c>
-      <c r="B83" t="s">
-        <v>35</v>
+      <c r="B83" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C83">
         <v>89.635999999999996</v>
@@ -2635,8 +2676,9 @@
       <c r="A84">
         <v>17</v>
       </c>
-      <c r="B84" t="s">
-        <v>50</v>
+      <c r="B84" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C84">
         <v>89.635999999999996</v>
@@ -2658,8 +2700,9 @@
       <c r="A85">
         <v>1</v>
       </c>
-      <c r="B85" t="s">
-        <v>35</v>
+      <c r="B85" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C85">
         <v>90.036000000000001</v>
@@ -2681,8 +2724,9 @@
       <c r="A86">
         <v>17</v>
       </c>
-      <c r="B86" t="s">
-        <v>50</v>
+      <c r="B86" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C86">
         <v>90.036000000000001</v>
@@ -2704,8 +2748,9 @@
       <c r="A87">
         <v>1</v>
       </c>
-      <c r="B87" t="s">
-        <v>35</v>
+      <c r="B87" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C87">
         <v>95.63600000000001</v>
@@ -2727,8 +2772,9 @@
       <c r="A88">
         <v>17</v>
       </c>
-      <c r="B88" t="s">
-        <v>50</v>
+      <c r="B88" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C88">
         <v>95.63600000000001</v>
@@ -2750,8 +2796,9 @@
       <c r="A89">
         <v>1</v>
       </c>
-      <c r="B89" t="s">
-        <v>35</v>
+      <c r="B89" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C89">
         <v>96.036000000000001</v>
@@ -2773,8 +2820,9 @@
       <c r="A90">
         <v>17</v>
       </c>
-      <c r="B90" t="s">
-        <v>50</v>
+      <c r="B90" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C90">
         <v>96.036000000000001</v>
@@ -2796,8 +2844,9 @@
       <c r="A91">
         <v>1</v>
       </c>
-      <c r="B91" t="s">
-        <v>35</v>
+      <c r="B91" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C91">
         <v>96.436000000000007</v>
@@ -2819,8 +2868,9 @@
       <c r="A92">
         <v>17</v>
       </c>
-      <c r="B92" t="s">
-        <v>50</v>
+      <c r="B92" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C92">
         <v>96.436000000000007</v>
@@ -2842,8 +2892,9 @@
       <c r="A93">
         <v>1</v>
       </c>
-      <c r="B93" t="s">
-        <v>35</v>
+      <c r="B93" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C93">
         <v>97.236000000000004</v>
@@ -2865,8 +2916,9 @@
       <c r="A94">
         <v>17</v>
       </c>
-      <c r="B94" t="s">
-        <v>50</v>
+      <c r="B94" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C94">
         <v>97.236000000000004</v>
@@ -2888,8 +2940,9 @@
       <c r="A95">
         <v>1</v>
       </c>
-      <c r="B95" t="s">
-        <v>35</v>
+      <c r="B95" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C95">
         <v>97.536000000000001</v>
@@ -2911,8 +2964,9 @@
       <c r="A96">
         <v>17</v>
       </c>
-      <c r="B96" t="s">
-        <v>50</v>
+      <c r="B96" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C96">
         <v>97.536000000000001</v>
@@ -2934,8 +2988,9 @@
       <c r="A97">
         <v>1</v>
       </c>
-      <c r="B97" t="s">
-        <v>35</v>
+      <c r="B97" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C97">
         <v>97.835999999999999</v>
@@ -2957,8 +3012,9 @@
       <c r="A98">
         <v>17</v>
       </c>
-      <c r="B98" t="s">
-        <v>50</v>
+      <c r="B98" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C98">
         <v>97.835999999999999</v>
@@ -2980,8 +3036,9 @@
       <c r="A99">
         <v>1</v>
       </c>
-      <c r="B99" t="s">
-        <v>35</v>
+      <c r="B99" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C99">
         <v>98.135999999999996</v>
@@ -3003,8 +3060,9 @@
       <c r="A100">
         <v>17</v>
       </c>
-      <c r="B100" t="s">
-        <v>50</v>
+      <c r="B100" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C100">
         <v>98.135999999999996</v>
@@ -3026,8 +3084,9 @@
       <c r="A101">
         <v>1</v>
       </c>
-      <c r="B101" t="s">
-        <v>35</v>
+      <c r="B101" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C101">
         <v>98.835999999999999</v>
@@ -3049,8 +3108,9 @@
       <c r="A102">
         <v>1</v>
       </c>
-      <c r="B102" t="s">
-        <v>35</v>
+      <c r="B102" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C102">
         <v>99.034999999999997</v>
@@ -3072,8 +3132,9 @@
       <c r="A103">
         <v>1</v>
       </c>
-      <c r="B103" t="s">
-        <v>35</v>
+      <c r="B103" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C103">
         <v>99.036000000000001</v>
@@ -3095,8 +3156,9 @@
       <c r="A104">
         <v>1</v>
       </c>
-      <c r="B104" t="s">
-        <v>35</v>
+      <c r="B104" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C104">
         <v>99.234999999999999</v>
@@ -3118,8 +3180,9 @@
       <c r="A105">
         <v>1</v>
       </c>
-      <c r="B105" t="s">
-        <v>35</v>
+      <c r="B105" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C105">
         <v>99.236000000000004</v>
@@ -3141,8 +3204,9 @@
       <c r="A106">
         <v>1</v>
       </c>
-      <c r="B106" t="s">
-        <v>35</v>
+      <c r="B106" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C106">
         <v>99.435000000000002</v>
@@ -3164,8 +3228,9 @@
       <c r="A107">
         <v>1</v>
       </c>
-      <c r="B107" t="s">
-        <v>35</v>
+      <c r="B107" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C107">
         <v>99.436000000000007</v>
@@ -3187,8 +3252,9 @@
       <c r="A108">
         <v>17</v>
       </c>
-      <c r="B108" t="s">
-        <v>50</v>
+      <c r="B108" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C108">
         <v>98.835999999999999</v>
@@ -3210,8 +3276,9 @@
       <c r="A109">
         <v>1</v>
       </c>
-      <c r="B109" t="s">
-        <v>35</v>
+      <c r="B109" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C109">
         <v>99.635999999999996</v>
@@ -3233,8 +3300,9 @@
       <c r="A110">
         <v>17</v>
       </c>
-      <c r="B110" t="s">
-        <v>50</v>
+      <c r="B110" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C110">
         <v>99.635999999999996</v>
@@ -3256,8 +3324,9 @@
       <c r="A111">
         <v>1</v>
       </c>
-      <c r="B111" t="s">
-        <v>35</v>
+      <c r="B111" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C111">
         <v>99.736000000000004</v>
@@ -3279,8 +3348,9 @@
       <c r="A112">
         <v>17</v>
       </c>
-      <c r="B112" t="s">
-        <v>50</v>
+      <c r="B112" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C112">
         <v>99.736000000000004</v>
@@ -3302,8 +3372,9 @@
       <c r="A113">
         <v>17</v>
       </c>
-      <c r="B113" t="s">
-        <v>50</v>
+      <c r="B113" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C113">
         <v>108.43600000000001</v>
@@ -3325,8 +3396,9 @@
       <c r="A114">
         <v>1</v>
       </c>
-      <c r="B114" t="s">
-        <v>35</v>
+      <c r="B114" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C114">
         <v>109.236</v>
@@ -3348,8 +3420,9 @@
       <c r="A115">
         <v>1</v>
       </c>
-      <c r="B115" t="s">
-        <v>35</v>
+      <c r="B115" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C115">
         <v>109.336</v>
@@ -3371,8 +3444,9 @@
       <c r="A116">
         <v>17</v>
       </c>
-      <c r="B116" t="s">
-        <v>50</v>
+      <c r="B116" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C116">
         <v>109.236</v>
@@ -3394,8 +3468,9 @@
       <c r="A117">
         <v>17</v>
       </c>
-      <c r="B117" t="s">
-        <v>50</v>
+      <c r="B117" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C117">
         <v>110.83600000000001</v>
@@ -3417,8 +3492,9 @@
       <c r="A118">
         <v>1</v>
       </c>
-      <c r="B118" t="s">
-        <v>35</v>
+      <c r="B118" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C118">
         <v>111.636</v>
@@ -3440,8 +3516,9 @@
       <c r="A119">
         <v>17</v>
       </c>
-      <c r="B119" t="s">
-        <v>50</v>
+      <c r="B119" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C119">
         <v>111.636</v>
@@ -3463,8 +3540,9 @@
       <c r="A120">
         <v>1</v>
       </c>
-      <c r="B120" t="s">
-        <v>35</v>
+      <c r="B120" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C120">
         <v>112.036</v>
@@ -3486,8 +3564,9 @@
       <c r="A121">
         <v>1</v>
       </c>
-      <c r="B121" t="s">
-        <v>35</v>
+      <c r="B121" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C121">
         <v>112.43600000000001</v>
@@ -3509,8 +3588,9 @@
       <c r="A122">
         <v>17</v>
       </c>
-      <c r="B122" t="s">
-        <v>50</v>
+      <c r="B122" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C122">
         <v>112.036</v>
@@ -3532,8 +3612,9 @@
       <c r="A123">
         <v>1</v>
       </c>
-      <c r="B123" t="s">
-        <v>35</v>
+      <c r="B123" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C123">
         <v>121.236</v>
@@ -3555,8 +3636,9 @@
       <c r="A124">
         <v>1</v>
       </c>
-      <c r="B124" t="s">
-        <v>35</v>
+      <c r="B124" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C124">
         <v>122.036</v>
@@ -3578,8 +3660,9 @@
       <c r="A125">
         <v>1</v>
       </c>
-      <c r="B125" t="s">
-        <v>35</v>
+      <c r="B125" t="str">
+        <f t="shared" si="1"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C125">
         <v>122.43600000000001</v>
@@ -3601,8 +3684,9 @@
       <c r="A126">
         <v>17</v>
       </c>
-      <c r="B126" t="s">
-        <v>50</v>
+      <c r="B126" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C126">
         <v>123.652</v>
@@ -3624,8 +3708,9 @@
       <c r="A127">
         <v>17</v>
       </c>
-      <c r="B127" t="s">
-        <v>50</v>
+      <c r="B127" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C127">
         <v>125.152</v>
@@ -3647,8 +3732,9 @@
       <c r="A128">
         <v>17</v>
       </c>
-      <c r="B128" t="s">
-        <v>50</v>
+      <c r="B128" t="str">
+        <f t="shared" si="1"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C128">
         <v>125.97199999999999</v>
@@ -3670,8 +3756,9 @@
       <c r="A129">
         <v>18</v>
       </c>
-      <c r="B129" t="s">
-        <v>51</v>
+      <c r="B129" t="str">
+        <f t="shared" si="1"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C129">
         <v>125.152</v>
@@ -3693,8 +3780,9 @@
       <c r="A130">
         <v>18</v>
       </c>
-      <c r="B130" t="s">
-        <v>51</v>
+      <c r="B130" t="str">
+        <f t="shared" si="1"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C130">
         <v>125.97199999999999</v>
@@ -3716,8 +3804,9 @@
       <c r="A131">
         <v>17</v>
       </c>
-      <c r="B131" t="s">
-        <v>50</v>
+      <c r="B131" t="str">
+        <f t="shared" ref="B131:B194" si="2">VLOOKUP(A131,$K$1:$L$20,2,FALSE)</f>
+        <v>#8ee5ee</v>
       </c>
       <c r="C131">
         <v>128.447</v>
@@ -3739,8 +3828,9 @@
       <c r="A132">
         <v>17</v>
       </c>
-      <c r="B132" t="s">
-        <v>50</v>
+      <c r="B132" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C132">
         <v>129.267</v>
@@ -3762,8 +3852,9 @@
       <c r="A133">
         <v>18</v>
       </c>
-      <c r="B133" t="s">
-        <v>51</v>
+      <c r="B133" t="str">
+        <f t="shared" si="2"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C133">
         <v>128.447</v>
@@ -3785,8 +3876,9 @@
       <c r="A134">
         <v>18</v>
       </c>
-      <c r="B134" t="s">
-        <v>51</v>
+      <c r="B134" t="str">
+        <f t="shared" si="2"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C134">
         <v>129.267</v>
@@ -3808,8 +3900,9 @@
       <c r="A135">
         <v>17</v>
       </c>
-      <c r="B135" t="s">
-        <v>50</v>
+      <c r="B135" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C135">
         <v>131.637</v>
@@ -3831,8 +3924,9 @@
       <c r="A136">
         <v>17</v>
       </c>
-      <c r="B136" t="s">
-        <v>50</v>
+      <c r="B136" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C136">
         <v>132.45699999999999</v>
@@ -3854,8 +3948,9 @@
       <c r="A137">
         <v>18</v>
       </c>
-      <c r="B137" t="s">
-        <v>51</v>
+      <c r="B137" t="str">
+        <f t="shared" si="2"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C137">
         <v>131.637</v>
@@ -3877,8 +3972,9 @@
       <c r="A138">
         <v>18</v>
       </c>
-      <c r="B138" t="s">
-        <v>51</v>
+      <c r="B138" t="str">
+        <f t="shared" si="2"/>
+        <v>#dda0dd</v>
       </c>
       <c r="C138">
         <v>132.45699999999999</v>
@@ -3900,8 +3996,9 @@
       <c r="A139">
         <v>17</v>
       </c>
-      <c r="B139" t="s">
-        <v>50</v>
+      <c r="B139" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C139">
         <v>134.83600000000001</v>
@@ -3923,8 +4020,9 @@
       <c r="A140">
         <v>17</v>
       </c>
-      <c r="B140" t="s">
-        <v>50</v>
+      <c r="B140" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C140">
         <v>135.43600000000004</v>
@@ -3946,8 +4044,9 @@
       <c r="A141">
         <v>17</v>
       </c>
-      <c r="B141" t="s">
-        <v>50</v>
+      <c r="B141" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C141">
         <v>136.03600000000006</v>
@@ -3969,8 +4068,9 @@
       <c r="A142">
         <v>1</v>
       </c>
-      <c r="B142" t="s">
-        <v>35</v>
+      <c r="B142" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C142">
         <v>137.636</v>
@@ -3992,8 +4092,9 @@
       <c r="A143">
         <v>1</v>
       </c>
-      <c r="B143" t="s">
-        <v>35</v>
+      <c r="B143" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C143">
         <v>138.036</v>
@@ -4015,8 +4116,9 @@
       <c r="A144">
         <v>1</v>
       </c>
-      <c r="B144" t="s">
-        <v>35</v>
+      <c r="B144" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C144">
         <v>138.23599999999999</v>
@@ -4038,8 +4140,9 @@
       <c r="A145">
         <v>1</v>
       </c>
-      <c r="B145" t="s">
-        <v>35</v>
+      <c r="B145" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C145">
         <v>138.636</v>
@@ -4061,8 +4164,9 @@
       <c r="A146">
         <v>17</v>
       </c>
-      <c r="B146" t="s">
-        <v>50</v>
+      <c r="B146" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C146">
         <v>141.23599999999999</v>
@@ -4084,8 +4188,9 @@
       <c r="A147">
         <v>1</v>
       </c>
-      <c r="B147" t="s">
-        <v>35</v>
+      <c r="B147" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C147">
         <v>141.23599999999999</v>
@@ -4107,8 +4212,9 @@
       <c r="A148">
         <v>17</v>
       </c>
-      <c r="B148" t="s">
-        <v>50</v>
+      <c r="B148" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C148">
         <v>141.636</v>
@@ -4130,8 +4236,9 @@
       <c r="A149">
         <v>1</v>
       </c>
-      <c r="B149" t="s">
-        <v>35</v>
+      <c r="B149" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C149">
         <v>141.636</v>
@@ -4153,8 +4260,9 @@
       <c r="A150">
         <v>1</v>
       </c>
-      <c r="B150" t="s">
-        <v>35</v>
+      <c r="B150" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C150">
         <v>151.036</v>
@@ -4176,8 +4284,9 @@
       <c r="A151">
         <v>1</v>
       </c>
-      <c r="B151" t="s">
-        <v>35</v>
+      <c r="B151" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C151">
         <v>151.43600000000001</v>
@@ -4199,8 +4308,9 @@
       <c r="A152">
         <v>1</v>
       </c>
-      <c r="B152" t="s">
-        <v>35</v>
+      <c r="B152" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C152">
         <v>152.036</v>
@@ -4222,8 +4332,9 @@
       <c r="A153">
         <v>1</v>
       </c>
-      <c r="B153" t="s">
-        <v>35</v>
+      <c r="B153" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C153">
         <v>152.23599999999999</v>
@@ -4245,8 +4356,9 @@
       <c r="A154">
         <v>17</v>
       </c>
-      <c r="B154" t="s">
-        <v>50</v>
+      <c r="B154" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C154">
         <v>151.036</v>
@@ -4268,8 +4380,9 @@
       <c r="A155">
         <v>17</v>
       </c>
-      <c r="B155" t="s">
-        <v>50</v>
+      <c r="B155" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C155">
         <v>151.43600000000001</v>
@@ -4291,8 +4404,9 @@
       <c r="A156">
         <v>17</v>
       </c>
-      <c r="B156" t="s">
-        <v>50</v>
+      <c r="B156" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C156">
         <v>152.036</v>
@@ -4314,8 +4428,9 @@
       <c r="A157">
         <v>17</v>
       </c>
-      <c r="B157" t="s">
-        <v>50</v>
+      <c r="B157" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C157">
         <v>152.23599999999999</v>
@@ -4337,8 +4452,9 @@
       <c r="A158">
         <v>1</v>
       </c>
-      <c r="B158" t="s">
-        <v>35</v>
+      <c r="B158" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C158">
         <v>161.636</v>
@@ -4360,8 +4476,9 @@
       <c r="A159">
         <v>1</v>
       </c>
-      <c r="B159" t="s">
-        <v>35</v>
+      <c r="B159" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C159">
         <v>161.83600000000001</v>
@@ -4383,8 +4500,9 @@
       <c r="A160">
         <v>1</v>
       </c>
-      <c r="B160" t="s">
-        <v>35</v>
+      <c r="B160" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C160">
         <v>163.636</v>
@@ -4406,8 +4524,9 @@
       <c r="A161">
         <v>1</v>
       </c>
-      <c r="B161" t="s">
-        <v>35</v>
+      <c r="B161" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C161">
         <v>168.43600000000001</v>
@@ -4429,8 +4548,9 @@
       <c r="A162">
         <v>1</v>
       </c>
-      <c r="B162" t="s">
-        <v>35</v>
+      <c r="B162" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C162">
         <v>170.036</v>
@@ -4452,8 +4572,9 @@
       <c r="A163">
         <v>1</v>
       </c>
-      <c r="B163" t="s">
-        <v>35</v>
+      <c r="B163" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C163">
         <v>172.83600000000001</v>
@@ -4475,8 +4596,9 @@
       <c r="A164">
         <v>1</v>
       </c>
-      <c r="B164" t="s">
-        <v>35</v>
+      <c r="B164" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C164">
         <v>173.23599999999999</v>
@@ -4498,8 +4620,9 @@
       <c r="A165">
         <v>17</v>
       </c>
-      <c r="B165" t="s">
-        <v>50</v>
+      <c r="B165" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C165">
         <v>187.83600000000001</v>
@@ -4521,8 +4644,9 @@
       <c r="A166">
         <v>1</v>
       </c>
-      <c r="B166" t="s">
-        <v>35</v>
+      <c r="B166" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C166">
         <v>187.83600000000001</v>
@@ -4544,8 +4668,9 @@
       <c r="A167">
         <v>17</v>
       </c>
-      <c r="B167" t="s">
-        <v>50</v>
+      <c r="B167" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C167">
         <v>188.036</v>
@@ -4567,8 +4692,9 @@
       <c r="A168">
         <v>1</v>
       </c>
-      <c r="B168" t="s">
-        <v>35</v>
+      <c r="B168" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C168">
         <v>188.036</v>
@@ -4590,8 +4716,9 @@
       <c r="A169">
         <v>17</v>
       </c>
-      <c r="B169" t="s">
-        <v>50</v>
+      <c r="B169" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C169">
         <v>188.23599999999999</v>
@@ -4613,8 +4740,9 @@
       <c r="A170">
         <v>1</v>
       </c>
-      <c r="B170" t="s">
-        <v>35</v>
+      <c r="B170" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C170">
         <v>188.23599999999999</v>
@@ -4636,8 +4764,9 @@
       <c r="A171">
         <v>19</v>
       </c>
-      <c r="B171" t="s">
-        <v>35</v>
+      <c r="B171" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C171">
         <v>188.23599999999999</v>
@@ -4659,8 +4788,9 @@
       <c r="A172">
         <v>17</v>
       </c>
-      <c r="B172" t="s">
-        <v>50</v>
+      <c r="B172" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C172">
         <v>188.43600000000001</v>
@@ -4682,8 +4812,9 @@
       <c r="A173">
         <v>19</v>
       </c>
-      <c r="B173" t="s">
-        <v>35</v>
+      <c r="B173" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C173">
         <v>188.43600000000001</v>
@@ -4705,8 +4836,9 @@
       <c r="A174">
         <v>17</v>
       </c>
-      <c r="B174" t="s">
-        <v>50</v>
+      <c r="B174" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C174">
         <v>188.63600000000002</v>
@@ -4728,8 +4860,9 @@
       <c r="A175">
         <v>19</v>
       </c>
-      <c r="B175" t="s">
-        <v>35</v>
+      <c r="B175" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C175">
         <v>188.63600000000002</v>
@@ -4751,8 +4884,9 @@
       <c r="A176">
         <v>17</v>
       </c>
-      <c r="B176" t="s">
-        <v>50</v>
+      <c r="B176" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C176">
         <v>188.83600000000001</v>
@@ -4774,8 +4908,9 @@
       <c r="A177">
         <v>19</v>
       </c>
-      <c r="B177" t="s">
-        <v>35</v>
+      <c r="B177" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C177">
         <v>188.83600000000001</v>
@@ -4797,8 +4932,9 @@
       <c r="A178">
         <v>19</v>
       </c>
-      <c r="B178" t="s">
-        <v>35</v>
+      <c r="B178" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C178">
         <v>189.036</v>
@@ -4820,8 +4956,9 @@
       <c r="A179">
         <v>17</v>
       </c>
-      <c r="B179" t="s">
-        <v>50</v>
+      <c r="B179" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C179">
         <v>189.23599999999999</v>
@@ -4843,8 +4980,9 @@
       <c r="A180">
         <v>19</v>
       </c>
-      <c r="B180" t="s">
-        <v>35</v>
+      <c r="B180" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C180">
         <v>189.23599999999999</v>
@@ -4866,8 +5004,9 @@
       <c r="A181">
         <v>17</v>
       </c>
-      <c r="B181" t="s">
-        <v>50</v>
+      <c r="B181" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C181">
         <v>194.83600000000001</v>
@@ -4889,8 +5028,9 @@
       <c r="A182">
         <v>19</v>
       </c>
-      <c r="B182" t="s">
-        <v>35</v>
+      <c r="B182" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C182">
         <v>194.83600000000001</v>
@@ -4912,8 +5052,9 @@
       <c r="A183">
         <v>17</v>
       </c>
-      <c r="B183" t="s">
-        <v>50</v>
+      <c r="B183" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C183">
         <v>195.136</v>
@@ -4935,8 +5076,9 @@
       <c r="A184">
         <v>19</v>
       </c>
-      <c r="B184" t="s">
-        <v>35</v>
+      <c r="B184" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C184">
         <v>195.136</v>
@@ -4958,8 +5100,9 @@
       <c r="A185">
         <v>17</v>
       </c>
-      <c r="B185" t="s">
-        <v>50</v>
+      <c r="B185" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C185">
         <v>195.43600000000001</v>
@@ -4981,8 +5124,9 @@
       <c r="A186">
         <v>19</v>
       </c>
-      <c r="B186" t="s">
-        <v>35</v>
+      <c r="B186" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C186">
         <v>195.43600000000001</v>
@@ -5004,8 +5148,9 @@
       <c r="A187">
         <v>17</v>
       </c>
-      <c r="B187" t="s">
-        <v>50</v>
+      <c r="B187" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C187">
         <v>195.636</v>
@@ -5027,8 +5172,9 @@
       <c r="A188">
         <v>19</v>
       </c>
-      <c r="B188" t="s">
-        <v>35</v>
+      <c r="B188" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C188">
         <v>195.636</v>
@@ -5050,8 +5196,9 @@
       <c r="A189">
         <v>17</v>
       </c>
-      <c r="B189" t="s">
-        <v>50</v>
+      <c r="B189" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C189">
         <v>195.93600000000001</v>
@@ -5073,8 +5220,9 @@
       <c r="A190">
         <v>19</v>
       </c>
-      <c r="B190" t="s">
-        <v>35</v>
+      <c r="B190" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C190">
         <v>195.93600000000001</v>
@@ -5096,8 +5244,9 @@
       <c r="A191">
         <v>17</v>
       </c>
-      <c r="B191" t="s">
-        <v>50</v>
+      <c r="B191" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C191">
         <v>196.23599999999999</v>
@@ -5119,8 +5268,9 @@
       <c r="A192">
         <v>19</v>
       </c>
-      <c r="B192" t="s">
-        <v>35</v>
+      <c r="B192" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C192">
         <v>196.23599999999999</v>
@@ -5142,8 +5292,9 @@
       <c r="A193">
         <v>17</v>
       </c>
-      <c r="B193" t="s">
-        <v>50</v>
+      <c r="B193" t="str">
+        <f t="shared" si="2"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C193">
         <v>196.43600000000001</v>
@@ -5165,8 +5316,9 @@
       <c r="A194">
         <v>19</v>
       </c>
-      <c r="B194" t="s">
-        <v>35</v>
+      <c r="B194" t="str">
+        <f t="shared" si="2"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C194">
         <v>196.43600000000001</v>
@@ -5188,8 +5340,9 @@
       <c r="A195">
         <v>17</v>
       </c>
-      <c r="B195" t="s">
-        <v>50</v>
+      <c r="B195" t="str">
+        <f t="shared" ref="B195:B240" si="3">VLOOKUP(A195,$K$1:$L$20,2,FALSE)</f>
+        <v>#8ee5ee</v>
       </c>
       <c r="C195">
         <v>200.23599999999999</v>
@@ -5211,8 +5364,9 @@
       <c r="A196">
         <v>17</v>
       </c>
-      <c r="B196" t="s">
-        <v>50</v>
+      <c r="B196" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C196">
         <v>200.83600000000001</v>
@@ -5234,8 +5388,9 @@
       <c r="A197">
         <v>19</v>
       </c>
-      <c r="B197" t="s">
-        <v>35</v>
+      <c r="B197" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C197">
         <v>201.636</v>
@@ -5257,8 +5412,9 @@
       <c r="A198">
         <v>19</v>
       </c>
-      <c r="B198" t="s">
-        <v>35</v>
+      <c r="B198" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C198">
         <v>201.73599999999999</v>
@@ -5280,8 +5436,9 @@
       <c r="A199">
         <v>17</v>
       </c>
-      <c r="B199" t="s">
-        <v>50</v>
+      <c r="B199" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C199">
         <v>207.63600000000002</v>
@@ -5303,8 +5460,9 @@
       <c r="A200">
         <v>19</v>
       </c>
-      <c r="B200" t="s">
-        <v>35</v>
+      <c r="B200" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C200">
         <v>207.63600000000002</v>
@@ -5326,8 +5484,9 @@
       <c r="A201">
         <v>17</v>
       </c>
-      <c r="B201" t="s">
-        <v>50</v>
+      <c r="B201" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C201">
         <v>207.93600000000001</v>
@@ -5349,8 +5508,9 @@
       <c r="A202">
         <v>19</v>
       </c>
-      <c r="B202" t="s">
-        <v>35</v>
+      <c r="B202" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C202">
         <v>207.93600000000001</v>
@@ -5372,8 +5532,9 @@
       <c r="A203">
         <v>17</v>
       </c>
-      <c r="B203" t="s">
-        <v>50</v>
+      <c r="B203" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C203">
         <v>208.23600000000002</v>
@@ -5395,8 +5556,9 @@
       <c r="A204">
         <v>19</v>
       </c>
-      <c r="B204" t="s">
-        <v>35</v>
+      <c r="B204" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C204">
         <v>208.23600000000002</v>
@@ -5418,8 +5580,9 @@
       <c r="A205">
         <v>17</v>
       </c>
-      <c r="B205" t="s">
-        <v>50</v>
+      <c r="B205" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C205">
         <v>208.43600000000001</v>
@@ -5441,8 +5604,9 @@
       <c r="A206">
         <v>19</v>
       </c>
-      <c r="B206" t="s">
-        <v>35</v>
+      <c r="B206" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C206">
         <v>208.43600000000001</v>
@@ -5464,8 +5628,9 @@
       <c r="A207">
         <v>17</v>
       </c>
-      <c r="B207" t="s">
-        <v>50</v>
+      <c r="B207" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C207">
         <v>208.73600000000002</v>
@@ -5487,8 +5652,9 @@
       <c r="A208">
         <v>19</v>
       </c>
-      <c r="B208" t="s">
-        <v>35</v>
+      <c r="B208" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C208">
         <v>208.73600000000002</v>
@@ -5510,8 +5676,9 @@
       <c r="A209">
         <v>17</v>
       </c>
-      <c r="B209" t="s">
-        <v>50</v>
+      <c r="B209" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C209">
         <v>209.036</v>
@@ -5533,8 +5700,9 @@
       <c r="A210">
         <v>19</v>
       </c>
-      <c r="B210" t="s">
-        <v>35</v>
+      <c r="B210" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C210">
         <v>209.036</v>
@@ -5556,8 +5724,9 @@
       <c r="A211">
         <v>17</v>
       </c>
-      <c r="B211" t="s">
-        <v>50</v>
+      <c r="B211" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C211">
         <v>209.23600000000002</v>
@@ -5579,8 +5748,9 @@
       <c r="A212">
         <v>19</v>
       </c>
-      <c r="B212" t="s">
-        <v>35</v>
+      <c r="B212" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C212">
         <v>209.23600000000002</v>
@@ -5602,8 +5772,9 @@
       <c r="A213">
         <v>17</v>
       </c>
-      <c r="B213" t="s">
-        <v>50</v>
+      <c r="B213" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C213">
         <v>219.23599999999999</v>
@@ -5625,8 +5796,9 @@
       <c r="A214">
         <v>19</v>
       </c>
-      <c r="B214" t="s">
-        <v>35</v>
+      <c r="B214" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C214">
         <v>219.23599999999999</v>
@@ -5648,8 +5820,9 @@
       <c r="A215">
         <v>17</v>
       </c>
-      <c r="B215" t="s">
-        <v>50</v>
+      <c r="B215" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C215">
         <v>219.536</v>
@@ -5671,8 +5844,9 @@
       <c r="A216">
         <v>19</v>
       </c>
-      <c r="B216" t="s">
-        <v>35</v>
+      <c r="B216" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C216">
         <v>219.536</v>
@@ -5694,8 +5868,9 @@
       <c r="A217">
         <v>17</v>
       </c>
-      <c r="B217" t="s">
-        <v>50</v>
+      <c r="B217" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C217">
         <v>219.83600000000001</v>
@@ -5717,8 +5892,9 @@
       <c r="A218">
         <v>19</v>
       </c>
-      <c r="B218" t="s">
-        <v>35</v>
+      <c r="B218" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C218">
         <v>219.83600000000001</v>
@@ -5740,8 +5916,9 @@
       <c r="A219">
         <v>17</v>
       </c>
-      <c r="B219" t="s">
-        <v>50</v>
+      <c r="B219" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C219">
         <v>220.136</v>
@@ -5763,8 +5940,9 @@
       <c r="A220">
         <v>19</v>
       </c>
-      <c r="B220" t="s">
-        <v>35</v>
+      <c r="B220" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C220">
         <v>220.136</v>
@@ -5786,8 +5964,9 @@
       <c r="A221">
         <v>17</v>
       </c>
-      <c r="B221" t="s">
-        <v>50</v>
+      <c r="B221" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C221">
         <v>220.43600000000001</v>
@@ -5809,8 +5988,9 @@
       <c r="A222">
         <v>19</v>
       </c>
-      <c r="B222" t="s">
-        <v>35</v>
+      <c r="B222" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C222">
         <v>220.43600000000001</v>
@@ -5832,8 +6012,9 @@
       <c r="A223">
         <v>17</v>
       </c>
-      <c r="B223" t="s">
-        <v>50</v>
+      <c r="B223" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C223">
         <v>232.036</v>
@@ -5855,8 +6036,9 @@
       <c r="A224">
         <v>19</v>
       </c>
-      <c r="B224" t="s">
-        <v>35</v>
+      <c r="B224" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C224">
         <v>232.036</v>
@@ -5878,8 +6060,9 @@
       <c r="A225">
         <v>17</v>
       </c>
-      <c r="B225" t="s">
-        <v>50</v>
+      <c r="B225" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C225">
         <v>232.33600000000001</v>
@@ -5901,8 +6084,9 @@
       <c r="A226">
         <v>19</v>
       </c>
-      <c r="B226" t="s">
-        <v>35</v>
+      <c r="B226" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C226">
         <v>232.33600000000001</v>
@@ -5924,8 +6108,9 @@
       <c r="A227">
         <v>17</v>
       </c>
-      <c r="B227" t="s">
-        <v>50</v>
+      <c r="B227" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C227">
         <v>232.63600000000002</v>
@@ -5947,8 +6132,9 @@
       <c r="A228">
         <v>19</v>
       </c>
-      <c r="B228" t="s">
-        <v>35</v>
+      <c r="B228" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C228">
         <v>232.63600000000002</v>
@@ -5970,8 +6156,9 @@
       <c r="A229">
         <v>17</v>
       </c>
-      <c r="B229" t="s">
-        <v>50</v>
+      <c r="B229" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C229">
         <v>232.93600000000001</v>
@@ -5993,8 +6180,9 @@
       <c r="A230">
         <v>19</v>
       </c>
-      <c r="B230" t="s">
-        <v>35</v>
+      <c r="B230" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C230">
         <v>232.93600000000001</v>
@@ -6016,8 +6204,9 @@
       <c r="A231">
         <v>17</v>
       </c>
-      <c r="B231" t="s">
-        <v>50</v>
+      <c r="B231" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C231">
         <v>233.23600000000002</v>
@@ -6039,8 +6228,9 @@
       <c r="A232">
         <v>19</v>
       </c>
-      <c r="B232" t="s">
-        <v>35</v>
+      <c r="B232" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C232">
         <v>233.23600000000002</v>
@@ -6062,8 +6252,9 @@
       <c r="A233">
         <v>17</v>
       </c>
-      <c r="B233" t="s">
-        <v>50</v>
+      <c r="B233" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C233">
         <v>238.43600000000001</v>
@@ -6085,8 +6276,9 @@
       <c r="A234">
         <v>19</v>
       </c>
-      <c r="B234" t="s">
-        <v>35</v>
+      <c r="B234" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C234">
         <v>238.43600000000001</v>
@@ -6108,8 +6300,9 @@
       <c r="A235">
         <v>17</v>
       </c>
-      <c r="B235" t="s">
-        <v>50</v>
+      <c r="B235" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C235">
         <v>238.83600000000001</v>
@@ -6131,8 +6324,9 @@
       <c r="A236">
         <v>19</v>
       </c>
-      <c r="B236" t="s">
-        <v>35</v>
+      <c r="B236" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C236">
         <v>238.83600000000001</v>
@@ -6154,8 +6348,9 @@
       <c r="A237">
         <v>17</v>
       </c>
-      <c r="B237" t="s">
-        <v>50</v>
+      <c r="B237" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C237">
         <v>240.43600000000001</v>
@@ -6177,8 +6372,9 @@
       <c r="A238">
         <v>19</v>
       </c>
-      <c r="B238" t="s">
-        <v>35</v>
+      <c r="B238" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C238">
         <v>240.43600000000001</v>
@@ -6200,8 +6396,9 @@
       <c r="A239">
         <v>17</v>
       </c>
-      <c r="B239" t="s">
-        <v>50</v>
+      <c r="B239" t="str">
+        <f t="shared" si="3"/>
+        <v>#8ee5ee</v>
       </c>
       <c r="C239">
         <v>245.23599999999999</v>
@@ -6223,8 +6420,9 @@
       <c r="A240">
         <v>19</v>
       </c>
-      <c r="B240" t="s">
-        <v>35</v>
+      <c r="B240" t="str">
+        <f t="shared" si="3"/>
+        <v>#63b8ff</v>
       </c>
       <c r="C240">
         <v>245.23599999999999</v>

</xml_diff>

<commit_message>
A new version, which looks pretty fine as a demo...
</commit_message>
<xml_diff>
--- a/Assets/Scripts/Chart示例.xlsx
+++ b/Assets/Scripts/Chart示例.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Xenody-master\Assets\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD581C71-1D6E-4017-9131-683A265F9B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E9E021-61A1-412C-A8B2-97F08DF8F785}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{733D2C9F-C334-4499-8550-BE8F5C9E8DF7}"/>
   </bookViews>
   <sheets>
     <sheet name="planes" sheetId="1" r:id="rId1"/>
@@ -555,8 +555,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L240"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6452,8 +6452,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D1026"/>
   <sheetViews>
-    <sheetView topLeftCell="A430" workbookViewId="0">
-      <selection activeCell="K496" sqref="K496"/>
+    <sheetView topLeftCell="A140" workbookViewId="0">
+      <selection activeCell="F620" sqref="F620"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -15073,7 +15073,7 @@
         <v>161.83600000000001</v>
       </c>
       <c r="B616">
-        <v>-1.6</v>
+        <v>-1.2</v>
       </c>
       <c r="C616">
         <v>0.8</v>
@@ -31666,10 +31666,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C76DC57-EF49-44CE-8A21-D4353938F627}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:D317"/>
+  <dimension ref="A1:D316"/>
   <sheetViews>
-    <sheetView topLeftCell="A221" workbookViewId="0">
-      <selection activeCell="F249" sqref="F249"/>
+    <sheetView topLeftCell="A182" workbookViewId="0">
+      <selection activeCell="J197" sqref="J197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -34350,13 +34350,13 @@
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192">
-        <v>116.336</v>
+        <v>115.836</v>
       </c>
       <c r="B192">
         <v>0</v>
       </c>
       <c r="C192">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="D192">
         <v>1</v>
@@ -34364,13 +34364,13 @@
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193">
-        <v>115.836</v>
+        <v>115.886</v>
       </c>
       <c r="B193">
-        <v>0</v>
+        <v>-0.6</v>
       </c>
       <c r="C193">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="D193">
         <v>1</v>
@@ -34378,13 +34378,13 @@
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194">
-        <v>115.886</v>
+        <v>115.93599999999999</v>
       </c>
       <c r="B194">
-        <v>-0.6</v>
+        <v>-1.4</v>
       </c>
       <c r="C194">
-        <v>0.9</v>
+        <v>1.2</v>
       </c>
       <c r="D194">
         <v>1</v>
@@ -34392,13 +34392,13 @@
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195">
-        <v>115.93599999999999</v>
+        <v>116.236</v>
       </c>
       <c r="B195">
-        <v>-1.4</v>
+        <v>1.5</v>
       </c>
       <c r="C195">
-        <v>1.2</v>
+        <v>0.6</v>
       </c>
       <c r="D195">
         <v>1</v>
@@ -34406,13 +34406,13 @@
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196">
-        <v>116.236</v>
+        <v>116.286</v>
       </c>
       <c r="B196">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="C196">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="D196">
         <v>1</v>
@@ -34420,13 +34420,13 @@
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197">
-        <v>116.286</v>
+        <v>116.336</v>
       </c>
       <c r="B197">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C197">
-        <v>0.9</v>
+        <v>1.2</v>
       </c>
       <c r="D197">
         <v>1</v>
@@ -34434,13 +34434,13 @@
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198">
-        <v>116.336</v>
+        <v>123.036</v>
       </c>
       <c r="B198">
-        <v>0</v>
+        <v>-1.5</v>
       </c>
       <c r="C198">
-        <v>1.2</v>
+        <v>0.8</v>
       </c>
       <c r="D198">
         <v>1</v>
@@ -34448,13 +34448,13 @@
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199">
-        <v>123.036</v>
+        <v>123.11583333333334</v>
       </c>
       <c r="B199">
-        <v>-1.5</v>
+        <v>-1.1625000000000001</v>
       </c>
       <c r="C199">
-        <v>0.8</v>
+        <v>0.76250000000000007</v>
       </c>
       <c r="D199">
         <v>1</v>
@@ -34462,13 +34462,13 @@
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200">
-        <v>123.11583333333334</v>
+        <v>123.19566666666667</v>
       </c>
       <c r="B200">
-        <v>-1.1625000000000001</v>
+        <v>-0.82499999999999996</v>
       </c>
       <c r="C200">
-        <v>0.76250000000000007</v>
+        <v>0.72500000000000009</v>
       </c>
       <c r="D200">
         <v>1</v>
@@ -34476,13 +34476,13 @@
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201">
-        <v>123.19566666666667</v>
+        <v>123.27549999999999</v>
       </c>
       <c r="B201">
-        <v>-0.82499999999999996</v>
+        <v>-0.48749999999999982</v>
       </c>
       <c r="C201">
-        <v>0.72500000000000009</v>
+        <v>0.6875</v>
       </c>
       <c r="D201">
         <v>1</v>
@@ -34490,13 +34490,13 @@
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202">
-        <v>123.27549999999999</v>
+        <v>123.35533333333333</v>
       </c>
       <c r="B202">
-        <v>-0.48749999999999982</v>
+        <v>-0.14999999999999991</v>
       </c>
       <c r="C202">
-        <v>0.6875</v>
+        <v>0.65</v>
       </c>
       <c r="D202">
         <v>1</v>
@@ -34504,13 +34504,13 @@
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203">
-        <v>123.35533333333333</v>
+        <v>123.43516666666667</v>
       </c>
       <c r="B203">
-        <v>-0.14999999999999991</v>
+        <v>0.1875</v>
       </c>
       <c r="C203">
-        <v>0.65</v>
+        <v>0.61250000000000004</v>
       </c>
       <c r="D203">
         <v>1</v>
@@ -34518,13 +34518,13 @@
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204">
-        <v>123.43516666666667</v>
+        <v>123.515</v>
       </c>
       <c r="B204">
-        <v>0.1875</v>
+        <v>0.52500000000000036</v>
       </c>
       <c r="C204">
-        <v>0.61250000000000004</v>
+        <v>0.57500000000000007</v>
       </c>
       <c r="D204">
         <v>1</v>
@@ -34532,13 +34532,13 @@
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205">
-        <v>123.515</v>
+        <v>123.56166666666667</v>
       </c>
       <c r="B205">
-        <v>0.52500000000000036</v>
+        <v>0.86250000000000027</v>
       </c>
       <c r="C205">
-        <v>0.57500000000000007</v>
+        <v>0.53750000000000009</v>
       </c>
       <c r="D205">
         <v>1</v>
@@ -34546,13 +34546,13 @@
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206">
-        <v>123.56166666666667</v>
+        <v>123.60833333333333</v>
       </c>
       <c r="B206">
-        <v>0.86250000000000027</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="C206">
-        <v>0.53750000000000009</v>
+        <v>0.5</v>
       </c>
       <c r="D206">
         <v>1</v>
@@ -34560,24 +34560,24 @@
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207">
-        <v>123.60833333333333</v>
+        <v>172.83600000000001</v>
       </c>
       <c r="B207">
-        <v>1.2000000000000002</v>
+        <v>0.9</v>
       </c>
       <c r="C207">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="D207">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208">
-        <v>172.83600000000001</v>
+        <v>172.90300000000002</v>
       </c>
       <c r="B208">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="C208">
         <v>0.6</v>
@@ -34588,10 +34588,10 @@
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209">
-        <v>172.90300000000002</v>
+        <v>172.97000000000003</v>
       </c>
       <c r="B209">
-        <v>0.4</v>
+        <v>-0.1</v>
       </c>
       <c r="C209">
         <v>0.6</v>
@@ -34602,10 +34602,10 @@
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210">
-        <v>172.97000000000003</v>
+        <v>173.03700000000003</v>
       </c>
       <c r="B210">
-        <v>-0.1</v>
+        <v>-0.6</v>
       </c>
       <c r="C210">
         <v>0.6</v>
@@ -34616,10 +34616,10 @@
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211">
-        <v>173.03700000000003</v>
+        <v>173.10400000000004</v>
       </c>
       <c r="B211">
-        <v>-0.6</v>
+        <v>0.1</v>
       </c>
       <c r="C211">
         <v>0.6</v>
@@ -34630,10 +34630,10 @@
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212">
-        <v>173.10400000000004</v>
+        <v>173.17100000000005</v>
       </c>
       <c r="B212">
-        <v>0.1</v>
+        <v>0.8</v>
       </c>
       <c r="C212">
         <v>0.6</v>
@@ -34644,10 +34644,10 @@
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213">
-        <v>173.17100000000005</v>
+        <v>177.566</v>
       </c>
       <c r="B213">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="C213">
         <v>0.6</v>
@@ -34658,10 +34658,10 @@
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214">
-        <v>177.566</v>
+        <v>178.499</v>
       </c>
       <c r="B214">
-        <v>1</v>
+        <v>1.7</v>
       </c>
       <c r="C214">
         <v>0.6</v>
@@ -34672,10 +34672,10 @@
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215">
-        <v>178.499</v>
+        <v>178.54300000000001</v>
       </c>
       <c r="B215">
-        <v>1.7</v>
+        <v>1.4</v>
       </c>
       <c r="C215">
         <v>0.6</v>
@@ -34686,10 +34686,10 @@
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216">
-        <v>178.54300000000001</v>
+        <v>178.636</v>
       </c>
       <c r="B216">
-        <v>1.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C216">
         <v>0.6</v>
@@ -34700,13 +34700,13 @@
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217">
-        <v>178.636</v>
+        <v>191.636</v>
       </c>
       <c r="B217">
-        <v>1.1000000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="C217">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="D217">
         <v>17</v>
@@ -34714,13 +34714,13 @@
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218">
-        <v>191.636</v>
+        <v>191.703</v>
       </c>
       <c r="B218">
-        <v>0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="C218">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D218">
         <v>17</v>
@@ -34728,13 +34728,13 @@
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219">
-        <v>191.703</v>
+        <v>191.77</v>
       </c>
       <c r="B219">
-        <v>-0.3</v>
+        <v>-1</v>
       </c>
       <c r="C219">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D219">
         <v>17</v>
@@ -34742,13 +34742,13 @@
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220">
-        <v>191.77</v>
+        <v>191.83700000000002</v>
       </c>
       <c r="B220">
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="C220">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D220">
         <v>17</v>
@@ -34756,13 +34756,13 @@
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221">
-        <v>191.83700000000002</v>
+        <v>191.90400000000002</v>
       </c>
       <c r="B221">
-        <v>-1.5</v>
+        <v>-1.2</v>
       </c>
       <c r="C221">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D221">
         <v>17</v>
@@ -34770,13 +34770,13 @@
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222">
-        <v>191.90400000000002</v>
+        <v>191.97100000000003</v>
       </c>
       <c r="B222">
-        <v>-1.2</v>
+        <v>-0.85</v>
       </c>
       <c r="C222">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D222">
         <v>17</v>
@@ -34784,13 +34784,13 @@
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223">
-        <v>191.97100000000003</v>
+        <v>192.03800000000004</v>
       </c>
       <c r="B223">
-        <v>-0.85</v>
+        <v>-0.45</v>
       </c>
       <c r="C223">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D223">
         <v>17</v>
@@ -34798,13 +34798,13 @@
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224">
-        <v>192.03800000000004</v>
+        <v>192.10500000000005</v>
       </c>
       <c r="B224">
-        <v>-0.45</v>
+        <v>0</v>
       </c>
       <c r="C224">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D224">
         <v>17</v>
@@ -34812,13 +34812,13 @@
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225">
-        <v>192.10500000000005</v>
+        <v>192.17200000000005</v>
       </c>
       <c r="B225">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="C225">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D225">
         <v>17</v>
@@ -34826,13 +34826,13 @@
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226">
-        <v>192.17200000000005</v>
+        <v>192.23900000000006</v>
       </c>
       <c r="B226">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="C226">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D226">
         <v>17</v>
@@ -34840,13 +34840,13 @@
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227">
-        <v>192.23900000000006</v>
+        <v>192.30600000000007</v>
       </c>
       <c r="B227">
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="C227">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D227">
         <v>17</v>
@@ -34854,13 +34854,13 @@
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228">
-        <v>192.30600000000007</v>
+        <v>192.37300000000008</v>
       </c>
       <c r="B228">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="C228">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D228">
         <v>17</v>
@@ -34868,13 +34868,13 @@
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229">
-        <v>192.37300000000008</v>
+        <v>204.43600000000001</v>
       </c>
       <c r="B229">
-        <v>1.6</v>
+        <v>-0.5</v>
       </c>
       <c r="C229">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D229">
         <v>17</v>
@@ -34882,13 +34882,13 @@
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230">
-        <v>204.43600000000001</v>
+        <v>204.50300000000001</v>
       </c>
       <c r="B230">
-        <v>-0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C230">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D230">
         <v>17</v>
@@ -34896,13 +34896,13 @@
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231">
-        <v>204.50300000000001</v>
+        <v>204.57000000000002</v>
       </c>
       <c r="B231">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="C231">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D231">
         <v>17</v>
@@ -34910,13 +34910,13 @@
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232">
-        <v>204.57000000000002</v>
+        <v>204.63700000000003</v>
       </c>
       <c r="B232">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="C232">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D232">
         <v>17</v>
@@ -34924,13 +34924,13 @@
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233">
-        <v>204.63700000000003</v>
+        <v>204.70400000000004</v>
       </c>
       <c r="B233">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="C233">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D233">
         <v>17</v>
@@ -34938,13 +34938,13 @@
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234">
-        <v>204.70400000000004</v>
+        <v>204.77100000000004</v>
       </c>
       <c r="B234">
-        <v>1.2</v>
+        <v>0.85</v>
       </c>
       <c r="C234">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D234">
         <v>17</v>
@@ -34952,13 +34952,13 @@
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235">
-        <v>204.77100000000004</v>
+        <v>204.83800000000005</v>
       </c>
       <c r="B235">
-        <v>0.85</v>
+        <v>0.45</v>
       </c>
       <c r="C235">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D235">
         <v>17</v>
@@ -34966,13 +34966,13 @@
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236">
-        <v>204.83800000000005</v>
+        <v>204.90500000000006</v>
       </c>
       <c r="B236">
-        <v>0.45</v>
+        <v>0</v>
       </c>
       <c r="C236">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D236">
         <v>17</v>
@@ -34980,13 +34980,13 @@
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237">
-        <v>204.90500000000006</v>
+        <v>204.97200000000007</v>
       </c>
       <c r="B237">
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="C237">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D237">
         <v>17</v>
@@ -34994,13 +34994,13 @@
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238">
-        <v>204.97200000000007</v>
+        <v>205.03900000000007</v>
       </c>
       <c r="B238">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="C238">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D238">
         <v>17</v>
@@ -35008,13 +35008,13 @@
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239">
-        <v>205.03900000000007</v>
+        <v>205.10600000000008</v>
       </c>
       <c r="B239">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="C239">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D239">
         <v>17</v>
@@ -35022,13 +35022,13 @@
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240">
-        <v>205.10600000000008</v>
+        <v>205.17300000000009</v>
       </c>
       <c r="B240">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
       <c r="C240">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D240">
         <v>17</v>
@@ -35036,21 +35036,21 @@
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241">
-        <v>205.17300000000009</v>
+        <v>218.93600000000001</v>
       </c>
       <c r="B241">
-        <v>-1.6</v>
+        <v>-1</v>
       </c>
       <c r="C241">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D241">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242">
-        <v>218.93600000000001</v>
+        <v>219.036</v>
       </c>
       <c r="B242">
         <v>-1</v>
@@ -35064,7 +35064,7 @@
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243">
-        <v>219.036</v>
+        <v>219.10300000000001</v>
       </c>
       <c r="B243">
         <v>-1</v>
@@ -35078,7 +35078,7 @@
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244">
-        <v>219.10300000000001</v>
+        <v>219.17000000000002</v>
       </c>
       <c r="B244">
         <v>-1</v>
@@ -35092,13 +35092,13 @@
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245">
-        <v>219.17000000000002</v>
+        <v>220.565</v>
       </c>
       <c r="B245">
-        <v>-1</v>
+        <v>0.6</v>
       </c>
       <c r="C245">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="D245">
         <v>19</v>
@@ -35106,10 +35106,10 @@
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246">
-        <v>220.565</v>
+        <v>220.61500000000001</v>
       </c>
       <c r="B246">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="C246">
         <v>0.6</v>
@@ -35120,10 +35120,10 @@
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247">
-        <v>220.61500000000001</v>
+        <v>220.66499999999999</v>
       </c>
       <c r="B247">
-        <v>0</v>
+        <v>-0.6</v>
       </c>
       <c r="C247">
         <v>0.6</v>
@@ -35134,13 +35134,13 @@
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248">
-        <v>220.66499999999999</v>
+        <v>222.43600000000001</v>
       </c>
       <c r="B248">
-        <v>-0.6</v>
+        <v>1.5</v>
       </c>
       <c r="C248">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="D248">
         <v>19</v>
@@ -35148,10 +35148,10 @@
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249">
-        <v>222.43600000000001</v>
+        <v>222.536</v>
       </c>
       <c r="B249">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="C249">
         <v>0.7</v>
@@ -35162,10 +35162,10 @@
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250">
-        <v>222.536</v>
+        <v>222.636</v>
       </c>
       <c r="B250">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="C250">
         <v>0.7</v>
@@ -35176,10 +35176,10 @@
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251">
-        <v>222.636</v>
+        <v>222.73599999999999</v>
       </c>
       <c r="B251">
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C251">
         <v>0.7</v>
@@ -35190,10 +35190,10 @@
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252">
-        <v>222.73599999999999</v>
+        <v>222.83600000000001</v>
       </c>
       <c r="B252">
-        <v>-1.5</v>
+        <v>1.5</v>
       </c>
       <c r="C252">
         <v>0.7</v>
@@ -35204,10 +35204,10 @@
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253">
-        <v>222.83600000000001</v>
+        <v>222.93600000000001</v>
       </c>
       <c r="B253">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="C253">
         <v>0.7</v>
@@ -35218,10 +35218,10 @@
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254">
-        <v>222.93600000000001</v>
+        <v>223.036</v>
       </c>
       <c r="B254">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="C254">
         <v>0.7</v>
@@ -35232,10 +35232,10 @@
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255">
-        <v>223.036</v>
+        <v>223.136</v>
       </c>
       <c r="B255">
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C255">
         <v>0.7</v>
@@ -35246,10 +35246,10 @@
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A256">
-        <v>223.136</v>
+        <v>223.23599999999999</v>
       </c>
       <c r="B256">
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="C256">
         <v>0.7</v>
@@ -35260,10 +35260,10 @@
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A257">
-        <v>223.23599999999999</v>
+        <v>223.33600000000001</v>
       </c>
       <c r="B257">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="C257">
         <v>0.7</v>
@@ -35274,10 +35274,10 @@
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A258">
-        <v>223.33600000000001</v>
+        <v>223.43600000000001</v>
       </c>
       <c r="B258">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="C258">
         <v>0.7</v>
@@ -35288,10 +35288,10 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A259">
-        <v>223.43600000000001</v>
+        <v>223.536</v>
       </c>
       <c r="B259">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="C259">
         <v>0.7</v>
@@ -35302,10 +35302,10 @@
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A260">
-        <v>223.536</v>
+        <v>223.636</v>
       </c>
       <c r="B260">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="C260">
         <v>0.7</v>
@@ -35316,10 +35316,10 @@
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A261">
-        <v>223.636</v>
+        <v>223.73599999999999</v>
       </c>
       <c r="B261">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C261">
         <v>0.7</v>
@@ -35330,10 +35330,10 @@
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A262">
-        <v>223.73599999999999</v>
+        <v>223.83600000000001</v>
       </c>
       <c r="B262">
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="C262">
         <v>0.7</v>
@@ -35344,10 +35344,10 @@
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A263">
-        <v>223.83600000000001</v>
+        <v>223.93600000000001</v>
       </c>
       <c r="B263">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="C263">
         <v>0.7</v>
@@ -35358,10 +35358,10 @@
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A264">
-        <v>223.93600000000001</v>
+        <v>224.036</v>
       </c>
       <c r="B264">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="C264">
         <v>0.7</v>
@@ -35372,10 +35372,10 @@
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A265">
-        <v>224.036</v>
+        <v>224.136</v>
       </c>
       <c r="B265">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="C265">
         <v>0.7</v>
@@ -35386,10 +35386,10 @@
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A266">
-        <v>224.136</v>
+        <v>224.23599999999999</v>
       </c>
       <c r="B266">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="C266">
         <v>0.7</v>
@@ -35400,10 +35400,10 @@
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A267">
-        <v>224.23599999999999</v>
+        <v>224.33600000000001</v>
       </c>
       <c r="B267">
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C267">
         <v>0.7</v>
@@ -35414,10 +35414,10 @@
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A268">
-        <v>224.33600000000001</v>
+        <v>224.43600000000001</v>
       </c>
       <c r="B268">
-        <v>-1.5</v>
+        <v>1.5</v>
       </c>
       <c r="C268">
         <v>0.7</v>
@@ -35428,10 +35428,10 @@
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A269">
-        <v>224.43600000000001</v>
+        <v>224.536</v>
       </c>
       <c r="B269">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="C269">
         <v>0.7</v>
@@ -35442,10 +35442,10 @@
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A270">
-        <v>224.536</v>
+        <v>224.636</v>
       </c>
       <c r="B270">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="C270">
         <v>0.7</v>
@@ -35456,10 +35456,10 @@
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A271">
-        <v>224.636</v>
+        <v>224.73599999999999</v>
       </c>
       <c r="B271">
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C271">
         <v>0.7</v>
@@ -35470,10 +35470,10 @@
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A272">
-        <v>224.73599999999999</v>
+        <v>224.83600000000001</v>
       </c>
       <c r="B272">
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="C272">
         <v>0.7</v>
@@ -35484,10 +35484,10 @@
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273">
-        <v>224.83600000000001</v>
+        <v>224.93600000000001</v>
       </c>
       <c r="B273">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="C273">
         <v>0.7</v>
@@ -35498,10 +35498,10 @@
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A274">
-        <v>224.93600000000001</v>
+        <v>225.036</v>
       </c>
       <c r="B274">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="C274">
         <v>0.7</v>
@@ -35512,10 +35512,10 @@
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A275">
-        <v>225.036</v>
+        <v>225.136</v>
       </c>
       <c r="B275">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="C275">
         <v>0.7</v>
@@ -35526,10 +35526,10 @@
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A276">
-        <v>225.136</v>
+        <v>225.23599999999999</v>
       </c>
       <c r="B276">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="C276">
         <v>0.7</v>
@@ -35540,10 +35540,10 @@
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A277">
-        <v>225.23599999999999</v>
+        <v>225.33600000000001</v>
       </c>
       <c r="B277">
-        <v>-0.5</v>
+        <v>-1.5</v>
       </c>
       <c r="C277">
         <v>0.7</v>
@@ -35554,10 +35554,10 @@
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A278">
-        <v>225.33600000000001</v>
+        <v>225.43600000000001</v>
       </c>
       <c r="B278">
-        <v>-1.5</v>
+        <v>-0.5</v>
       </c>
       <c r="C278">
         <v>0.7</v>
@@ -35568,10 +35568,10 @@
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A279">
-        <v>225.43600000000001</v>
+        <v>225.536</v>
       </c>
       <c r="B279">
-        <v>-0.5</v>
+        <v>0.5</v>
       </c>
       <c r="C279">
         <v>0.7</v>
@@ -35582,10 +35582,10 @@
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A280">
-        <v>225.536</v>
+        <v>225.636</v>
       </c>
       <c r="B280">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="C280">
         <v>0.7</v>
@@ -35596,10 +35596,10 @@
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A281">
-        <v>225.636</v>
+        <v>225.79900000000001</v>
       </c>
       <c r="B281">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="C281">
         <v>0.7</v>
@@ -35610,10 +35610,10 @@
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A282">
-        <v>225.79900000000001</v>
+        <v>225.86500000000001</v>
       </c>
       <c r="B282">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="C282">
         <v>0.7</v>
@@ -35624,10 +35624,10 @@
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A283">
-        <v>225.86500000000001</v>
+        <v>225.93199999999999</v>
       </c>
       <c r="B283">
-        <v>1.25</v>
+        <v>0.5</v>
       </c>
       <c r="C283">
         <v>0.7</v>
@@ -35638,10 +35638,10 @@
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A284">
-        <v>225.93199999999999</v>
+        <v>225.999</v>
       </c>
       <c r="B284">
-        <v>0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="C284">
         <v>0.7</v>
@@ -35652,10 +35652,10 @@
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A285">
-        <v>225.999</v>
+        <v>226.065</v>
       </c>
       <c r="B285">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="C285">
         <v>0.7</v>
@@ -35666,10 +35666,10 @@
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A286">
-        <v>226.065</v>
+        <v>226.13200000000001</v>
       </c>
       <c r="B286">
-        <v>0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="C286">
         <v>0.7</v>
@@ -35680,10 +35680,10 @@
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A287">
-        <v>226.13200000000001</v>
+        <v>226.19900000000001</v>
       </c>
       <c r="B287">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="C287">
         <v>0.7</v>
@@ -35694,10 +35694,10 @@
     </row>
     <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A288">
-        <v>226.19900000000001</v>
+        <v>226.26499999999999</v>
       </c>
       <c r="B288">
-        <v>-1</v>
+        <v>-0.4</v>
       </c>
       <c r="C288">
         <v>0.7</v>
@@ -35708,10 +35708,10 @@
     </row>
     <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A289">
-        <v>226.26499999999999</v>
+        <v>226.315</v>
       </c>
       <c r="B289">
-        <v>-0.4</v>
+        <v>-0.8</v>
       </c>
       <c r="C289">
         <v>0.7</v>
@@ -35722,10 +35722,10 @@
     </row>
     <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A290">
-        <v>226.315</v>
+        <v>226.36500000000001</v>
       </c>
       <c r="B290">
-        <v>-0.8</v>
+        <v>-1.2</v>
       </c>
       <c r="C290">
         <v>0.7</v>
@@ -35736,10 +35736,10 @@
     </row>
     <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291">
-        <v>226.36500000000001</v>
+        <v>226.41499999999999</v>
       </c>
       <c r="B291">
-        <v>-1.2</v>
+        <v>-1.6</v>
       </c>
       <c r="C291">
         <v>0.7</v>
@@ -35750,13 +35750,13 @@
     </row>
     <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A292">
-        <v>226.41499999999999</v>
+        <v>231.73600000000002</v>
       </c>
       <c r="B292">
-        <v>-1.6</v>
+        <v>1</v>
       </c>
       <c r="C292">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="D292">
         <v>19</v>
@@ -35764,7 +35764,7 @@
     </row>
     <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A293">
-        <v>231.73600000000002</v>
+        <v>231.83600000000001</v>
       </c>
       <c r="B293">
         <v>1</v>
@@ -35778,7 +35778,7 @@
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A294">
-        <v>231.83600000000001</v>
+        <v>231.90300000000002</v>
       </c>
       <c r="B294">
         <v>1</v>
@@ -35792,7 +35792,7 @@
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A295">
-        <v>231.90300000000002</v>
+        <v>231.97000000000003</v>
       </c>
       <c r="B295">
         <v>1</v>
@@ -35806,13 +35806,13 @@
     </row>
     <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A296">
-        <v>231.97000000000003</v>
+        <v>233.36500000000001</v>
       </c>
       <c r="B296">
-        <v>1</v>
+        <v>-0.6</v>
       </c>
       <c r="C296">
-        <v>0.9</v>
+        <v>0.6</v>
       </c>
       <c r="D296">
         <v>19</v>
@@ -35820,10 +35820,10 @@
     </row>
     <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A297">
-        <v>233.36500000000001</v>
+        <v>233.41500000000002</v>
       </c>
       <c r="B297">
-        <v>-0.6</v>
+        <v>0</v>
       </c>
       <c r="C297">
         <v>0.6</v>
@@ -35834,10 +35834,10 @@
     </row>
     <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A298">
-        <v>233.41500000000002</v>
+        <v>233.465</v>
       </c>
       <c r="B298">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="C298">
         <v>0.6</v>
@@ -35848,13 +35848,13 @@
     </row>
     <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A299">
-        <v>233.465</v>
+        <v>238.036</v>
       </c>
       <c r="B299">
-        <v>0.6</v>
+        <v>1.5</v>
       </c>
       <c r="C299">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="D299">
         <v>19</v>
@@ -35862,10 +35862,10 @@
     </row>
     <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A300">
-        <v>238.036</v>
+        <v>238.08600000000001</v>
       </c>
       <c r="B300">
-        <v>1.5</v>
+        <v>0.8</v>
       </c>
       <c r="C300">
         <v>0.8</v>
@@ -35876,10 +35876,10 @@
     </row>
     <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A301">
-        <v>238.08600000000001</v>
+        <v>238.136</v>
       </c>
       <c r="B301">
-        <v>0.8</v>
+        <v>0.1</v>
       </c>
       <c r="C301">
         <v>0.8</v>
@@ -35890,13 +35890,13 @@
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A302">
-        <v>238.136</v>
+        <v>244.83600000000001</v>
       </c>
       <c r="B302">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="C302">
-        <v>0.8</v>
+        <v>1.3</v>
       </c>
       <c r="D302">
         <v>19</v>
@@ -35904,13 +35904,13 @@
     </row>
     <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A303">
-        <v>244.83600000000001</v>
+        <v>244.93600000000001</v>
       </c>
       <c r="B303">
         <v>0</v>
       </c>
       <c r="C303">
-        <v>1.3</v>
+        <v>1.35</v>
       </c>
       <c r="D303">
         <v>19</v>
@@ -35918,13 +35918,13 @@
     </row>
     <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A304">
-        <v>244.93600000000001</v>
+        <v>245.036</v>
       </c>
       <c r="B304">
         <v>0</v>
       </c>
       <c r="C304">
-        <v>1.35</v>
+        <v>1.4</v>
       </c>
       <c r="D304">
         <v>19</v>
@@ -35932,13 +35932,13 @@
     </row>
     <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A305">
-        <v>245.036</v>
+        <v>245.136</v>
       </c>
       <c r="B305">
         <v>0</v>
       </c>
       <c r="C305">
-        <v>1.4</v>
+        <v>1.45</v>
       </c>
       <c r="D305">
         <v>19</v>
@@ -35946,13 +35946,13 @@
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A306">
-        <v>245.136</v>
+        <v>245.23599999999999</v>
       </c>
       <c r="B306">
         <v>0</v>
       </c>
       <c r="C306">
-        <v>1.45</v>
+        <v>1.5</v>
       </c>
       <c r="D306">
         <v>19</v>
@@ -35960,27 +35960,27 @@
     </row>
     <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A307">
-        <v>245.23599999999999</v>
+        <v>244.83600000000001</v>
       </c>
       <c r="B307">
-        <v>0</v>
+        <v>-1.05</v>
       </c>
       <c r="C307">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="D307">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A308">
-        <v>244.83600000000001</v>
+        <v>244.93600000000001</v>
       </c>
       <c r="B308">
-        <v>-1.05</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="C308">
-        <v>1.3</v>
+        <v>1.35</v>
       </c>
       <c r="D308">
         <v>17</v>
@@ -35988,13 +35988,13 @@
     </row>
     <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309">
-        <v>244.93600000000001</v>
+        <v>245.036</v>
       </c>
       <c r="B309">
-        <v>-1.1000000000000001</v>
+        <v>-1.1499999999999999</v>
       </c>
       <c r="C309">
-        <v>1.35</v>
+        <v>1.4</v>
       </c>
       <c r="D309">
         <v>17</v>
@@ -36002,13 +36002,13 @@
     </row>
     <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A310">
-        <v>245.036</v>
+        <v>245.136</v>
       </c>
       <c r="B310">
-        <v>-1.1499999999999999</v>
+        <v>-1.2</v>
       </c>
       <c r="C310">
-        <v>1.4</v>
+        <v>1.45</v>
       </c>
       <c r="D310">
         <v>17</v>
@@ -36016,13 +36016,13 @@
     </row>
     <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A311">
-        <v>245.136</v>
+        <v>245.23599999999999</v>
       </c>
       <c r="B311">
-        <v>-1.2</v>
+        <v>-1.25</v>
       </c>
       <c r="C311">
-        <v>1.45</v>
+        <v>1.5</v>
       </c>
       <c r="D311">
         <v>17</v>
@@ -36030,13 +36030,13 @@
     </row>
     <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A312">
-        <v>245.23599999999999</v>
+        <v>244.83600000000001</v>
       </c>
       <c r="B312">
-        <v>-1.25</v>
+        <v>1.05</v>
       </c>
       <c r="C312">
-        <v>1.5</v>
+        <v>1.3</v>
       </c>
       <c r="D312">
         <v>17</v>
@@ -36044,13 +36044,13 @@
     </row>
     <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A313">
-        <v>244.83600000000001</v>
+        <v>244.93600000000001</v>
       </c>
       <c r="B313">
-        <v>1.05</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C313">
-        <v>1.3</v>
+        <v>1.35</v>
       </c>
       <c r="D313">
         <v>17</v>
@@ -36058,13 +36058,13 @@
     </row>
     <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A314">
-        <v>244.93600000000001</v>
+        <v>245.036</v>
       </c>
       <c r="B314">
-        <v>1.1000000000000001</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C314">
-        <v>1.35</v>
+        <v>1.4</v>
       </c>
       <c r="D314">
         <v>17</v>
@@ -36072,13 +36072,13 @@
     </row>
     <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A315">
-        <v>245.036</v>
+        <v>245.136</v>
       </c>
       <c r="B315">
-        <v>1.1499999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="C315">
-        <v>1.4</v>
+        <v>1.45</v>
       </c>
       <c r="D315">
         <v>17</v>
@@ -36086,29 +36086,15 @@
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A316">
-        <v>245.136</v>
+        <v>245.23599999999999</v>
       </c>
       <c r="B316">
-        <v>1.2</v>
+        <v>1.25</v>
       </c>
       <c r="C316">
-        <v>1.45</v>
+        <v>1.5</v>
       </c>
       <c r="D316">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A317">
-        <v>245.23599999999999</v>
-      </c>
-      <c r="B317">
-        <v>1.25</v>
-      </c>
-      <c r="C317">
-        <v>1.5</v>
-      </c>
-      <c r="D317">
         <v>17</v>
       </c>
     </row>
@@ -38369,8 +38355,8 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:J106"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L42" sqref="L42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -38808,7 +38794,7 @@
         <v>37.636000000000003</v>
       </c>
       <c r="F14">
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
       <c r="G14">
         <v>0</v>
@@ -38846,7 +38832,7 @@
         <v>1</v>
       </c>
       <c r="H15">
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
       <c r="I15">
         <v>0</v>
@@ -38872,7 +38858,7 @@
         <v>39.235999999999997</v>
       </c>
       <c r="F16">
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -38904,7 +38890,7 @@
         <v>40.036000000000001</v>
       </c>
       <c r="F17">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -38942,7 +38928,7 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -39614,7 +39600,7 @@
         <v>1</v>
       </c>
       <c r="H39">
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -39640,7 +39626,7 @@
         <v>55.835999999999999</v>
       </c>
       <c r="F40">
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
       <c r="G40">
         <v>0</v>
@@ -39678,7 +39664,7 @@
         <v>1</v>
       </c>
       <c r="H41">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -39704,7 +39690,7 @@
         <v>57.436</v>
       </c>
       <c r="F42">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="G42">
         <v>0</v>
@@ -39742,7 +39728,7 @@
         <v>1</v>
       </c>
       <c r="H43">
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -39768,7 +39754,7 @@
         <v>59.036000000000001</v>
       </c>
       <c r="F44">
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -39838,7 +39824,7 @@
         <v>1.5</v>
       </c>
       <c r="H46">
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
       <c r="I46">
         <v>0.75</v>
@@ -39864,7 +39850,7 @@
         <v>128.24700000000001</v>
       </c>
       <c r="F47">
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
       <c r="G47">
         <v>0.75</v>
@@ -39902,7 +39888,7 @@
         <v>1.5</v>
       </c>
       <c r="H48">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I48">
         <v>0.75</v>
@@ -39928,7 +39914,7 @@
         <v>128.24700000000001</v>
       </c>
       <c r="F49">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="G49">
         <v>0.75</v>
@@ -40158,7 +40144,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="I56">
         <v>0.75</v>
@@ -40184,7 +40170,7 @@
         <v>135.43600000000004</v>
       </c>
       <c r="F57">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="G57">
         <v>0.75</v>
@@ -40222,7 +40208,7 @@
         <v>1.5</v>
       </c>
       <c r="H58">
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
       <c r="I58">
         <v>0.75</v>
@@ -40248,7 +40234,7 @@
         <v>136.03600000000006</v>
       </c>
       <c r="F59">
-        <v>-1.2</v>
+        <v>-1</v>
       </c>
       <c r="G59">
         <v>0.75</v>
@@ -40760,7 +40746,7 @@
         <v>162.43600000000001</v>
       </c>
       <c r="F75">
-        <v>-1.6</v>
+        <v>-1.2</v>
       </c>
       <c r="G75">
         <v>1.2</v>
@@ -40798,7 +40784,7 @@
         <v>0</v>
       </c>
       <c r="H76">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="I76">
         <v>0.6</v>
@@ -40824,7 +40810,7 @@
         <v>162.83600000000001</v>
       </c>
       <c r="F77">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="G77">
         <v>0.6</v>
@@ -40862,7 +40848,7 @@
         <v>1.2</v>
       </c>
       <c r="H78">
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
       <c r="I78">
         <v>0</v>
@@ -40888,7 +40874,7 @@
         <v>162.43600000000001</v>
       </c>
       <c r="F79">
-        <v>1.6</v>
+        <v>1.2</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -40926,7 +40912,7 @@
         <v>1.2</v>
       </c>
       <c r="H80">
-        <v>-0.8</v>
+        <v>-0.6</v>
       </c>
       <c r="I80">
         <v>0.6</v>
@@ -40952,7 +40938,7 @@
         <v>162.83600000000001</v>
       </c>
       <c r="F81">
-        <v>-0.8</v>
+        <v>-0.6</v>
       </c>
       <c r="G81">
         <v>0.6</v>
@@ -40990,7 +40976,7 @@
         <v>0</v>
       </c>
       <c r="H82">
-        <v>-1.6</v>
+        <v>-1.2</v>
       </c>
       <c r="I82">
         <v>1.2</v>

</xml_diff>